<commit_message>
Update health sync task
</commit_message>
<xml_diff>
--- a/utils/HealthSolutionsData.xlsx
+++ b/utils/HealthSolutionsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sconrad/DIAL/exchange-backend/utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0EE6A0-D099-BB44-8603-C0BD41FEA550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DE02AB-581F-524B-AC75-9DD73D1D2074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8040" yWindow="880" windowWidth="27960" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6800" yWindow="2420" windowWidth="27960" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -529,9 +529,6 @@
     <t>Sophie ChatRobot Limited</t>
   </si>
   <si>
-    <t xml:space="preserve">SophieBot </t>
-  </si>
-  <si>
     <t>SophieBot is an artificial intelligence persona to answer users' questions on sexual health. Think of her as "Siri for sexual health".We take great care to feed her with curated verified information from our partner/investor UNFPA Kenya.</t>
   </si>
   <si>
@@ -898,6 +895,9 @@
   </si>
   <si>
     <t>https://drive.google.com/uc?export=download&amp;id=1pEAL9VJC4W8wzRkxjrKj_5Xo19Ptv43B</t>
+  </si>
+  <si>
+    <t>SophieBot</t>
   </si>
 </sst>
 </file>
@@ -1636,7 +1636,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1676,7 +1676,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H1" s="19" t="s">
         <v>6</v>
@@ -1817,7 +1817,7 @@
         <v>51</v>
       </c>
       <c r="BB1" s="19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="BC1" s="19" t="s">
         <v>52</v>
@@ -1846,10 +1846,10 @@
         <v>58</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
@@ -2400,25 +2400,25 @@
         <v>144</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>149</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>67</v>
@@ -2463,7 +2463,7 @@
         <v>63</v>
       </c>
       <c r="AD6" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
@@ -2471,10 +2471,10 @@
         <v>63</v>
       </c>
       <c r="AH6" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI6" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="AI6" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="AJ6" s="2" t="s">
         <v>63</v>
@@ -2483,16 +2483,16 @@
         <v>67</v>
       </c>
       <c r="AL6" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="AM6" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="AM6" s="2" t="s">
-        <v>155</v>
       </c>
       <c r="AN6" s="2" t="s">
         <v>116</v>
       </c>
       <c r="AO6" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AP6" s="2" t="s">
         <v>67</v>
@@ -2507,7 +2507,7 @@
       <c r="AX6" s="2"/>
       <c r="AY6" s="2"/>
       <c r="AZ6" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BA6" s="2"/>
       <c r="BB6" s="2"/>
@@ -2519,42 +2519,42 @@
         <v>45549.185348842591</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="F7" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>162</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="K7" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="L7" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="M7" s="8" t="s">
         <v>166</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>167</v>
       </c>
       <c r="N7" s="8" t="s">
         <v>67</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P7" s="8" t="s">
         <v>63</v>
@@ -2572,13 +2572,13 @@
         <v>63</v>
       </c>
       <c r="U7" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="V7" s="8">
         <v>1</v>
       </c>
       <c r="W7" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="X7" s="8" t="s">
         <v>111</v>
@@ -2593,7 +2593,7 @@
         <v>63</v>
       </c>
       <c r="AB7" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AC7" s="8" t="s">
         <v>63</v>
@@ -2605,22 +2605,22 @@
         <v>63</v>
       </c>
       <c r="AH7" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI7" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="AI7" s="8" t="s">
+      <c r="AJ7" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK7" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL7" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="AJ7" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="AK7" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL7" s="8" t="s">
+      <c r="AM7" s="8" t="s">
         <v>174</v>
-      </c>
-      <c r="AM7" s="8" t="s">
-        <v>175</v>
       </c>
       <c r="AN7" s="8" t="s">
         <v>116</v>
@@ -2635,7 +2635,7 @@
       <c r="AR7" s="8"/>
       <c r="AS7" s="8"/>
       <c r="AT7" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AU7" s="8"/>
       <c r="AV7" s="8" t="s">
@@ -2644,7 +2644,7 @@
       <c r="AW7" s="8"/>
       <c r="AX7" s="8"/>
       <c r="AY7" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AZ7" s="8" t="s">
         <v>122</v>
@@ -2659,42 +2659,42 @@
         <v>45550.202852604169</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O8" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="P8" s="2" t="s">
         <v>67</v>
@@ -2712,10 +2712,10 @@
         <v>63</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="W8" s="2">
         <v>18</v>
@@ -2727,7 +2727,7 @@
         <v>40000</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AA8" s="2" t="s">
         <v>67</v>
@@ -2743,22 +2743,22 @@
         <v>63</v>
       </c>
       <c r="AH8" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="AI8" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="AI8" s="2" t="s">
+      <c r="AJ8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL8" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="AJ8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AK8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL8" s="2" t="s">
+      <c r="AM8" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="AM8" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="AN8" s="2" t="s">
         <v>116</v>
@@ -2770,7 +2770,7 @@
         <v>63</v>
       </c>
       <c r="AQ8" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AR8" s="2"/>
       <c r="AS8" s="2"/>
@@ -2778,14 +2778,14 @@
       <c r="AU8" s="2"/>
       <c r="AV8" s="2"/>
       <c r="AW8" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AX8" s="2"/>
       <c r="AY8" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AZ8" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="AZ8" s="2" t="s">
-        <v>196</v>
       </c>
       <c r="BA8" s="2"/>
       <c r="BB8" s="2"/>
@@ -2797,44 +2797,44 @@
         <v>45550.367459953704</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C9" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E9" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="F9" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>201</v>
-      </c>
       <c r="G9" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H9" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="K9" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="L9" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="L9" s="8" t="s">
+      <c r="M9" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="M9" s="8" t="s">
-        <v>205</v>
-      </c>
       <c r="N9" s="8" t="s">
         <v>63</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="P9" s="8" t="s">
         <v>63</v>
@@ -2852,19 +2852,19 @@
         <v>63</v>
       </c>
       <c r="U9" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="V9" s="8">
         <v>9</v>
       </c>
       <c r="W9" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="X9" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="X9" s="8" t="s">
+      <c r="Y9" s="8" t="s">
         <v>208</v>
-      </c>
-      <c r="Y9" s="8" t="s">
-        <v>209</v>
       </c>
       <c r="Z9" s="11">
         <v>3000000</v>
@@ -2873,13 +2873,13 @@
         <v>63</v>
       </c>
       <c r="AB9" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="AC9" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD9" s="9" t="s">
         <v>210</v>
-      </c>
-      <c r="AC9" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD9" s="9" t="s">
-        <v>211</v>
       </c>
       <c r="AE9" s="8"/>
       <c r="AF9" s="8"/>
@@ -2887,56 +2887,56 @@
         <v>63</v>
       </c>
       <c r="AH9" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="AI9" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="AI9" s="8" t="s">
+      <c r="AJ9" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK9" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL9" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="AJ9" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="AK9" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL9" s="8" t="s">
+      <c r="AM9" s="8" t="s">
         <v>214</v>
-      </c>
-      <c r="AM9" s="8" t="s">
-        <v>215</v>
       </c>
       <c r="AN9" s="8" t="s">
         <v>68</v>
       </c>
       <c r="AO9" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AP9" s="8" t="s">
         <v>63</v>
       </c>
       <c r="AQ9" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AR9" s="8"/>
       <c r="AS9" s="8"/>
       <c r="AT9" s="8"/>
       <c r="AU9" s="8"/>
       <c r="AV9" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="AW9" s="8" t="s">
         <v>217</v>
-      </c>
-      <c r="AW9" s="8" t="s">
-        <v>218</v>
       </c>
       <c r="AX9" s="8" t="s">
         <v>120</v>
       </c>
       <c r="AY9" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="AZ9" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="AZ9" s="8" t="s">
+      <c r="BA9" s="8" t="s">
         <v>220</v>
-      </c>
-      <c r="BA9" s="8" t="s">
-        <v>221</v>
       </c>
       <c r="BB9" s="8"/>
       <c r="BC9" s="8"/>
@@ -2947,44 +2947,44 @@
         <v>45551.295963229168</v>
       </c>
       <c r="B10" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>222</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="D10" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="E10" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>225</v>
-      </c>
       <c r="G10" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I10" s="14"/>
       <c r="J10" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="K10" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="L10" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="L10" s="14" t="s">
+      <c r="M10" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="M10" s="14" t="s">
+      <c r="N10" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="O10" s="14" t="s">
         <v>229</v>
-      </c>
-      <c r="N10" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="O10" s="14" t="s">
-        <v>230</v>
       </c>
       <c r="P10" s="14" t="s">
         <v>63</v>
@@ -3002,28 +3002,28 @@
         <v>63</v>
       </c>
       <c r="U10" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="V10" s="14">
         <v>5</v>
       </c>
       <c r="W10" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="X10" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="X10" s="14" t="s">
+      <c r="Y10" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="Y10" s="14" t="s">
+      <c r="Z10" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="Z10" s="14" t="s">
+      <c r="AA10" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB10" s="14" t="s">
         <v>235</v>
-      </c>
-      <c r="AA10" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB10" s="14" t="s">
-        <v>236</v>
       </c>
       <c r="AC10" s="14" t="s">
         <v>67</v>
@@ -3035,10 +3035,10 @@
         <v>63</v>
       </c>
       <c r="AH10" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="AI10" s="15" t="s">
         <v>237</v>
-      </c>
-      <c r="AI10" s="15" t="s">
-        <v>238</v>
       </c>
       <c r="AJ10" s="14" t="s">
         <v>63</v>
@@ -3047,10 +3047,10 @@
         <v>67</v>
       </c>
       <c r="AL10" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="AM10" s="14" t="s">
         <v>239</v>
-      </c>
-      <c r="AM10" s="14" t="s">
-        <v>240</v>
       </c>
       <c r="AN10" s="14" t="s">
         <v>116</v>
@@ -3062,27 +3062,27 @@
         <v>63</v>
       </c>
       <c r="AQ10" s="15" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AR10" s="14"/>
       <c r="AS10" s="14"/>
       <c r="AT10" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AU10" s="14"/>
       <c r="AV10" s="14"/>
       <c r="AW10" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="AX10" s="14" t="s">
         <v>243</v>
-      </c>
-      <c r="AX10" s="14" t="s">
-        <v>244</v>
       </c>
       <c r="AY10" s="14" t="s">
         <v>121</v>
       </c>
       <c r="AZ10" s="14"/>
       <c r="BA10" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="BB10" s="14"/>
       <c r="BC10" s="14"/>
@@ -3111,10 +3111,13 @@
     <hyperlink ref="AI10" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
     <hyperlink ref="AQ10" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
     <hyperlink ref="H9" r:id="rId21" xr:uid="{AE970523-A716-D741-9507-5F4E284CB487}"/>
+    <hyperlink ref="C8" r:id="rId22" xr:uid="{C62867EA-93D7-C849-A012-9CFE28D4A250}"/>
+    <hyperlink ref="C9" r:id="rId23" xr:uid="{9F75A5C9-EA34-B943-8820-0AC5DE257800}"/>
+    <hyperlink ref="C10" r:id="rId24" xr:uid="{B9CBE54E-F13F-3D43-97CD-00DFC561B172}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId22"/>
+    <tablePart r:id="rId25"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update health solutions spreadsheet
</commit_message>
<xml_diff>
--- a/utils/HealthSolutionsData.xlsx
+++ b/utils/HealthSolutionsData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="390">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1054,6 +1054,353 @@
   </si>
   <si>
     <t>Customizable data collection forms</t>
+  </si>
+  <si>
+    <t>Gozie Udemba</t>
+  </si>
+  <si>
+    <t>gudemba@gmail.com</t>
+  </si>
+  <si>
+    <t>Norrig Wellness Solutions</t>
+  </si>
+  <si>
+    <t>Norrig Wellness Solutions is an all-in-one Software-as-a-Service platform for modern healthcare management to streamline workflows, empower staff, and deliver exceptional patient care.</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1Fx57EqYq-vnoffprWr7vsuOL9pUWMPYL</t>
+  </si>
+  <si>
+    <t>Electronic Health Record, Pharmacy, National and Community Health, Analytics and Data Aggregation, AI for Health, Virtual Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How Norrig Wellness Solutions Improves African Health Outcomes
+Norrig Wellness Solutions' hospital-management-as-a-service platform offers a comprehensive suite of features designed to address the unique challenges facing the African healthcare sector. By integrating solutions like a learning management system, procurement management, team collaboration, telehealth, customer relationship management, and data analytics, Norrig aims to enhance health outcomes through:
+1.Enhanced Healthcare Education and Training:
+Learning Management System: Provides a centralized platform for healthcare professionals to access training materials, participate in online courses, and earn certifications. This ensures that healthcare providers are equipped with the latest knowledge and skills to deliver quality care.
+Skill Development: Tailored training programs can be developed to address specific healthcare needs in African communities, such as disease prevention, maternal and child health, and chronic disease management.
+2. Efficient Resource Management and Procurement:
+Procurement Management: Streamlines the procurement process for medical supplies, equipment, and pharmaceuticals, ensuring timely delivery and cost-effective sourcing.
+Inventory Management: Helps hospitals maintain optimal inventory levels, reducing waste and minimizing stockouts.
+3. Improved Collaboration and Communication:
+Team Collaboration: Facilitates seamless communication and collaboration among healthcare providers, improving patient care coordination and reducing medical errors.
+Knowledge Sharing: A centralized platform for sharing best practices and clinical guidelines can enhance the quality of care provided.
+4. Increased Access to Healthcare:
+Telehealth: Enables remote consultations with healthcare providers, expanding access to care for patients in rural or underserved areas.
+Mobile Health: Integration with mobile health technologies can facilitate patient education, appointment scheduling, and medication reminders.
+5. Data-Driven Decision Making:
+Data Analytics: Provides valuable insights into patient demographics, disease trends, and healthcare utilization patterns. This data can be used to inform evidence-based decision-making and improve resource allocation.
+Quality Improvement: Identifies areas for improvement in healthcare delivery and helps implement targeted interventions to enhance patient outcomes.
+6. Strengthened Healthcare Systems:
+Capacity Building: Supports the development of sustainable healthcare systems by providing the necessary tools and infrastructure.
+Policy Development: Contributes to evidence-based healthcare policy formulation and implementation.
+</t>
+  </si>
+  <si>
+    <t>Norrig Wellness Solutions is currently in development. When it goes live the platform will address several critical gaps in the African healthcare landscape such as; 
+1. Digital Infrastructure: Many African healthcare facilities need robust digital infrastructure, hindering efficient operations and access to essential services.
+2. Limited Access to Quality Education: Healthcare professionals often need more opportunities for continuous learning and skill development.
+3. Supply Chain Challenges: Procurement and management of medical supplies can be inefficient, leading to shortages and increased costs.
+4. Communication and Collaboration: Effective communication and collaboration among healthcare teams are essential for providing quality care, but this can be hampered by distance and infrastructure limitations.
+5. Limited Access to Healthcare: Telehealth services can help bridge the gap between urban and rural areas, improving access to care for underserved populations.
+The platform will have the following impact on the African health ecosystem; 
+1. Improved Efficiency: The platform's integrated features can streamline operations, reducing administrative burdens and allowing healthcare professionals to focus on patient care.
+2. Enhanced Education: The learning management system can provide access to high-quality training and development opportunities, improving the skills and knowledge of healthcare workers.
+3. Strengthened Supply Chain: Efficient procurement management can help ensure healthcare facilities have the necessary supplies and equipment for effective care.
+Improved Communication and Collaboration: The team collaboration features can facilitate communication and knowledge sharing among healthcare teams, leading to better patient outcomes.
+4. Increased Access to Care: Telehealth services can expand access to healthcare, particularly in remote or underserved areas.
+5. Data-Driven Decision-Making: The data analytics feature can provide valuable insights into healthcare operations, enabling evidence-based decision-making and continuous improvement.</t>
+  </si>
+  <si>
+    <t>Not yet deployed</t>
+  </si>
+  <si>
+    <t>100 percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The solution is in development. </t>
+  </si>
+  <si>
+    <t>Not yet</t>
+  </si>
+  <si>
+    <t>Startup bootstrapping</t>
+  </si>
+  <si>
+    <t>The solution is in development</t>
+  </si>
+  <si>
+    <t>Adherence to HIPAA and GDPR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The solution in development </t>
+  </si>
+  <si>
+    <t>Data visualization, Dashboards, Clinical data dashboards, Business Intelligence, Data processing (extract, transform, load - ETL)</t>
+  </si>
+  <si>
+    <t>Guided self help, Telemedicine appointments, Interactive services/chatbots, Remote patient (or person) monitoring</t>
+  </si>
+  <si>
+    <t>Integration and data exchange with local health facility (EMR), Integration with national health systems (DHIS2 or other)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A description of the Minimum Viable Product of the solution has been provided. As more funding becomes available, and based on feedback, even as received from filling this form, we will continue to iterate and build more features.  </t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/company/norrigwellnesssolutions</t>
+  </si>
+  <si>
+    <t>Mkata Nyoni</t>
+  </si>
+  <si>
+    <t>mnyoni@tanzmed.africa</t>
+  </si>
+  <si>
+    <t>Africa Healthtech Limited</t>
+  </si>
+  <si>
+    <t>TanzMED</t>
+  </si>
+  <si>
+    <t>TanzMED is transforming the healthcare landscape across Tanzania and East Africa by making high-quality, affordable, and personalized healthcare services accessible to everyone, regardless of their location or socioeconomic status. We harness the power of AI and data analytics to deliver efficient and effective care tailored to the unique needs of our users.
+Our comprehensive platform offers a range of services, including:
+-- Telemedicine: Seamless virtual consultations with healthcare providers.
+-- Mental Health Resources: Counseling and support to address mental health needs.
+-- Maternal &amp; Neonatal Care: Expert guidance during pregnancy and early childhood.
+-- Women's Health: Reproductive health, family planning, and menstrual cycle tracking.
+-- ePharmacy &amp; eLab: Convenient access to medications and laboratory services.
+-- Pediatric Care: Growth and development monitoring for children.
+-- HIV/AIDS Resources: Prevention, testing, and treatment information.
+-- Reproductive Health: Fertility tracking and sexual health education.
+-- BMI &amp; Weight Control: Tools for managing healthy weight.
+-- Vaccines &amp; Medication Reminders: Automated healthcare reminders.
+Available in both English and Swahili, TanzMED’s user-friendly platform is designed to meet the needs of diverse users, from mothers to community health workers. Through strategic partnerships, we aim to break down the barriers to healthcare access and make quality care a reality for everyone.</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1FUFfismyc0C6ceMx6H9cSvWwVdFOS5lf</t>
+  </si>
+  <si>
+    <t>hello@tanzmed.africa</t>
+  </si>
+  <si>
+    <t>AI for Health, Virtual Health, Vaccination</t>
+  </si>
+  <si>
+    <t>TanzMED is specifically designed to address the unique healthcare challenges faced in African countries, particularly in underserved areas where access to quality healthcare is limited. By leveraging digital innovations and AI-driven technologies, TanzMED aims to improve health outcomes across the continent through several key approaches:
+1. Bridging the Healthcare Access Gap
+In many parts of Africa, healthcare infrastructure is limited, with many people living in rural areas far from healthcare facilities. TanzMED’s telemedicine platform enables patients to connect with healthcare providers from the comfort of their homes, regardless of geographic location. This solution reduces travel time and costs associated with seeking care, especially in regions with a shortage of healthcare professionals.
+2. Improving Mental Health Support
+Mental health services in Africa are often under-resourced, stigmatized, or inaccessible. TanzMED’s mental health resources, including AI-powered chatbots and access to licensed therapists, provide a safe and private way for individuals to seek help. By offering services in local languages (English and Swahili), TanzMED is breaking down barriers to mental health care, especially for youth, where stigma is a significant deterrent.
+3. Maternal &amp; Child Health Improvement
+Africa faces high rates of maternal and neonatal mortality due to inadequate healthcare access. TanzMED addresses this by providing maternal and neonatal care services, allowing pregnant women and new mothers to receive timely expert advice and guidance. This helps monitor pregnancies, ensures safe deliveries, and supports the healthy development of newborns.
+4. Preventive Care and Disease Management
+Many African countries face high burdens of preventable diseases such as HIV/AIDS and non-communicable diseases (NCDs). TanzMED’s reproductive health tools offer essential services such as fertility tracking, family planning, and sexual health education, while also providing HIV/AIDS resources for testing, prevention, and treatment. Additionally, the platform offers BMI &amp; weight control tools to promote healthy lifestyles and combat rising cases of obesity and diabetes.
+5. Enhancing Treatment Compliance
+In Africa, medication non-compliance is a major issue leading to poor health outcomes. TanzMED’s vaccine and medication reminders send automated alerts to users, ensuring they don’t miss vital treatments or vaccinations, ultimately improving adherence and reducing the burden of preventable diseases.
+6. Affordability &amp; Scalability
+Cost is a significant barrier to healthcare access in Africa. TanzMED provides affordable healthcare services, ensuring that users can access consultations, medications, and health education without financial strain. By using a digital platform, TanzMED is also highly scalable, with the ability to reach large populations across Africa quickly and effectively, particularly through strategic partnerships and mobile technology integration.
+7. Localized Solutions with a User-Centric Approach
+TanzMED’s platform is built with a deep understanding of the African context. By providing services in local languages and tailoring content to specific health needs across different regions, the platform ensures that users can access culturally relevant and actionable health information. TanzMED’s data-driven approach further enables targeted health interventions, improving user engagement and health outcomes.</t>
+  </si>
+  <si>
+    <t>TanzMED addresses a significant market need in Africa, where healthcare systems are often overburdened, and access to quality healthcare remains limited, particularly in rural and underserved areas. Here's how TanzMED fills this gap and its impact on the African health ecosystem:
+Market Need
+Limited Access to Healthcare: Many people in Africa, especially in rural areas, struggle to access quality healthcare due to long distances, high costs, and a shortage of healthcare professionals.
+Mental Health Support: Mental health services are scarce, and stigma prevents many people from seeking help, particularly youth.
+Maternal &amp; Child Health: High rates of maternal and child mortality highlight the need for accessible healthcare during pregnancy and early childhood.
+Preventive Health: There is a lack of accessible health education and tools for managing preventable diseases like HIV and non-communicable diseases (NCDs).
+Digital Solutions: Despite high mobile phone usage, there are few digital health platforms that offer accessible healthcare services in local languages.
+TanzMED’s Impact
+Reaching 4.3 Million Users: TanzMED has expanded to four countries—Tanzania, Kenya, Congo, and Uganda providing healthcare services to millions.
+Health Education: Over 600 health articles have been read more than 21 million times, helping people make informed health decisions.
+Maternal Health: TanzMED supports 1,000 maternal clinics, improving care for pregnant women and mothers.
+Symptom Assessment: Over 3,000 users have benefited from the tool, which helps people understand their health symptoms and seek care.
+Mental Health for Youth: More than 2,000 young people are using TanzMED’s mental health tools to manage their well-being.
+Empowering Health Workers: TanzMED has trained 300 Community Health Workers (CHWs), improving healthcare delivery at the community level.</t>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Kenya, Congo (DRC), Uganda and USA</t>
+  </si>
+  <si>
+    <t>https://tanzmed.co.tz/privacy-policy.html</t>
+  </si>
+  <si>
+    <t>TanzMED ensures the privacy and protection of Personal Health Information (PHI) through the following measures:
+Encryption: All user data is encrypted both in transit and at rest, ensuring secure communication and storage of sensitive health information.
+Compliance with Data Protection Laws: TanzMED follows international and local data protection regulations.
+Access Controls: Only authorized personnel have access to user data, with strict authentication measures in place.
+Anonymization: User data is anonymized for reporting and analytics to prevent the identification of individuals, even Doctors can not see previous chat records.
+Regular Security Audits: TanzMED conducts regular security audits and updates to protect against data breaches and vulnerabilities.</t>
+  </si>
+  <si>
+    <t>Activity Logs: Tracks all user actions on the platform.
+Immutable Logs: Logs are stored securely and cannot be altered.
+Access Control: Only authorized personnel can access logs.
+Automated Alerts: Alerts for any suspicious activity or login to backend Doctor portal.
+Log Retention: Logs are stored based on policy for compliance.</t>
+  </si>
+  <si>
+    <t>Users need username and Password, SMS/WhatsApp OTP is used as Double Authentication method (TFA)</t>
+  </si>
+  <si>
+    <t>Online medicine ordering</t>
+  </si>
+  <si>
+    <t>Home/Office lab test booking</t>
+  </si>
+  <si>
+    <t>Track and trace, Case reporting, Case Investigation, Vaccine-related adverse events monitoring</t>
+  </si>
+  <si>
+    <t>Data visualization, Dashboards, Clinical data dashboards, Business Intelligence</t>
+  </si>
+  <si>
+    <t>Vaccine-related adverse events monitoring, Maternal Vaccination Reminders</t>
+  </si>
+  <si>
+    <t>In addition to the features listed earlier, TanzMED offers several other key functionalities:
+Mental Health Tools:
+Mental Health Assessment: Users can assess their mental well-being using AI-driven tools.
+Mood Tracker: Allows users to log and track their moods over time for better mental health management.
+Goal Tracking: Helps users set and monitor personal health and wellness goals.
+HIV/AIDS Support:
+CTC Tracker: Monitors HIV treatment progress for users attending Care and Treatment Clinics (CTC).
+CTC Appointment Booking: Allows users to schedule and manage their clinic appointments.
+Youth HIV/AIDS Risk Factor Assessment: Offers tools to assess and educate youth on HIV risk factors.
+Women Health:
+Pregnancy Tracker: Helps expecting mothers track their pregnancy milestones.
+Clinic Day &amp; Service Reminders: Sends automated reminders for important clinic visits and services.
+SRH: Allow Girls and Young Women to track their period, reminded on period cycle and get direct Support form specialists.
+Virtual Doctor Chats: Users can consult healthcare professionals through virtual chat or call, ensuring easy access to medical advice and consultations.</t>
+  </si>
+  <si>
+    <t>https://tanzmed.africa</t>
+  </si>
+  <si>
+    <t>Henry Mathayo</t>
+  </si>
+  <si>
+    <t>henry@medpack.co.tz</t>
+  </si>
+  <si>
+    <t>MedPack Inc.</t>
+  </si>
+  <si>
+    <t>MedPack Business</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MedPack Business  is a digital platform that revolutionizes the pharmaceutical supply chain by providing an efficient, technology-driven solution for healthcare facilities to procure and manage essential medicines. Designed for pharmacies, hospitals, clinics, and health centers, MedPack streamlines the procurement process by offering real-time access to a vast network of suppliers. It not only enables healthcare providers to order medications, but also integrates features like inventory management, digital payments, and microfinancing, allowing facilities to buy medicines on credit, improving cash flow.
+MedPack offers unique value by guaranteeing delivery of medications within three hours in urban areas, while also serving rural and underserved regions. The platform helps healthcare providers maintain stock levels, avoid shortages, and provide patients with timely, life-saving treatments.
+</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1dmbhRI8mPSowZVpnzXw_dgqehXwjS18Z</t>
+  </si>
+  <si>
+    <t>Pharmacy, Analytics and Data Aggregation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MedPack is a digital health platform designed to improve the pharmaceutical supply chain, specifically in Africa. By addressing the chronic issue of stockouts and inefficient distribution, MedPack ensures that healthcare facilities across the continent have timely access to essential medicines. The platform offers an integrated system for real-time procurement, inventory management, and microfinancing, which allows health centers to maintain optimal stock levels and reduce shortages. With a unique focus on rural and underserved areas, MedPack ensures that critical medications reach those who need them the most, offering 3-hour delivery within urban centers and efficient distribution to remote areas. This innovation directly enhances healthcare outcomes by ensuring patients receive timely treatment, improving overall public health and reducing mortality rates.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tanzania boasts over 25,000 healthcare facilities, including pharmacies, clinics, health centers, and hospitals, serving a population of more than 60 million people. Currently, MedPack services 1,012 facilities, representing around 4% of the market. Given the widespread need for reliable, digital procurement systems, the Wezesha Project seeks to expand to 2,000 facilities within the next six months. With the healthcare sector in Tanzania growing steadily, there is significant room for MedPack to scale its operations, potentially reaching 20-30% market penetration in the coming years as demand for digital health solutions rises.
+Currently operational in Tanzania, MedPack plans to expand to the Southern African Development Community (SADC), serving millions of patients. With more facilities gaining access to MedPack, we are on track to significantly enhance healthcare outcomes across Africa by ensuring faster deliveries and affordable financing for health centers, especially in rural areas.
+</t>
+  </si>
+  <si>
+    <t>Dar es salaam, Tanzania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tanzania </t>
+  </si>
+  <si>
+    <t>100% Africans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100% local developed </t>
+  </si>
+  <si>
+    <t>1012 health facilities (Customers)</t>
+  </si>
+  <si>
+    <t>1 country - Tanzania</t>
+  </si>
+  <si>
+    <t>1012 users</t>
+  </si>
+  <si>
+    <t>350+ completed orders  worth $22,000+/Month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MedPack is deeply committed to ensuring the privacy and protection of Personal Health Information (PHI) in compliance with global standards such as the Health Insurance Portability and Accountability Act (HIPAA) and local data protection laws. Our platform employs multiple layers of security to safeguard sensitive data at every stage.
+Data Encryption: All PHI is encrypted both at rest and in transit using industry-standard encryption methods. This ensures that data is unreadable if intercepted.
+Access Control: We enforce strict access controls, ensuring that only authorized personnel can view or manage patient data. User permissions are role-based, minimizing unnecessary exposure to PHI.
+Secure Authentication: MedPack utilizes multi-factor authentication (MFA) for users accessing the platform, adding an extra layer of security to prevent unauthorized logins.
+Data Minimization: We collect only the necessary information for the provision of healthcare services, ensuring that no unnecessary personal data is stored or shared.
+Compliance and Auditing: MedPack regularly audits its data handling processes and undergoes compliance checks to ensure adherence to privacy regulations.
+</t>
+  </si>
+  <si>
+    <t>Dispensing and Medication Administration Record (MAR), Inventory Management, Decision Support</t>
+  </si>
+  <si>
+    <t>https://www.medpack.co.tz</t>
+  </si>
+  <si>
+    <t>Mostafa Dawoud</t>
+  </si>
+  <si>
+    <t>md@dentolize.com</t>
+  </si>
+  <si>
+    <t>Dentolize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dentolize </t>
+  </si>
+  <si>
+    <t>Dentolize offers an all-in-one clinic management software that automates administrative tasks such as appointment scheduling, patient records, billing, and communication. Through our mobile app, patients can easily book appointments, receive reminders, and access their prescriptions. Clinics benefit from a streamlined workflow that enhances efficiency, improves patient care, and reduces operational overhead, allowing them to focus more on delivering quality healthcare.</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1JK44kt--96mfUOM1d7_k3RNmDYu-KKw2</t>
+  </si>
+  <si>
+    <t>info@dentolize.com</t>
+  </si>
+  <si>
+    <t>Electronic Health Record, Analytics and Data Aggregation, AI for Health</t>
+  </si>
+  <si>
+    <t>Dentolize enhances healthcare in Africa by streamlining clinic management, improving patient care, and reducing administrative burdens. Our platform supports digital appointment scheduling, patient record management, and automated billing, making healthcare more accessible. We also integrate telemedicine and digital invoicing, catering to underserved areas with limited access to traditional healthcare. By improving clinic efficiency, Dentolize contributes to better health outcomes across Africa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cairo, Egypt </t>
+  </si>
+  <si>
+    <t>Egypt, Libya, Tunisia, Morocco, South Africa, Sudan and Nigeria</t>
+  </si>
+  <si>
+    <t>1000+ Unique customers</t>
+  </si>
+  <si>
+    <t>19 countries</t>
+  </si>
+  <si>
+    <t>https://dentolize.com/privacy-policy/</t>
+  </si>
+  <si>
+    <t>Patient Record Management, Clinical decision support, CPOE/Order Management, Patient Billing, Patient Data Import/Export, X-Ray and Imaging, Patient care templates, Encounter Data Import/Export, Surgical Management, Virtual care, Encounter Workflow Support</t>
+  </si>
+  <si>
+    <t>Inventory Management, Electronic prescribing, EHR Integration</t>
+  </si>
+  <si>
+    <t>Inventory Management, EHR Integration</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1467,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border/>
     <border>
       <left style="thin">
@@ -1276,20 +1623,6 @@
         <color rgb="FF442F65"/>
       </bottom>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFF8F9FA"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF442F65"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF8F9FA"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF442F65"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
@@ -1403,6 +1736,9 @@
     <xf borderId="5" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -1413,9 +1749,6 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1476,7 +1809,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:BD13" displayName="Form_Responses1" name="Form_Responses1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:BD17" displayName="Form_Responses1" name="Form_Responses1" id="1">
   <tableColumns count="56">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Your name" id="2"/>
@@ -3446,131 +3779,664 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="36">
+      <c r="A13" s="25">
         <v>45562.248555115744</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="26" t="s">
         <v>288</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="26" t="s">
         <v>289</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="26" t="s">
         <v>290</v>
       </c>
-      <c r="E13" s="37" t="s">
+      <c r="E13" s="26" t="s">
         <v>291</v>
       </c>
-      <c r="F13" s="37" t="s">
+      <c r="F13" s="26" t="s">
         <v>292</v>
       </c>
-      <c r="G13" s="38" t="s">
+      <c r="G13" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="H13" s="37" t="s">
+      <c r="H13" s="26" t="s">
         <v>294</v>
       </c>
-      <c r="I13" s="37" t="s">
+      <c r="I13" s="26" t="s">
         <v>295</v>
       </c>
-      <c r="J13" s="37" t="s">
+      <c r="J13" s="26" t="s">
         <v>296</v>
       </c>
-      <c r="K13" s="37" t="s">
+      <c r="K13" s="26" t="s">
         <v>297</v>
       </c>
-      <c r="L13" s="37" t="s">
+      <c r="L13" s="26" t="s">
         <v>298</v>
       </c>
-      <c r="M13" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="N13" s="37" t="s">
+      <c r="M13" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="N13" s="26" t="s">
         <v>269</v>
       </c>
-      <c r="O13" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="P13" s="39">
+      <c r="O13" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="P13" s="28">
         <v>1.0</v>
       </c>
-      <c r="Q13" s="39">
+      <c r="Q13" s="28">
         <v>1.0</v>
       </c>
-      <c r="R13" s="37" t="s">
+      <c r="R13" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="S13" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="T13" s="37" t="s">
+      <c r="S13" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="T13" s="26" t="s">
         <v>299</v>
       </c>
-      <c r="U13" s="37">
+      <c r="U13" s="26">
         <v>1.0</v>
       </c>
-      <c r="V13" s="37">
+      <c r="V13" s="26">
         <v>400.0</v>
       </c>
-      <c r="W13" s="37">
+      <c r="W13" s="26">
         <v>2000.0</v>
       </c>
-      <c r="Y13" s="37" t="s">
+      <c r="Y13" s="26" t="s">
         <v>300</v>
       </c>
-      <c r="Z13" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB13" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC13" s="38" t="s">
+      <c r="Z13" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB13" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC13" s="27" t="s">
         <v>301</v>
       </c>
-      <c r="AI13" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ13" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="AM13" s="37" t="s">
+      <c r="AI13" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ13" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM13" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="AN13" s="37" t="s">
+      <c r="AN13" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="AO13" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="AQ13" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="AR13" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS13" s="37" t="s">
+      <c r="AO13" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ13" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR13" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS13" s="26" t="s">
         <v>302</v>
       </c>
-      <c r="AT13" s="37" t="s">
+      <c r="AT13" s="26" t="s">
         <v>303</v>
       </c>
-      <c r="AV13" s="37" t="s">
+      <c r="AV13" s="26" t="s">
         <v>304</v>
       </c>
-      <c r="AY13" s="37" t="s">
+      <c r="AY13" s="26" t="s">
         <v>305</v>
       </c>
-      <c r="AZ13" s="37" t="s">
+      <c r="AZ13" s="26" t="s">
         <v>273</v>
       </c>
-      <c r="BA13" s="37" t="s">
+      <c r="BA13" s="26" t="s">
         <v>306</v>
       </c>
-      <c r="BC13" s="37" t="s">
+      <c r="BC13" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="BD13" s="40" t="s">
+      <c r="BD13" s="30" t="s">
         <v>308</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="31">
+        <v>45564.18480020833</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>309</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>310</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>311</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>311</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>312</v>
+      </c>
+      <c r="G14" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="H14" s="32" t="s">
+        <v>310</v>
+      </c>
+      <c r="I14" s="32" t="s">
+        <v>314</v>
+      </c>
+      <c r="J14" s="32" t="s">
+        <v>315</v>
+      </c>
+      <c r="K14" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="L14" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="M14" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="N14" s="32" t="s">
+        <v>317</v>
+      </c>
+      <c r="O14" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="P14" s="32" t="s">
+        <v>318</v>
+      </c>
+      <c r="Q14" s="32" t="s">
+        <v>318</v>
+      </c>
+      <c r="R14" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="S14" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="T14" s="32" t="s">
+        <v>319</v>
+      </c>
+      <c r="U14" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="V14" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="W14" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="X14" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y14" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="Z14" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA14" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="AB14" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC14" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="AD14" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE14" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="AF14" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG14" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="AH14" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="AI14" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM14" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN14" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="AO14" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP14" s="32" t="s">
+        <v>324</v>
+      </c>
+      <c r="AQ14" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR14" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AX14" s="32" t="s">
+        <v>325</v>
+      </c>
+      <c r="AY14" s="32" t="s">
+        <v>326</v>
+      </c>
+      <c r="AZ14" s="32" t="s">
+        <v>327</v>
+      </c>
+      <c r="BB14" s="32" t="s">
+        <v>328</v>
+      </c>
+      <c r="BC14" s="33" t="s">
+        <v>329</v>
+      </c>
+      <c r="BD14" s="36" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="25">
+        <v>45565.538122025464</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>333</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>335</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>337</v>
+      </c>
+      <c r="J15" s="26" t="s">
+        <v>338</v>
+      </c>
+      <c r="K15" s="26" t="s">
+        <v>339</v>
+      </c>
+      <c r="L15" s="26" t="s">
+        <v>340</v>
+      </c>
+      <c r="M15" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="N15" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="O15" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="P15" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="Q15" s="28">
+        <v>0.9</v>
+      </c>
+      <c r="R15" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="S15" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="T15" s="26">
+        <v>31260.0</v>
+      </c>
+      <c r="U15" s="26">
+        <v>5.0</v>
+      </c>
+      <c r="V15" s="26">
+        <v>6000.0</v>
+      </c>
+      <c r="W15" s="29">
+        <v>11399.0</v>
+      </c>
+      <c r="X15" s="29">
+        <v>96543.0</v>
+      </c>
+      <c r="Y15" s="29">
+        <v>45000.0</v>
+      </c>
+      <c r="Z15" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB15" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD15" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF15" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG15" s="27" t="s">
+        <v>342</v>
+      </c>
+      <c r="AH15" s="26" t="s">
+        <v>343</v>
+      </c>
+      <c r="AI15" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ15" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK15" s="26" t="s">
+        <v>344</v>
+      </c>
+      <c r="AL15" s="26" t="s">
+        <v>345</v>
+      </c>
+      <c r="AM15" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN15" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO15" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ15" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR15" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AT15" s="26" t="s">
+        <v>346</v>
+      </c>
+      <c r="AU15" s="26" t="s">
+        <v>347</v>
+      </c>
+      <c r="AV15" s="26" t="s">
+        <v>348</v>
+      </c>
+      <c r="AX15" s="26" t="s">
+        <v>349</v>
+      </c>
+      <c r="AY15" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="BA15" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="BB15" s="26" t="s">
+        <v>351</v>
+      </c>
+      <c r="BC15" s="27" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="31">
+        <v>45565.5513366088</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>355</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>356</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>357</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>358</v>
+      </c>
+      <c r="H16" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="I16" s="32" t="s">
+        <v>359</v>
+      </c>
+      <c r="J16" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="K16" s="32" t="s">
+        <v>361</v>
+      </c>
+      <c r="L16" s="32" t="s">
+        <v>362</v>
+      </c>
+      <c r="M16" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="N16" s="32" t="s">
+        <v>363</v>
+      </c>
+      <c r="O16" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="P16" s="32" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q16" s="32" t="s">
+        <v>365</v>
+      </c>
+      <c r="R16" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="S16" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="T16" s="32" t="s">
+        <v>366</v>
+      </c>
+      <c r="U16" s="32" t="s">
+        <v>367</v>
+      </c>
+      <c r="V16" s="32" t="s">
+        <v>368</v>
+      </c>
+      <c r="W16" s="32" t="s">
+        <v>369</v>
+      </c>
+      <c r="X16" s="35">
+        <v>267643.0</v>
+      </c>
+      <c r="Y16" s="35">
+        <v>25000.0</v>
+      </c>
+      <c r="Z16" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB16" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD16" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF16" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH16" s="32" t="s">
+        <v>370</v>
+      </c>
+      <c r="AI16" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM16" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN16" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO16" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ16" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR16" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AT16" s="32" t="s">
+        <v>371</v>
+      </c>
+      <c r="AX16" s="32" t="s">
+        <v>325</v>
+      </c>
+      <c r="BC16" s="33" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="37">
+        <v>45565.592789525464</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>373</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>374</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>375</v>
+      </c>
+      <c r="E17" s="38" t="s">
+        <v>376</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>377</v>
+      </c>
+      <c r="G17" s="39" t="s">
+        <v>378</v>
+      </c>
+      <c r="H17" s="38" t="s">
+        <v>379</v>
+      </c>
+      <c r="I17" s="38" t="s">
+        <v>380</v>
+      </c>
+      <c r="J17" s="38" t="s">
+        <v>381</v>
+      </c>
+      <c r="L17" s="38" t="s">
+        <v>382</v>
+      </c>
+      <c r="M17" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="N17" s="38" t="s">
+        <v>383</v>
+      </c>
+      <c r="O17" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="P17" s="40">
+        <v>1.0</v>
+      </c>
+      <c r="Q17" s="40">
+        <v>1.0</v>
+      </c>
+      <c r="R17" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="S17" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="T17" s="38" t="s">
+        <v>384</v>
+      </c>
+      <c r="U17" s="38" t="s">
+        <v>385</v>
+      </c>
+      <c r="V17" s="38">
+        <v>9000.0</v>
+      </c>
+      <c r="W17" s="38">
+        <v>800000.0</v>
+      </c>
+      <c r="X17" s="38">
+        <v>250000.0</v>
+      </c>
+      <c r="Y17" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z17" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB17" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD17" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF17" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG17" s="39" t="s">
+        <v>386</v>
+      </c>
+      <c r="AI17" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ17" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM17" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN17" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="AO17" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ17" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR17" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS17" s="38" t="s">
+        <v>387</v>
+      </c>
+      <c r="AT17" s="38" t="s">
+        <v>388</v>
+      </c>
+      <c r="AU17" s="38" t="s">
+        <v>389</v>
+      </c>
+      <c r="AX17" s="38" t="s">
+        <v>349</v>
+      </c>
+      <c r="AY17" s="38" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3607,10 +4473,19 @@
     <hyperlink r:id="rId30" ref="BC12"/>
     <hyperlink r:id="rId31" ref="G13"/>
     <hyperlink r:id="rId32" ref="AC13"/>
+    <hyperlink r:id="rId33" ref="G14"/>
+    <hyperlink r:id="rId34" ref="BC14"/>
+    <hyperlink r:id="rId35" ref="G15"/>
+    <hyperlink r:id="rId36" ref="AG15"/>
+    <hyperlink r:id="rId37" ref="BC15"/>
+    <hyperlink r:id="rId38" ref="G16"/>
+    <hyperlink r:id="rId39" ref="BC16"/>
+    <hyperlink r:id="rId40" ref="G17"/>
+    <hyperlink r:id="rId41" ref="AG17"/>
   </hyperlinks>
-  <drawing r:id="rId33"/>
+  <drawing r:id="rId42"/>
   <tableParts count="1">
-    <tablePart r:id="rId35"/>
+    <tablePart r:id="rId44"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add to list of health solutions
</commit_message>
<xml_diff>
--- a/utils/HealthSolutionsData.xlsx
+++ b/utils/HealthSolutionsData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="823">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1402,14 +1402,1626 @@
   <si>
     <t>Inventory Management, EHR Integration</t>
   </si>
+  <si>
+    <t>Ahmad Al-Kabbany</t>
+  </si>
+  <si>
+    <t>alkabbany@myvrapeutic.com</t>
+  </si>
+  <si>
+    <t>VRapeutic Inc.</t>
+  </si>
+  <si>
+    <t>Yubreevi</t>
+  </si>
+  <si>
+    <t>Yubreevi is a system that enables the delivery of remotely supervised physical rehabilitation sessions, with a major focus on children with motor disorders. The proposed system combines VR with machine learning to realize data-centered, context-rich training plans.</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1f_uSSbyYVahup8Kyca3jnJhhgT5PFTYx</t>
+  </si>
+  <si>
+    <t>info@myvrapeutic.com</t>
+  </si>
+  <si>
+    <t>Electronic Health Record, AI for Health, Virtual Health</t>
+  </si>
+  <si>
+    <t>WHO reports that around 400 million person in Africa would benefit from rehabilitation.
+Another estimate indicates that 80% of the world’s disabled population live in Africa.
+Accordingly, the societal and economic impact of providing high-quality, science-backed,
+unconventional, and effective physical healthcare is HUGE, and the need for better
+healthcare that harnesses the power of technology is significantly pressing.
+Also, providing means of effective early intervention to highly prevalent physical developmental disorders has been shown to lead to higher chances of recovery and higher
+quality of life. This would have a positive impact on the readiness of future workforces. Finally, a positive impact on a population's health, including the senior population, is supposed to promote social inclusion.
+Our proposed system empowers healthcare facilities to deliver higher quality healthcare, with higher accessibility potential, using better user-centric systems, and data-driven design that facilitates better follow-up, rehab plans development, and health insurance coverage.</t>
+  </si>
+  <si>
+    <t>Since we operate in Egypt, this response will focus on Egypt only. Nevertheless, our solution is very scalable, and it addresses challenges that are common between Egypt and the African ecosystem at large. 
+Market needs that this solution fills:
+============================
+There is a growing need for physical rehabilitation in Egypt. A rough estimate would surpass
+five million Egyptians who need physical healthcare. The need has recently expanded beyond people with disabilities to include typical adults, early seniors, and even children. This is due to several factors including modern lifestyles and daily habits which are strongly affected by electronic devices, transportation patterns, in addition to other factors. 
+The challenges of delivering high quality physical rehabilitation in Egypt is multi-fold. First,
+there is lack of patients’ commitment to physical rehabilitation plans due to low
+engagement level of traditional interventions approaches. So, it is a matter of quality.
+Second, there is a challenge in providing tele-healthcare services for physical rehabilitation,
+mainly because classical interventions don’t support this. Reducing commutes would
+result in societal as well as environmental positive impact.
+Third, there is lack of data centered, automated, real-time performance data acquisition and
+analysis, which is realized when the user is at the center of the design goals. So, it is a matter of user centrism.
+The impact this health solution has made in the African health ecosystem
+============================================================
+We are currently collaborating with the Faculty of Physical Therapy of Cairo University in Egypt, and their affiliated on-campus outpatient clinics. Our solution has been consistently used for 2 years in their therapy sessions that have targeted several conditions including cerebral palsy-related disorders such as hypertonia and deficient bilateral coordination, shoulder disorders such as Erb's palsy, and neck disorders such as faulty head posture.
+An example of a publication that documented the positive impact of our solution can be found through the following link:
+https://www.semanticscholar.org/paper/Movement-analysis-of-fully-immersive-virtual-module-Allah-Khalil/f994ca87de3d0efe6a34484b8b20103a582febd9
+The authors of the above publication are professors and researchers at the Faculty of Physical Therapy of Cairo University in Egypt.</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>We are B2B, selling to hospitals, clinics, and centers. While our current customers are 8 centers, our current end-users exceed 500 children and adult.</t>
+  </si>
+  <si>
+    <t>Egypt and Vietnam.</t>
+  </si>
+  <si>
+    <t>An average of 5 users a day.</t>
+  </si>
+  <si>
+    <t>An average of 2 transactions per month.</t>
+  </si>
+  <si>
+    <t>We make 5000 USD as a monthly recurring revenue. This sums up to 60000 USD a year.</t>
+  </si>
+  <si>
+    <t>280,000 USD including investments and grants</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1r29OY1ABIf1cDXBsbwvihAsdflGJwrhS/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://myvrapeutic.com/privacy-policy/</t>
+  </si>
+  <si>
+    <t>Our solution upholds the guidelines of HIPAA compliance which can be found here:
+https://www.hhs.gov/hipaa/for-professionals/security/laws-regulations/index.html</t>
+  </si>
+  <si>
+    <t>Please, find VRapeutic’s document of Accounting Policy and Procedures through the following link:
+https://drive.google.com/file/d/1r29OY1ABIf1cDXBsbwvihAsdflGJwrhS/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>VRapeutic’s adopted mechanisms for authentication and authorization are a part of the company’s Accounting Policy and Procedures document. Please, see our response to the previous question.</t>
+  </si>
+  <si>
+    <t>Patient Record Management, Individual Registration, Patient Data Import/Export, Virtual care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not applicable </t>
+  </si>
+  <si>
+    <t>Capture results from digital devices, EHR Integration</t>
+  </si>
+  <si>
+    <t>While we are not currently integrating our patient records with any public or governmental databases, our records and databases were designed to be ready for integration. They are now being hosted on AWS which is a HIPAA compliant cloud services provider.</t>
+  </si>
+  <si>
+    <t>https://myvrapeutic.com/</t>
+  </si>
+  <si>
+    <t>OUATTARA CORINE MAURICE</t>
+  </si>
+  <si>
+    <t>dg@mcm-ci.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCM </t>
+  </si>
+  <si>
+    <t>Pass Sante Mousso</t>
+  </si>
+  <si>
+    <t>PASS SANTÉ MOUSSO is an integrated digital health solution enabling the management of electronic medical records, telemedicine and vaccination tracking. The solution includes physical media such as a bracelet, a card and a waterproof smartwatch, promoting the mobility of medical data. Connected to the platform (digital health record), these media ensure real-time monitoring, with instant sharing of medical information to healthcare professionals, thus enabling better care and increased responsiveness in the event of an emergency, especially for chronically ill patients.</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1quC2yy8zPQJGFcEt0ylIUGa78Y_14uIr</t>
+  </si>
+  <si>
+    <t>emmazebre@santemousso.net</t>
+  </si>
+  <si>
+    <t>Electronic Health Record, Pharmacy, Disease Surveillance, National and Community Health, Front-line (CHW) tools, Vaccination</t>
+  </si>
+  <si>
+    <t>PASS SANTE MOUSSO contributes to improving health outcomes in Africa by providing a secure and easily accessible digital infrastructure for patient monitoring. It allows vulnerable populations, particularly in rural areas, to benefit from faster and more efficient health management. By integrating with public and private health systems, it improves continuity of care and allows health professionals to make more informed decisions thanks to medical information available in real time.</t>
+  </si>
+  <si>
+    <t>PASS SANTE MOUSSO addresses the critical need for centralized medical information and access to healthcare for patients in Africa. Fragmented healthcare systems, lack of chronic disease monitoring, and limited access to care in rural areas have generated a growing need for a solution like this. To date, PASS SANTE MOUSSO has enrolled over 67,000 people in Côte d’Ivoire, with a direct impact on the monitoring of 3,744 cancer patients in partnership with CNRAO. The solution helps streamline care, improve access to medical services, and reduce the cost of care for patients.</t>
+  </si>
+  <si>
+    <t>Abidjan, Côte d'Ivoire</t>
+  </si>
+  <si>
+    <t>BENIN, SENEGAL, TOGO, BURKINA FASO</t>
+  </si>
+  <si>
+    <t>100% (All members of the management team are based in Africa, specifically in Ivory Coast)</t>
+  </si>
+  <si>
+    <t>100% (All software development was carried out by African developers, specifically Ivorian)</t>
+  </si>
+  <si>
+    <t>The solution is currently deployed in 97 healthcare structures with more than 1,237 healthcare professionals using the platform, and 67,297 patients enrolled.</t>
+  </si>
+  <si>
+    <t>The solution is currently deployed in Ivory Coast and as a pilot in Benin, Senegal, Togo, and Burkina Faso</t>
+  </si>
+  <si>
+    <t>Approximately 5,000 daily active users, including patients and healthcare professionals</t>
+  </si>
+  <si>
+    <t>The solution processes approximately 10,000 monthly transactions, including access to medical records and medical consultations.</t>
+  </si>
+  <si>
+    <t>The current annual revenue of the organization for the year 2023 is 59,685,645 FCFA, which is approximately 97,050 USD</t>
+  </si>
+  <si>
+    <t>No external funding has been raised so far. The project has been entirely self-financed, and grants were obtained to support the development of the solution.</t>
+  </si>
+  <si>
+    <t>https://santemousso.net/politique-confidentialite</t>
+  </si>
+  <si>
+    <t>The PASS SANTE MOUSSO solution uses data encryption and strict protocols for accessing health information. Only authorized persons, such as healthcare professionals, can access patients' medical records. The system follows local data protection rules and international best practices in terms of security.</t>
+  </si>
+  <si>
+    <t>The solution uses audit logging tools to track all user actions and transactions in the system, ensuring complete traceability of access and changes. Errors are reported in real time and tracked using an incident management system.</t>
+  </si>
+  <si>
+    <t>Authentication for PASS SANTE MOUSSO is done via a secure role-based system with a login and password for healthcare professional users. For patient identification, an ID, PIN, and phone number are used. Patients receive a notification each time their medical record is consulted to enhance transparency and security. Two-factor authentication (2FA) can also be used for additional levels of security. Access rights are defined according to user roles (healthcare professionals, patients, administrators), ensuring that each user can only access data relevant to their role.</t>
+  </si>
+  <si>
+    <t>Patient Record Management, Individual Registration, Clinical decision support, Patient Billing, Patient Data Import/Export, Patient care templates, ER - Triage and Dashboard, Virtual care</t>
+  </si>
+  <si>
+    <t>Dispensing and Medication Administration Record (MAR), Drug interaction monitoring, Electronic prescribing</t>
+  </si>
+  <si>
+    <t>Transmit and track diagnostic orders, Send diagnostic results to providers, EHR Integration</t>
+  </si>
+  <si>
+    <t>Case reporting, Vaccine-related adverse events monitoring</t>
+  </si>
+  <si>
+    <t>National health domain-specific registries, Clinical data repository, Clinical data warehouse</t>
+  </si>
+  <si>
+    <t>Telemedicine appointments, Remote patient (or person) monitoring</t>
+  </si>
+  <si>
+    <t>Customizable data collection forms, Integration and data exchange with local health facility (EMR), Integration with national health systems (DHIS2 or other)</t>
+  </si>
+  <si>
+    <t>Patient vaccination record, Digital vaccine card, Vaccine-related adverse events monitoring</t>
+  </si>
+  <si>
+    <t>PASS SANTE MOUSSO inclut également une plateforme pour la téléconsultation, la gestion des constantes vitales des patients, ainsi que l'accès à des services de paiement flexibles via PassPay</t>
+  </si>
+  <si>
+    <t>https://santemousso.net/</t>
+  </si>
+  <si>
+    <t>Joseph Olowe</t>
+  </si>
+  <si>
+    <t>joseph@josmolgroup.com</t>
+  </si>
+  <si>
+    <t>Josmol Human Resources Ltd</t>
+  </si>
+  <si>
+    <t>Doktorconnect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+DoktorConnect offers a comprehensive digital health platform that leverages personalized medical care through wellness-based assessments, genetic analysis, mental health screening, and advanced technologies. By analyzing genetic data and wellness metrics, we create evidence-based lifestyle management plans for individuals. Our platform enables virtual consultations with licensed doctors, therapists, dieticians, and health coaches, along with real-time vital signs tracking using smart medical IoT devices. We also integrate AI-driven methodologies to promote healthy behaviors, lifestyle modifications, medication management, and tailored exercise regimens.
+Doktorconnect Digital Assets
+Website 
+www.doktorconnect.com/ng
+MOBILE WELLNESS UNIT
+https://bit.ly/mobile-wellness-van
+https://bit.ly/wellness-on-the-move
+PREVENTIVE HEALTH AND WELLNESS SAMPLE RESULT
+Sample result of our wellness report
+ - https://bit.ly/wellnessreportsample 
+https://bit.ly/dna-analysis-report
+https://selfdecode.com/en/selfdecode-pro-connect/
+APP DEMO
+Doktorconnect App Demo
+- https://bit.ly/DoktorconnectAppDemo
+REMOTE MONITORING AND DIAGNOSTIC TOOLS
+LifePro Body Composition SmartScale - https://bit.ly/BodyCompositionSmartScale
+6-in-1 Health Monitor - https://bit.ly/6-in-1HealthMonitor
+Lifepro Sleep Monitor - https://bit.ly/LifeproSleepMonitor
+</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=17Z6LS9hW_IGAVhKO8tpTd0HTUPtCgyRY</t>
+  </si>
+  <si>
+    <t>hello@doktorconnect.com</t>
+  </si>
+  <si>
+    <t>Pharmacy, Laboratory and Diagnostics, Analytics and Data Aggregation, Virtual Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My friend Jim died at the age of 42. Jim had diabetes. This happened because of an autoimmune disease that affected his pancreas, and he was unable to produce insulin, which led to type 1 diabetes, and he didn't know it until it was too late. He found out because of a wound he sustained at work that would not heal. Jim committed suicide. At the time of his passing, he was an amputee and severely depressed. He left two daughters and his wife with exciting data about his business and finances, but Jim was not tracking any data about his health. Since that happened, l vowed that there would not be another Jim. This is the story of 1 out 4 Africans ( especially Nigeria, the most populous nation in Africa)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMPACT-RELATED MEASURES
+In addition to financial metrics, Doktorconnect provides the following impact-related measures:
+1. Health outcomes: Tracking improvements in patient health outcomes and Overall well-being resulting from the services provided by Doktorconnect.
+2. Patient satisfaction and feedback: Monitoring patient satisfaction through surveys and feedback mechanisms to ensure that patients are receiving high-quality care and are happy with their experience.
+3. Access to care: Assessing the impact of Doktorconnect on increasing access to healthcare services, especially for underserved populations or those in remote areas.
+4. Health equity: Evaluating how Doktorconnect is contributing to reducing disparities in healthcare access and outcomes among different population groups.
+5. Employee well-being: Monitoring the well-being and job satisfaction of healthcare providers and staff working with Doktorconnect to ensure a positive and supportive work environment.
+6. Environmental sustainability: Considering the environmental impact of operations, such as energy usage, waste management, and carbon footprint, and implementing measures to promote sustainability.
+</t>
+  </si>
+  <si>
+    <t>LAGOS, Nigeria</t>
+  </si>
+  <si>
+    <t>One deployment /447,000 users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SaaS-based product </t>
+  </si>
+  <si>
+    <t>Custom API available</t>
+  </si>
+  <si>
+    <t>Within the application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIPPA, HLR 7 compliant and housed on Azure cloud services </t>
+  </si>
+  <si>
+    <t>A dedicated team auditing the platform for complaints on many fronts</t>
+  </si>
+  <si>
+    <t>Notification and multiple-factor authentication and authorization mechanism</t>
+  </si>
+  <si>
+    <t>Patient Record Management, Individual Registration, Patient Data Import/Export</t>
+  </si>
+  <si>
+    <t>Dashboards, Clinical data dashboards</t>
+  </si>
+  <si>
+    <t>www.doktorconnect.com/ng</t>
+  </si>
+  <si>
+    <t>Tobias Reiter</t>
+  </si>
+  <si>
+    <t>tobias@viebeg.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIEBEG Medical </t>
+  </si>
+  <si>
+    <t>VieProcure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viebeg offers medical equipment and products through a data-driven B2B procurement platform that de-risks and optimizes the procurement of medical equipment and supplies through Viebeg’s Health Demand Simulation Model (HDSM). 
+Our online "VieProcure" platform offers a free, data-driven procurement solution for hospitals, clinics, pharmacies and other healthcare providers. It enables a transparent and efficient procurement process, allowing healthcare providers to select from a diverse product range online, eliminating the need for time-consuming manual processes. 
+The platform is complemented by our Health Demand Simulation Model (HDSM). The HDSM, based on demographic and public health data, assesses the current availability of medical services and equipment in a specific region and then compares it to the health demand in that region, to identify healthcare infrastructure gaps. Using predictive analytics, the model also forecasts the profitability of medical equipment and the credit score of each health care provider in a specific location. Based on this data health care facilities can make informed investment decisions, address specific diseases, and enhance the efficiency of the healthcare system. 
+In addition to providing in-house equipment financing, we partner with 3rd party financing partners. For this purpose our credit scoring algorithm for equipment financing connects clients to financing partners, leveraging the HDSM for informed lending decisions.
+</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1v-gmnYSUARd8KtaIFEatsUR5C3-BMP6S</t>
+  </si>
+  <si>
+    <t>Pharmacy, Laboratory and Diagnostics, Analytics and Data Aggregation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our overarching impact vision is to transform the healthcare sector in our target markets by improving the quality of health services which are accessible, comprehensive, connected and affordable for all. Our venture creates impact in three main areas: 1) Accessibility, 2) Affordability, 3) Quality. 
+Accessibility: We provide medical equipment and products to a wide range of public and private healthcare facilities in urban and rural areas through our network of sales agents, supported by our procurement platform. This means Viebeg is a one-stop-shop for healthcare providers enabling them to offer better quality and/or new products &amp; services. As a result, patients get access to previously unavailable medical care, and disease burdens in the regions served are reduced.  
+Affordability: Our venture offers lower prices for higher quality products, equipment financing and flexible payment mechanisms. This means healthcare facilities get access to financing (previously unattainable for many) and/or better credit terms. Healthcare facilities are able to save costs as a result of direct procurement, better financing, and lower prices, providing the opportunity to increase profitability. Patients benefit from greater affordability as services are offered closer to their home.
+Quality: In addition to offering high-quality medical products, we support healthcare facilities to better manage patients &amp; clinic operations through our procurement platform and our HDSM. Healthcare facilities receive access to health demand data, enabling them to make more informed procurement decisions. Our Equipment Lifecycle Management approach, offers maintenance, training, and support, and thus ensures the longevity and optimal performance of medical equipment. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Over the last two years, Viebeg has significantly expanded its reach and impact within the healthcare sector. To date, we have served more than 1000 unique healthcare providers, including hospitals, clinics, health posts, health centers, dispensaries, and pharmacies in Rwanda, DRC and Kenya. We have sold 400,000+ medical products with an estimated reach to 2 million people. 
+Our commitment to improving healthcare accessibility is reflected in the diverse range of institutions we collaborate with. When defining and counting end-users, we focus on healthcare providers who directly interact with our products. This includes medical professionals, administrators, and staff members at hospitals, clinics, health posts, health centers, dispensaries, and pharmacies. We consider each of these entities as a unique end-user, recognizing the pivotal role they play in delivering quality healthcare to communities. In addition, we estimate the number of patients that are diagnosed/treated with our equipment. We do this based on data derived from our CRM and regular customer surveys as well as public health data obtained from the Ministry of Health. 
+The first version of our Health Demand Simulation Model (HDSM) covers 3500+ health facilities in Rwanda, incorporates 90,000+ types of medical equipment and 225 diseases, aiding targeted infrastructure improvements and informed lending decisions through predictive analytics. The HDSM demonstrates the social and economic impact that a healthcare infrastructure investment can have on a certain community or in a certain region. </t>
+  </si>
+  <si>
+    <t>Kigali, Rwanda</t>
+  </si>
+  <si>
+    <t>Rwanda, Kenya, DRC</t>
+  </si>
+  <si>
+    <t>1000+ healthcare providers served</t>
+  </si>
+  <si>
+    <t>Rwanda, DRC, Kenya</t>
+  </si>
+  <si>
+    <t>3000+</t>
+  </si>
+  <si>
+    <t>$3M+</t>
+  </si>
+  <si>
+    <t>Rwanda HIMS</t>
+  </si>
+  <si>
+    <t>We do not collect any PHI</t>
+  </si>
+  <si>
+    <t>We have a team of support staff that is always available</t>
+  </si>
+  <si>
+    <t>Inventory Management</t>
+  </si>
+  <si>
+    <t>www.viebeg.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Courtney Moxley </t>
+  </si>
+  <si>
+    <t>courtney@reachdigitalhealth.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reach Digital Health </t>
+  </si>
+  <si>
+    <t>Young Africa Live</t>
+  </si>
+  <si>
+    <t>Young Africa Live (YAL) is a digital health platform designed to empower young people in Africa with comprehensive sexual and reproductive health (SRH) information. YAL combines the privacy of a WhatsApp chatbot with the community engagement of Facebook, delivering personalized content to users aged 15-24. By addressing the unique needs and challenges faced by young people in accessing SRH information and services, YAL aims to improve their overall well-being and health outcomes.
+The program utilizes a human-centered design approach, ensuring that the content and delivery are tailored to the specific cultural and social contexts of the users. YAL not only provides information but also fosters a safe and inclusive space for young people to discuss sensitive health topics, ask questions, and receive support. Through personalized interventions, smart user profiling, and advanced data analytics, YAL continuously adapts to user needs and preferences, promoting long-lasting behavior change and improved SRH outcomes.</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1IbdpPtvO_AH9NLQN367rgDZ4oZqXtDy3</t>
+  </si>
+  <si>
+    <t>info@reachdigitalhealth.org</t>
+  </si>
+  <si>
+    <t>National and Community Health, Analytics and Data Aggregation, AI for Health</t>
+  </si>
+  <si>
+    <t>Young Africa Live (YAL) utilizes a multi-pronged approach to improve health outcomes among youth. By disseminating accurate SRH information and fostering open dialogue, YAL aims to increase health literacy and empower young people to make informed decisions about their health and well-being, ultimately leading to positive behavior change and a reduction in negative health outcomes.By offering personalized interventions, YAL addresses key behavioral barriers, helping individuals make informed health decisions, which leads to improved health literacy and positive behavioral shifts. These interventions are designed to reduce harmful health outcomes such as unintended pregnancies and sexually transmitted infections.
+Additionally, YAL raises awareness and creates demand for essential health services, such as family planning, HIV prevention, and mental health support, ensuring that young people have access to the care they need. The platform’s screening algorithms guide users to appropriate healthcare services, bridging the gap between awareness and action. By empowering youth to take ownership of their health decisions and providing the necessary support and guidance, YAL fosters long-term engagement with healthier practices. This comprehensive and youth-centered approach ultimately strengthens health systems, improves health outcomes, and supports the overall well-being of young people across Africa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YAL addresses the unmet SRH needs of young people in South Africa, who often face significant barriers in accessing SRH information and services due to stigma, lack of youth-friendly services, and socio-cultural norms. YAL's digital platform overcomes these barriers by providing a safe and accessible space for young people to engage with SRH content, ask questions, and receive personalized support.
+YAL effectively leverages low-cost mobile technology, such as WhatsApp, to meet users where they are. By utilizing platforms like WhatsApp, which are already widely used and familiar to young people, YAL eliminates barriers to access and ensures that critical SRH information and services are readily available. 
+YAL's data-driven approach provides valuable insights into youth SRH needs and preferences at the national level, which contributes to health system strengthening. YAL has promising potential in improving SRH and mental health outcomes for young people in South Africa. By empowering young people with knowledge and agency, YAL has demonstrated: 
+- Improved SRH Knowledge: Statistically significant improvements were observed in SRH knowledge, particularly among highly engaged users.
+- Positive Changes in Attitudes: YAL contributed to reductions in poor body image and consent attitudes, promoting healthier perspectives.
+- Increased Condom Use: For users not planning to have children in the near future, condom usage increased, suggesting positive behavioral change.
+- Enhanced Mental Health: The platform fostered a sense of social connectedness and provided a safe space for discussing mental health issues, although further investigation is needed regarding the impact on depression and anxiety scores.
+- Greater Likelihood of Service Utilization: YAL users expressed increased intentions to visit healthcare facilities and seek counseling, suggesting potential for greater service uptake. </t>
+  </si>
+  <si>
+    <t>1 in South Africa</t>
+  </si>
+  <si>
+    <t>112,565 all time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">177,753 outbound messages per month on average (48 months) </t>
+  </si>
+  <si>
+    <t>$8 million</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1W3qqP01XtiLT4NwyJR4Wuc3SrucJ5tkxJ40GO-m4rO8/edit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reach ensures the privacy and protection of Personal Health Information (PHI) in solutions like YAL to provide a safe and secure environment for young people while safeguarding their privacy. Our approach includes:
+- End-to-end encryption: YAL leverages platforms like WhatsApp, which offer end-to-end encryption, ensuring that all user interactions and data remain private and secure.
+- Anonymity and data security: YAL collects and stores data anonymously and securely, adhering to strict data protection protocols and international standards.
+- User consent and control: YAL prioritizes user consent and control over their data, allowing them to choose what information they share and how it is used.
+- Ethical guidelines and compliance: YAL operates in accordance with ethical guidelines and complies with all relevant data privacy regulations, including the Protection of Personal Information Act (POPIA) in South Africa.
+- Transparency and accountability: YAL maintains transparency about its data practices and is accountable for the responsible and ethical use of user data.
+</t>
+  </si>
+  <si>
+    <t>Audit Logs: All logs are sent to AWS Cloudtrail to ensure a record of actions taken by a user, role, or an AWS service is captured. This information can be used to determine the request that was made, the IP address from which the request was made, who made the request, when it was made, and additional details. Administrator access to critical system hardware and servers is logged
+Monitoring: A set of rules and services have been implemented to monitor for changes to services, alert administrators of any potential risks, and diagnose overly permissive security group rules.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Network segmentation: A set of rules/configurations are in place to prevent databases from being accessible from the internet, to help mitigate the possibility of a data breach.
+Public Accessibility: Disabled to ensure databases are not assigned a publicly exposed DNS hostname.
+Network Demilitarized Zone (“DMZ”) architecture is in place to restrict access to protected data from the internet. Protected data is stored in a data tier and that is not allowed access to the public internet or be publicly accessible directly. There are no direct network routes to and from the data tier, making data exfiltration more difficult from any other services that are compromised.
+Network Access Control List (“NACL”) have been implemented to restrict access between subnets and and deny unnecessary network traffic to the data tier subnets. All outbound traffic from the data tier is denied from routing. Only database servers reside within the data tier, so network communication cannot originate from the data tier.
+Security Groups and Firewall: A set of stateful software firewalls (known as security groups) are in place to configure connections between any DMZ and the internal network zone, and to ensure network communication is restricted to a specified set of ports.
+Encryption: All databases are encrypted at rest. All database backup and snapshots are also encrypted.
+User Account Review: Data Owners perform regular user reviews to determine if there are any unused/underutilized or forgotten user accounts in the system that should be removed, ensuring that only active and authorised users retain access to the system.
+Granular User Permissions: Data Owners perform regular user permission reviews to determine if there are any user accounts that have excessive permissions that do not follow the principle of least privilege.
+User action auditing and review: Data Owners perform regular user actions reviews (sample review, or spot checks) to determine if there are any users that have performed any unauthorised or unscheduled data exports.
+Server hardening: The following measures have been implemented: Configure SSL/TLS with a valid, trusted certificate; Disable older versions of TLS; Configure SSL encryption for internal traffic; Enable firewall protection; Disable unused service; Session lifetime configuration Verified; Enabled HTTP Strict Transport Security for web browser clients; Disable Guest access.
+</t>
+  </si>
+  <si>
+    <t>No current active development</t>
+  </si>
+  <si>
+    <t>Individual Registration</t>
+  </si>
+  <si>
+    <t>Addressing National Health Priorities: YAL aligns with national health strategies in South Africa and Nigeria by focusing SRH, mental health, and HIV prevention, which are key priorities for both countries. Generating Demand for SRH Services: YAL increases awareness and demand for SRH services by providing young people with information and resources, and linking them to appropriate healthcare providers, contributing to improved community health outcomes. Promoting Community Dialogue: YAL fosters open dialogue and engagement within communities by creating a safe space for young people to discuss SRH topics, challenge stigma, and share information, ultimately contributing to a more supportive and informed community environment. Supporting Community-Based Organizations: YAL partners with community-based organizations (CBOs) to leverage their expertise, networks, and resources to reach and engage young people effectively within their communities.</t>
+  </si>
+  <si>
+    <t>Data visualization, Dashboards, Data processing (extract, transform, load - ETL)</t>
+  </si>
+  <si>
+    <t>Guided self help, Interactive services/chatbots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Linkage to SRH services on the ground
+- Safe Online Community: YAL provides a safe and moderated forum on Facebook for users to discuss SRH topics openly with their peers.
+- Browsable Content Library of SRH content that users can search for specific topics of interest.
+- Personalized Push Messages: YAL sends personalized push messages to users to encourage healthy behaviors and promote engagement with the platform.
+</t>
+  </si>
+  <si>
+    <t>https://www.youngafricalive.org/</t>
+  </si>
+  <si>
+    <t>Courtney Moxley</t>
+  </si>
+  <si>
+    <t>Reach Digital Health</t>
+  </si>
+  <si>
+    <t>MomConnect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reach's MNCH (Maternal, Newborn, and Child Health) offering, is a digital health platform designed to support and empower pregnant women and mothers in their journey through pregnancy and early childhood (until the child’s second birthday). By leveraging mobile technology, the service delivers stage-based health information, appointment reminders, and personalized support to women, aiming to improve maternal and child health outcomes. The service offers a variety of features, including push messages, browsable content, and access to a helpdesk for questions or concerns. It also incorporates risk assessment and personalized interventions, addressing barriers such as pregnancy literacy, self-healthcare practices, mental health, connectedness, and resilience. Through its comprehensive approach, Reach’s MNCH offering strives to enhance the health and well-being of mothers and their children, while promoting informed decision-making and active engagement in their healthcare. 
+MomConnect is Reach’s first implementation of the MNCH offering in South Africa, launched in August 2014 as a partnership between the South African National Department of Health (NDOH) and various stakeholders. The official endorsement and adoption by the NDOH solidified MomConnect's position as a flagship program in maternal and child health. This collaboration ensured the alignment of MomConnect with national health priorities and facilitated its widespread implementation across the country. Since its launch, MomConnect has evolved and expanded its services, reaching millions of mothers and making a significant impact on maternal and child health outcomes in South Africa. </t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=131EQIoCJS_-3n9GtkpyXTew5ZqxaRWxa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info@reachdigitalhealth.org </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reach’s MNCH offering has been instrumental in improving health outcomes in Africa by tackling several challenges. By delivering vital health information directly to mothers' phones, it addresses the lack of information and access, empowering women with knowledge and enabling informed decision-making. Additionally, MomConnect's stage-based health messages and automated responses alleviate the burden on healthcare workers, allowing them to focus on critical cases. Moreover, the platform promotes healthy behaviors and encourages timely healthcare utilization through features like appointment reminders and symptom checkers. By addressing these challenges and promoting preventive care, MomConnect contributes to reducing maternal and infant mortality rates, ultimately enhancing the health and well-being of mothers and children across Africa. </t>
+  </si>
+  <si>
+    <t>Reach’s MNCH offering tackles the challenges of limited access to maternal and child health information, overburdened health systems, and poor health-seeking behaviors in the African health ecosystem. With high maternal and infant mortality rates, the continent urgently requires scalable and effective solutions. MomConnect's impact has been significant, reaching millions of users with vital health information, improving antenatal care attendance, promoting healthy practices, and empowering women to make informed decisions about their health and their children's well-being. By leveraging mobile technology and evidence-based content, MomConnect has proven to be a valuable tool in strengthening health systems and improving maternal and child health outcomes in Africa. 
+Specifically, MomConnect has demonstrated positive impacts on several MNCH behaviors, including:
+- Increased uptake of family planning: MomConnect users, especially non-first-time moms, showed a greater likelihood of using family planning.
+- Improved breastfeeding practices: First-time moms and younger moms were more likely to breastfeed with MomConnect's support.
+- Improved ANC and PNC attendance: Evidence suggests that MomConnect users are more likely to attend ANC and PNC visits, leading to better maternal and child health outcomes.</t>
+  </si>
+  <si>
+    <t>4,820,950 all time users</t>
+  </si>
+  <si>
+    <t>403,277 outbound messages per month on average (108 months)</t>
+  </si>
+  <si>
+    <t>MomConnect has been designed to be compliant with South Africa’s Health Normative Standards Framework and leverages an HIE architecture and Interoperability Layer. The Patient Identifier Cross-Reference/Patient Demographic Query standards profile of Integrating the Healthcare Enterprise was initially considered for demographic data and the Mobile Health Document profile for clinic data, with a Clinical Document Architecture (Health Level Seven (HL7)) document for clinical data. However, a custom Javascript Object Notation (JSON) message was developed as there was no existing messaging profile catering for client enrolment and notification as well as HL7 Fast Health Interoperability Resourcesiv (FHIR) messages for specific clinical messaging, such as referral requests and clinical encounters (See MomConnect: an exemplar implementation of the Health Normative Standards Framework in South Africa - https://www.hst.org.za/publications/South%20African%20Health%20Reviews/11%20MomConnect%20An%20exemplar%20implementation%20of%20the%20Health%20Normative%20Standards%20Framework%20in%20SA.pdf  and Designing for scale: optimising the health information system architecture for mobile maternal health messaging in South Africa (MomConnect) - https://gh.bmj.com/content/3/Suppl_2/e000563)</t>
+  </si>
+  <si>
+    <t>MomConnect has been designed to integrate with DHIS2, South Africa’s national data reporting warehouse (See MomConnect: an exemplar implementation of the Health Normative Standards Framework in South Africa - https://www.hst.org.za/publications/South%20African%20Health%20Reviews/11%20MomConnect%20An%20exemplar%20implementation%20of%20the%20Health%20Normative%20Standards%20Framework%20in%20SA.pdf and Designing for scale: optimising the health information system architecture for mobile maternal health messaging in South Africa (MomConnect) - https://gh.bmj.com/content/3/Suppl_2/e000563 )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/document/d/1a4LK24xHWqjiD3OxtrMuhunUlfjAVpskIw61j-POCII/edit?usp=drive_link </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MomConnect ensures the privacy and protection of PHI through:
+- Compliance with Regulations: MomConnect adheres to South Africa's Protection of Personal Information Act (POPIA) and other relevant data privacy laws and regulations.
+- Informed Consent: MomConnect obtains informed consent from users before collecting, processing, or sharing their PHI. Users are informed about the purpose of data collection, how their data will be used, and who will have access to it.
+- Data Minimization: MomConnect collects only the minimum necessary PHI required to provide the service and achieve its public health objectives.
+- Secure Data Storage and Transmission: MomConnect employs robust security measures to protect PHI from unauthorized access, use, or disclosure.
+- Data Retention and Deletion: MomConnect has clear policies for data retention and deletion, ensuring that PHI is not kept longer than necessary and is securely deleted or anonymized when no longer needed.
+- User Control: MomConnect provides users with control over their PHI, allowing them to access, update, correct, and delete their information as needed.
+- Transparency: MomConnect maintains transparency about its data practices, providing users with clear and accessible information about how their PHI is handled.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Audit Logs: All logs are sent to AWS Cloudtrail to ensure a record of actions taken by a user, role, or an AWS service is captured. This information can be used to determine the request that was made, the IP address from which the request was made, who made the request, when it was made, and additional details. Administrator access to critical system hardware and servers is logged.
+Monitoring: A set of rules and services have been implemented to monitor for changes to services, alert administrators of any potential risks, and diagnose overly permissive security group rules.
+</t>
+  </si>
+  <si>
+    <t>Electronic pregnancy registration: MomConnect allows for early and comprehensive registration of pregnancies within the public health system, aiding in better tracking and management of maternal health at a national level. Targeted health promotion messages: MomConnect sends stage-based health messages to pregnant women and new mothers, promoting healthy behaviors and timely healthcare utilization, contributing to improved MNCH outcomes at both community and national levels. Interactive feedback mechanism: MomConnect provides a platform for women to provide feedback on the quality of care received at public health facilities, enabling the Department of Health to monitor and improve service delivery, impacting community health directly. Helpdesk and Chatbot Support: MomConnect offers a helpdesk for users to ask questions or report concerns, providing personalized support and guidance, contributing to positive health outcomes in the community.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Browsable Content Library of MNCH content that users can search for specific topics of interest.
+Personalized Push Messages: MomConnect sends personalized push messages to users to encourage healthy behaviors and promote engagement with the platform.
+</t>
+  </si>
+  <si>
+    <t>https://www.health.gov.za/momconnect/</t>
+  </si>
+  <si>
+    <t>Neal Bazirake</t>
+  </si>
+  <si>
+    <t>info@marascientific.org</t>
+  </si>
+  <si>
+    <t>Mara scientific</t>
+  </si>
+  <si>
+    <t>Mpeke HMIS</t>
+  </si>
+  <si>
+    <t>Mpeke HMIS is an advanced hospital enterprise resource planning tool designed to optimize healthcare operations and enhance patient outcomes by addressing critical inefficiencies such as manual processes and lack of real-time visibility. This comprehensive system includes specialized modules for patient and doctor management, laboratory services, pharmacy, billing, inventory ,surgery ,antenatal and even X-ray and scan capabilities. It also offers robust features like asset tracking, accounting , and extractable data analysis. Mpeke HMIS improves decision-making and care coordination by providing intuitive workflows and comprehensive analytics, making it an essential solution for healthcare organizations.</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1yfS0MlnG53Srq5NmJFhvZN0aDHw5lPnu</t>
+  </si>
+  <si>
+    <t>Electronic Health Record, Pharmacy, Laboratory and Diagnostics, Analytics and Data Aggregation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mpeke HMIS is designed to tackle the unique challenges faced by African healthcare systems, where limited resources, infrastructure, and accessibility often hinder the delivery of effective care. By transitioning from manual, paper-based processes to a fully digitized platform, Mpeke HMIS reduces errors, minimizes delays, and eases administrative workloads. This enables healthcare providers to focus more on patient care, improving efficiency and outcomes in resource-constrained environments.
+The system's ability to generate real-time data insights empowers hospitals to make informed decisions that directly affect patient outcomes. In regions with limited health resources, Mpeke HMIS enhances the visibility of hospital operations, optimizing the use of essential medications and improving care coordination. Additionally, the platform streamlines patient care management by tracking medical histories, diagnoses, and treatments, improving overall care continuity, especially in settings where patients frequently visit multiple providers.
+Mpeke HMIS is also tailored to local health use cases, such as maternal health management, aligning with the pressing needs of African healthcare systems. Its ability to generate detailed reports supports healthcare organizations in identifying areas for improvement, adapting to changing healthcare landscapes, and ultimately reducing mortality rates. By providing critical tools and insights, Mpeke HMIS enables healthcare providers to deliver better-quality care, driving improvements in health outcomes across Africa.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Market Need:The African healthcare system faces numerous challenges, including inadequate infrastructure, under-resourced hospitals, and reliance on manual processes that hinder the delivery of efficient care. Many facilities still operate with paper-based record keeping, leading to delays, errors, and inefficiencies in managing patient data, medications, and resources. There is also a significant gap in real-time data access, making it difficult for healthcare providers to make informed decisions or respond quickly to patient needs. Additionally, limited coordination between healthcare providers often leads to fragmented care, especially in rural areas. Furthermore, hospitals often struggle to generate accurate reports or use data for decision-making, limiting their ability to identify areas for improvement and respond to public health needs. Mpeke HMIS addresses these challenges by providing a digital platform that automates hospital operations, streamlines patient care management, and enhances coordination across the healthcare ecosystem.
+Impact in the African Health Ecosystem: Mpeke HMIS has significantly impacted the African healthcare landscape by enhancing the quality and efficiency of healthcare delivery. The hospital using the system has reported reductions in medical errors, faster access to large  patient data of about 13759 patients and improved operational efficiency. By eliminating manual processes, healthcare providers focus more on patient care and less on administrative tasks. Mpeke HMIS also promotes better coordination between healthcare providers, which is crucial in regions where patients often seek treatment from multiple facilities, ensuring continuity of care and reducing duplication of tests and treatments.
+Additionally, the system's ability to generate comprehensive reports and analytics has empowered healthcare organizations to make data-driven decisions, improving their response to public health issues such as maternal health and infectious diseases. This has led to better health outcomes, including reduced mortality rates and improved disease management. As a scalable and adaptable solution, Mpeke HMIS continues to meet the evolving needs of healthcare organizations across Africa, ultimately driving improvements in the quality of care and contributing to the modernization of the continent's healthcare infrastructure.
+</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>South Sudan</t>
+  </si>
+  <si>
+    <t>Mature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The link cant be provided because it is private </t>
+  </si>
+  <si>
+    <t>Mpeke HMIS ensures the privacy and protection of Personal Health Information (PHI) through a comprehensive approach that includes multiple layers of security, strict access controls, and adherence to regulatory standards.
+First, the system employs encryption to protect PHI both at rest and in transit. This means that sensitive data is encoded when stored in databases and when transmitted over networks, making it unreadable to unauthorized users. Additionally, Mpeke HMIS utilizes secure communication protocols, such as HTTPS, to safeguard data exchanges between users and the system, further mitigating the risk of interception.
+To enforce access controls, the system uses Role-Based Access Control (RBAC), which ensures that only authorized personnel can access PHI based on their roles and responsibilities. Each user’s permissions are carefully defined, limiting access to sensitive information to those who require it for their job functions. Furthermore, the solution includes audit logging features that track and record all access to PHI, enabling the identification of any unauthorized access attempts and promoting accountability.</t>
+  </si>
+  <si>
+    <t>Mpeke HMIS employs robust mechanisms for authentication and authorization to ensure secure access to the system and protect sensitive patient data. The authentication process requires users to create strong passwords that meet specific complexity requirements, which are stored using encryption techniques to safeguard them against unauthorized access. Secure communication protocols, such as HTTPS, are utilized during the login process to encrypt data transmitted between the user's device and the server. For authorization, the system implements Role-Based Access Control (RBAC), granting access based on assigned roles, which define permissions for actions and data access. Additionally, Mpeke HMIS includes session management features that monitor user activity and automatically log users out after periods of inactivity, further preventing unauthorized access. Together, these mechanisms establish a secure environment within Mpeke HMIS, ensuring that only verified users can access the system and that they have appropriate permissions based on their roles, thereby protecting patient data and maintaining compliance with healthcare regulations.</t>
+  </si>
+  <si>
+    <t>Mpeke HMIS incorporates robust mechanisms for audit logging and error reporting to enhance accountability, security, and system performance. The system features an inbuilt logging functionality that captures detailed records of all user transactions within the platform. This includes information on what actions were performed, when they occurred, and any changes made to patient records or administrative settings. Each log entry is timestamped and associated with the user’s identity, allowing for precise tracking of actions taken within the system. Mpeke HMIS provides an intuitive feature that records error logs and access logs automatically and sends them for review by the technical support team. This process ensures that issues are addressed promptly, minimizing disruptions in healthcare delivery.  These mechanisms ensure that Mpeke HMIS maintains high standards of security and operational integrity, critical in a healthcare environment.</t>
+  </si>
+  <si>
+    <t>Patient Record Management, Individual Registration, Clinical decision support, CPOE/Order Management, Patient Billing, Patient Data Import/Export, X-Ray and Imaging, ER - Triage and Dashboard, Surgical Management</t>
+  </si>
+  <si>
+    <t>Capture biological specimens, Transmit and track diagnostic orders, Send diagnostic results to providers, Capture results from digital devices, Inventory Management</t>
+  </si>
+  <si>
+    <t>everything that the system offers has been listed</t>
+  </si>
+  <si>
+    <t>https://marascientific.org</t>
+  </si>
+  <si>
+    <t>Jean Damascene Bigirimana</t>
+  </si>
+  <si>
+    <t>jdamascene@gmail.com</t>
+  </si>
+  <si>
+    <t>HealthEdu Ltd</t>
+  </si>
+  <si>
+    <t>HealthEdu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HealthEdu provides customized, accredited courses for healthcare professionals, available online and in-person. We offer 250+ tailored courses led by experts across Africa and empower health professionals and community healthcare workers. </t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1Iv3p8gLu_E7QF-ockCvknEwJpWWRgmbg</t>
+  </si>
+  <si>
+    <t>healthedultd@gmail.com</t>
+  </si>
+  <si>
+    <t>Pharmacy, Laboratory and Diagnostics, Front-line (CHW) tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our solution is to empower health professionals with real time information and courses that help empower them together with community health workers with vital information that help save lives and improve health as per Universal Health Coverage and SDGs 3. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In East Africa alone, more than 300,000 health professionals struggle to access evidence-based information that help them improve their knowledge base and disseminate it to their patients for general improved health, in Africa the need is beyond that. </t>
+  </si>
+  <si>
+    <t>Kigali Rwanda</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>90% is in Africa</t>
+  </si>
+  <si>
+    <t>100% was done in Africa</t>
+  </si>
+  <si>
+    <t>https://www.rahpc.org.rw/cpds</t>
+  </si>
+  <si>
+    <t>https://www.healthedu.rw/terms_condition</t>
+  </si>
+  <si>
+    <t>We abide to the Law for data protection in Rwanda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have developers that does this technically. </t>
+  </si>
+  <si>
+    <t>Clinical decision support, Virtual care</t>
+  </si>
+  <si>
+    <t>Decision Support</t>
+  </si>
+  <si>
+    <t>Provide necessary information for the healthcare professionals and layman on the diseases for prevention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are thinking of integrating AI for more knowledge sharing and customization. </t>
+  </si>
+  <si>
+    <t>Support dissemination of conditions that people can request for virtual care for</t>
+  </si>
+  <si>
+    <t>Inform the public on the information sharing tips for vaccination an warn the public about dangers and this can more supporting the prevention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have been able to support 7,000 Health care professionals and we are developing contents for community health workers; we have trained 20 public hospitals on digital literacy, and we have network of 65 clinical experts across the world. </t>
+  </si>
+  <si>
+    <t>www.healthedu.rw</t>
+  </si>
+  <si>
+    <t>Katrina A Prentice</t>
+  </si>
+  <si>
+    <t>katrina@zakhealth.com</t>
+  </si>
+  <si>
+    <t>Zak Health Ltd</t>
+  </si>
+  <si>
+    <t>Zak Health</t>
+  </si>
+  <si>
+    <t>Zak Health's AI Telemedicine solution provides advanced health assessments using 8 key biomarkers. Tailored for Africa, this comprehensive platform integrates virtual consultations with AI-driven insights, improving access to healthcare, diagnostics, and treatment, even in remote areas. The solution empowers patients and healthcare providers with real-time health data, ensuring proactive management of individual health outcomes.</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1q0iR77X_Bn7EX8UBwS0ufwsMvlYfzFCL</t>
+  </si>
+  <si>
+    <t>Electronic Health Record, Pharmacy, Analytics and Data Aggregation, AI for Health, Virtual Health</t>
+  </si>
+  <si>
+    <t>How Zak Health’s AI Telemedicine Solution Improves Health Outcomes in Africa
+Zak Health's AI Telemedicine solution is specifically designed to address the unique healthcare challenges in Africa by leveraging digital innovation to improve health outcomes. The platform integrates advanced AI health assessments using 8 key biomarkers, tailored to the needs of African healthcare systems. Key benefits include:
+Increased Accessibility to Healthcare: Africa faces a significant shortage of healthcare providers, particularly in rural areas. Our solution bridges this gap by offering remote consultations and AI-driven diagnostics, enabling patients in remote locations to receive timely medical care without the need for physical travel.
+Personalized Health Assessments: Using 8 biomarkers, our AI Health Assessments provide personalized health insights, helping identify early signs of chronic diseases such as diabetes, hypertension, and cardiovascular conditions. This enables earlier interventions, reducing the severity of conditions and improving long-term health outcomes.
+Cost-Effective Healthcare: By reducing the need for in-person visits and streamlining diagnostics, our platform lowers healthcare costs for both patients and providers. This affordability makes healthcare more accessible to underserved populations, contributing to improved health outcomes.
+Data-Driven Decision Making: The platform collects and analyzes health data in real time, allowing healthcare providers and governments to monitor health trends, allocate resources more efficiently, and develop targeted public health strategies.
+Scalability and Adaptability: Our solution is designed to scale across different regions in Africa, adapting to the specific needs of local healthcare systems. This flexibility allows for the delivery of relevant, culturally-sensitive healthcare services that address the diverse health challenges across the continent.
+By integrating AI health assessments with telemedicine, Zak Health’s solution enhances patient outcomes, improves resource efficiency, and delivers high-quality healthcare to areas that need it most.</t>
+  </si>
+  <si>
+    <t>Market Need for Zak Health’s AI Telemedicine Solution in Africa
+Africa faces several significant healthcare challenges, including inadequate healthcare infrastructure, a shortage of healthcare professionals, and limited access to healthcare services, particularly in rural and remote regions. The continent’s growing population, increasing burden of chronic diseases, and economic disparities further exacerbate these issues. There is a pressing need for innovative solutions that can provide accessible, cost-effective, and quality healthcare to millions of underserved people.
+Zak Health’s AI Telemedicine Solution: Addressing Market Needs
+Zak Health’s AI Telemedicine platform directly addresses these challenges by providing remote, AI-powered health assessments and consultations that are scalable and adaptable to the unique needs of the African continent. This solution fills critical gaps in the healthcare system by:
+Enhancing Access to Care: With healthcare facilities often concentrated in urban areas, many Africans in rural regions lack access to essential medical services. Zak Health’s telemedicine platform offers a solution by enabling virtual consultations and AI-driven health assessments, eliminating geographic barriers to care.
+Improving Early Detection and Prevention: The AI health assessments analyze 8 key biomarkers, facilitating early detection of conditions such as hypertension, diabetes, and cardiovascular disease. This enables timely interventions and helps shift the focus from reactive to preventive care, ultimately reducing the burden on overstretched healthcare systems.
+Providing Affordable Healthcare: In many African countries, healthcare costs can be prohibitive for low-income populations. By reducing the need for in-person visits, the solution lowers healthcare costs, making quality care more affordable and accessible to underserved communities.
+Impact on the African Health Ecosystem
+Zak Health’s solution has already begun making a tangible impact on the African health ecosystem by:
+Expanding Access to Healthcare Services: The platform has facilitated thousands of virtual consultations, particularly in regions where healthcare infrastructure is limited. By providing consistent and reliable access to healthcare, Zak Health has improved health outcomes in areas that previously had limited medical support.
+Empowering Patients and Providers with Data: Through AI-driven health assessments, both patients and healthcare providers have access to actionable health insights that guide treatment decisions and enhance preventive care strategies. This data-driven approach is helping reduce the prevalence of chronic diseases and improve patient outcomes.
+Building Health Equity: By leveraging digital tools, Zak Health is helping to close the healthcare gap between urban and rural populations. The solution promotes health equity by providing equal access to quality care, irrespective of location or socioeconomic status.
+Supporting Public Health Efforts: The platform’s ability to aggregate health data allows governments and public health organizations to identify emerging health trends and target interventions more effectively, contributing to stronger public health systems and more efficient resource allocation.
+Conclusion
+Zak Health’s AI Telemedicine solution is revolutionizing healthcare delivery in Africa by addressing critical market needs, improving access to care, and making a measurable impact on the health ecosystem. Through scalable, data-driven, and cost-effective innovations, Zak Health is contributing to the transformation of healthcare in Africa and advancing the goal of health equity across the continent.</t>
+  </si>
+  <si>
+    <t>London and Lagos</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Zero at present but that is not my intension</t>
+  </si>
+  <si>
+    <t>100% in India</t>
+  </si>
+  <si>
+    <t>None yet - just about to sign a government and an oil company</t>
+  </si>
+  <si>
+    <t>Nigeria and soon to be Kenya</t>
+  </si>
+  <si>
+    <t>zero</t>
+  </si>
+  <si>
+    <t>CE Medical Device, ISO 27001, GDPR</t>
+  </si>
+  <si>
+    <t>To follow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensuring Privacy and Protection of Personal Health Information (PHI)
+Zak Health takes the privacy and protection of Personal Health Information (PHI) seriously and has implemented robust measures to ensure that all patient data is handled securely and in compliance with international standards, such as HIPAA and GDPR. Our AI Telemedicine platform employs a multi-layered approach to safeguarding PHI, ensuring that data is kept confidential, secure, and protected from unauthorized access.
+Key Security Measures:
+Data Encryption:
+At Rest: All PHI stored in our system is encrypted using advanced encryption standards (AES-256) to prevent unauthorized access to data.
+In Transit: We use Transport Layer Security (TLS) to ensure that all data transmitted between patients, healthcare providers, and our servers is encrypted and secure from interception.
+Access Control:
+Role-Based Access: Access to PHI is restricted to authorized personnel based on their role within the healthcare ecosystem. This ensures that only healthcare providers and individuals directly involved in patient care can access sensitive information.
+Multi-Factor Authentication (MFA): Our platform implements multi-factor authentication for all users, adding an extra layer of security to prevent unauthorized access to accounts.
+Data Anonymization:
+Where appropriate, patient data is anonymized before it is used for analytics or research purposes. This ensures that individuals cannot be identified from aggregated health data.
+Audit Trails:
+Our system maintains comprehensive audit trails, tracking all access to PHI and any modifications made to patient records. This allows for real-time monitoring of data access and ensures transparency in how information is handled.
+Compliance with Regulatory Standards:
+HIPAA Compliance: Zak Health’s platform adheres to the Health Insurance Portability and Accountability Act (HIPAA), ensuring the confidentiality, integrity, and availability of patient health information for patients and healthcare providers.
+GDPR Compliance: For regions requiring GDPR compliance, Zak Health ensures that patients have control over their data, including rights to access, correct, or delete their information, as well as the right to data portability.
+Regular Security Audits and Penetration Testing:
+Our platform undergoes regular security audits and penetration testing by third-party cybersecurity experts to identify and resolve any vulnerabilities. This proactive approach ensures that our systems remain secure against evolving threats.
+Data Retention and Deletion Policies:
+We have strict data retention policies that ensure PHI is stored only for the necessary duration required for patient care or legal obligations. Upon request or when no longer required, PHI is securely deleted from our systems.
+Conclusion
+Zak Health is committed to the highest standards of privacy and data protection. Through encryption, access controls, compliance with regulatory frameworks, and continuous security monitoring, we ensure that Personal Health Information (PHI) remains secure and protected at all times. Our dedication to maintaining these rigorous standards ensures trust and confidence in our AI telemedicine platform from both healthcare providers and patients.
+</t>
+  </si>
+  <si>
+    <t>Audit Logging and Error Reporting Mechanisms in Zak Health’s AI Telemedicine Solution
+Zak Health employs robust audit logging and error reporting mechanisms to ensure transparency, security, and system reliability across the platform. These mechanisms play a critical role in tracking user activities, monitoring system performance, and identifying issues in real-time, ensuring that the platform operates efficiently and securely.
+Audit Logging Mechanisms
+Comprehensive Activity Tracking:
+Our platform maintains detailed audit logs of all user actions, including access to patient data, modifications made to health records, and system interactions (e.g., logins, logouts, and data transfers).
+Each log entry contains essential information such as user identity, timestamp, type of action performed, and the data or resource affected.
+Role-Based Audit Trails:
+Audit logs are role-based, meaning actions performed by different types of users (e.g., administrators, healthcare providers, or patients) are recorded and tracked based on their access privileges. This ensures that only authorized personnel are interacting with sensitive information.
+Tamper-Proof Logs:
+To ensure the integrity of the logs, all audit entries are stored in tamper-proof storage, where they cannot be modified or deleted by unauthorized users. This protects the integrity of the data for regulatory and security purposes.
+Real-Time Monitoring:
+The platform supports real-time monitoring of audit logs, allowing administrators to quickly detect and respond to unauthorized access attempts, suspicious activities, or policy violations.
+Compliance Reporting:
+The audit logs are designed to meet compliance requirements for HIPAA, GDPR, and other relevant data protection regulations. This ensures that we can provide accurate records of system activity during security audits and investigations.
+Error Reporting Mechanisms
+Automated Error Detection:
+The platform continuously monitors system performance through automated tools that detect and capture errors as they occur. These tools are integrated into the application and infrastructure, tracking issues such as system failures, latency spikes, and service disruptions.
+Real-Time Error Logging:
+Errors are logged in real-time and stored in centralized logging systems, ensuring that details such as error type, timestamp, affected components, and contextual information are recorded for immediate or later analysis.
+Alerts and Notifications:
+When an error occurs, our error reporting system automatically generates alerts and sends notifications to the appropriate technical teams. These alerts are triggered based on predefined thresholds or critical failures and are delivered via email, messaging services, or dedicated monitoring dashboards.
+Detailed Error Reports:
+Each error report includes stack traces, contextual logs, and impact assessments to help the development and operations teams diagnose the issue quickly and efficiently. The reports provide actionable insights into the root cause of the problem.
+User-Friendly Error Handling:
+For the end-users, the platform provides user-friendly error messages that help them understand the issue without exposing technical details. At the same time, detailed error logs are kept on the backend for the technical teams to resolve the problem without disrupting the user experience.
+Continuous Monitoring &amp; Feedback Loop:
+The platform utilizes continuous monitoring systems such as Prometheus and ELK (Elasticsearch, Logstash, Kibana) to track system performance and error occurrences. This feedback loop allows us to proactively address issues and improve system stability over time.
+Conclusion
+Zak Health’s audit logging and error reporting mechanisms ensure comprehensive oversight of all user activities and system operations. With real-time tracking, tamper-proof logs, automated error detection, and proactive alerts, we ensure the highest standards of security, compliance, and system performance. These mechanisms are vital in maintaining trust, improving system reliability, and enabling quick response to any operational issues that arise.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authentication and Authorization Mechanisms in Zak Health’s AI Telemedicine Solution
+Zak Health’s AI Telemedicine platform prioritizes security and privacy, especially in handling sensitive healthcare data. To ensure that only authorized individuals can access the system and that data remains secure, we have implemented robust authentication and authorization mechanisms. These mechanisms are designed to safeguard patient information and ensure that healthcare providers and users can only access the data they are permitted to view or interact with.
+Authentication Mechanisms
+Multi-Factor Authentication (MFA):
+MFA is used to provide an additional layer of security beyond just usernames and passwords. Users must provide at least two forms of authentication (e.g., a password and a one-time code sent to their phone or email) before they can access the system.
+This significantly reduces the risk of unauthorized access, even if login credentials are compromised.
+OAuth/OpenID Connect:
+OAuth 2.0 and OpenID Connect are employed for secure authentication, enabling users to log in via trusted identity providers (e.g., Google, Microsoft). This eliminates the need for storing sensitive credentials on our platform and leverages secure, well-established external authentication services.
+OAuth ensures that third-party services can securely interact with the system without exposing user credentials.
+Biometric Authentication (Optional):
+For heightened security, we offer biometric authentication options for mobile app users. This can include fingerprint scanning or facial recognition, ensuring secure access to the platform without needing passwords.
+Biometrics offer an additional layer of protection and ease of use for healthcare providers and patients.
+Password Policies:
+Our platform enforces strong password policies, requiring users to create complex passwords that meet specific criteria (e.g., minimum length, inclusion of numbers and symbols). Users are prompted to regularly update their passwords to maintain security.
+Passwords are stored using salted and hashed encryption, ensuring that they cannot be deciphered even if the database is compromised.
+Session Management:
+The platform implements session expiration and automatic logout features after periods of inactivity. This prevents unauthorized access through forgotten active sessions and ensures that users must reauthenticate after a certain time.
+Secure tokens are used to manage sessions, ensuring that authentication data is encrypted during user interactions.
+Authorization Mechanisms
+Role-Based Access Control (RBAC):
+Role-Based Access Control ensures that users are granted access only to the information and features necessary for their roles. Different user types (e.g., doctors, patients, administrators) have distinct roles, each with specific access permissions.
+For instance, a doctor might have access to detailed patient records, whereas a patient can only access their personal health data. This prevents unauthorized viewing or editing of sensitive data.
+Attribute-Based Access Control (ABAC):
+ABAC provides more granular control, allowing access based on user attributes such as location, department, or specific security clearance. This dynamic authorization model ensures that users are only permitted access based on real-time conditions and specific data attributes.
+For example, only users with the attribute of "clinical staff" might be granted access to diagnostic tools, and only users within a specific region might access certain healthcare records.
+Fine-Grained Permissions:
+Permissions can be set at a highly detailed level, including restricting access to specific functions or datasets within the system. These permissions ensure that even within certain roles, access is granted on a need-to-know basis.
+For instance, administrative staff may be able to view patient demographics but may not have permission to access detailed medical histories or diagnostic reports.
+Audit-Based Authorization:
+Every access request is logged in an audit trail, allowing the system to review and verify authorized access in real-time. If unauthorized attempts are detected, the system can revoke access immediately or alert system administrators.
+Token-Based Authorization:
+The platform uses JSON Web Tokens (JWT) for secure authorization. After authentication, users receive encrypted tokens that allow them access to specific areas of the platform. These tokens are time-limited and contain encoded permissions that the system verifies before granting access to sensitive data.
+Tokens are automatically refreshed to avoid session hijacking and can be revoked if security risks are identified.
+Dynamic Policy Management:
+Authorization policies can be dynamically adjusted based on changes in the user environment, role changes, or evolving security requirements. This ensures that the platform can adapt to new threats or organizational changes quickly, without the need for extensive reconfiguration.
+Conclusion
+Zak Health’s platform ensures the highest standards of security through rigorous authentication and authorization mechanisms. Multi-factor authentication, biometric options, role-based access control, and token-based authorization are just some of the ways we safeguard access to sensitive health data. These mechanisms not only protect personal health information but also ensure that users have the correct access needed to perform their roles efficiently and securely.
+</t>
+  </si>
+  <si>
+    <t>Patient Record Management</t>
+  </si>
+  <si>
+    <t>AI Health Assessments</t>
+  </si>
+  <si>
+    <t>Data processing (extract, transform, load - ETL)</t>
+  </si>
+  <si>
+    <t>Guided self help, Telemedicine appointments, AI Health Assessments</t>
+  </si>
+  <si>
+    <t>Digital vaccine card</t>
+  </si>
+  <si>
+    <t>www.zakhealth.com</t>
+  </si>
+  <si>
+    <t>David Chen</t>
+  </si>
+  <si>
+    <t>david@kapsuletech.com</t>
+  </si>
+  <si>
+    <t>Kapsule</t>
+  </si>
+  <si>
+    <t>Kapsule aggregates data from pharmacies, hospitals, insurers, and healthtech across Africa to give our customers insights into disease, treatment, and spend habits across African Healthcare.</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1YP7YxKrReYHD0WyJGbicv6xTr1D-_Ewh</t>
+  </si>
+  <si>
+    <t>info@kapsuletech.com</t>
+  </si>
+  <si>
+    <t>Analytics and Data Aggregation</t>
+  </si>
+  <si>
+    <t>Kapsule makes it easy for multinationals and large organizations to understand the health needs, and spend across Africa by making it easily accessible and digestible.</t>
+  </si>
+  <si>
+    <t>Investment into African healthcare has been limited by a lack of data, Kapsule's solution makes it easy for organizations to get the information that they need to make more informed, and data driven decisions.</t>
+  </si>
+  <si>
+    <t>South Africa, Zimbabwe, Kenya, Uganda, Ghana, Nigeria, Ethiopia, Egypt</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>230k</t>
+  </si>
+  <si>
+    <t>500k</t>
+  </si>
+  <si>
+    <t>will share separately</t>
+  </si>
+  <si>
+    <t>We do not collect Personally Identifiable Information (PII) we also have strict encryption and multiple factor authentication</t>
+  </si>
+  <si>
+    <t>Longitudinal health records, Clinical data repository, Clinical data warehouse</t>
+  </si>
+  <si>
+    <t>www.kapsuletech.com</t>
+  </si>
+  <si>
+    <t>Siraaj Adams</t>
+  </si>
+  <si>
+    <t>Siraaj.adams2003@gmail.com</t>
+  </si>
+  <si>
+    <t>Strategic Health Solutions</t>
+  </si>
+  <si>
+    <t>Prep Club</t>
+  </si>
+  <si>
+    <t>Online Prep E commerce platform to improve access to online telemedicine and PrEp medication</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=16CJcANhSMUynpXRCTqQoAYkEQdii2iaa</t>
+  </si>
+  <si>
+    <t>info@prepclub.co.za</t>
+  </si>
+  <si>
+    <t>Virtual Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strategic Health Solutions aims to revolutionize healthcare delivery through its integrated e-prescription and delivery process. The focus is on partnering with healthcare providers and professionals to enhance access to health products and services.
+The project aims to scale operations within South Africa and eventually expand into the rest of Africa.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adherence Issues: 
+Only 34% of healthseekers remain adherent after 12 months. PrEP Club offers ongoing digital support, reminders, Telemedicine counselling and peer engagement to improve adherence.
+Impact:
+With over 50% of at-risk individuals unaware of PrEP, PrEP Club aims to bridge this gap through technology, ensuring prevention is accessible, private, and effective.
+</t>
+  </si>
+  <si>
+    <t>Cape Town South Africa</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>We use Microsoft Azure FHIR</t>
+  </si>
+  <si>
+    <t>We do have a API</t>
+  </si>
+  <si>
+    <t>We apply the interoperable standards with the National Department of Health</t>
+  </si>
+  <si>
+    <t>https://prepclub.co.za/privacy-policy/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We encrypt the data </t>
+  </si>
+  <si>
+    <t>Azure Monitor:
+A comprehensive monitoring service that tracks the performance and health of your applications and infrastructure. It can be used to collect logs from various Azure resources.
+Activity Logs: Track all operations at the subscription level, such as resource creation, modification, or deletion.
+Diagnostic Logs: Provide detailed, resource-level logs that you can configure for Azure</t>
+  </si>
+  <si>
+    <t>Single Sign-On (SSO): Azure AD supports SSO, allowing users to log in once and access multiple Azure applications or external SaaS applications without needing to log in again.
+Multi-Factor Authentication (MFA): To increase security, Azure AD can require MFA, adding an extra layer of protection through phone verification, text codes, or mobile app authentication.</t>
+  </si>
+  <si>
+    <t>Patient Record Management, Individual Registration, Clinical decision support, CPOE/Order Management, Encounter Coding, ER - Triage and Dashboard, Virtual care</t>
+  </si>
+  <si>
+    <t>Dispensing and Medication Administration Record (MAR), Inventory Management, Drug interaction monitoring, Decision Support, Electronic prescribing, EHR Integration</t>
+  </si>
+  <si>
+    <t>Capture biological specimens, Transmit and track diagnostic orders, Send diagnostic results to providers, Capture results from digital devices, Inventory Management, EHR Integration</t>
+  </si>
+  <si>
+    <t>Vaccine-related adverse events monitoring</t>
+  </si>
+  <si>
+    <t>Longitudinal health records, National health domain-specific registries, Clinical data repository, Clinical data warehouse</t>
+  </si>
+  <si>
+    <t>Telemedicine appointments</t>
+  </si>
+  <si>
+    <t>Diagnosis support, Integration and data exchange with local health facility (EMR), Integration with national health systems (DHIS2 or other)</t>
+  </si>
+  <si>
+    <t>https://prepclub.co.za</t>
+  </si>
+  <si>
+    <t>Roy Bore</t>
+  </si>
+  <si>
+    <t>roy.bore@healthxafrica.com</t>
+  </si>
+  <si>
+    <t>HealthX Africa</t>
+  </si>
+  <si>
+    <t>HealthX</t>
+  </si>
+  <si>
+    <t>HealthX is a healthcare innovator that leverages technology to provide high quality, affordable primary care to all Kenyans, regardless of where they live. Through a combination of mobile and telehealth technology, HealthX enables consumers to access a team of licensed and trained primary care doctors, nutritionists &amp; psychologists 24 hours a day, 365 days a year</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1Dr_L8F2R371X2GQzEVCzYecrTlJagE8p</t>
+  </si>
+  <si>
+    <t>support@healthxafrica.com</t>
+  </si>
+  <si>
+    <t>Pharmacy, National and Community Health, AI for Health, Virtual Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HealthX Africa is a subscription-based, data-driven, primary health care provider offering hybrid digital and physical touch points spread strategically across the patient life cycle.
+Our unique phydigital model targeting the un and under-insured in the most vulnerable communities is tailored for Africa. 80% of our encounters are via toll-free indicating the relevance of tailoring digital health solutions for the African context.
+We have successfully integrated into community and national health systems in our service delivery model thus proving that innovative digital health solutions are the answer to Africa's healthcare needs </t>
+  </si>
+  <si>
+    <t>There are significant deficiencies in the African health ecosystem including:
+1. Access; very few doctors as well as very few facilities serving the population
+2. Affordability; very low insurance penetration in LMIC's
+3. Quality; Very few qualified doctors in rural populations
+4. Inequity; 80% of the doctors serve 20% of the population
+Africa's population is growing exponentially and without any interventions, these gaps will result in dire consequences</t>
+  </si>
+  <si>
+    <t>Currently serving over 12 thousand members in 40/47 counties of Kenya</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> On average 90</t>
+  </si>
+  <si>
+    <t>On average 2,800</t>
+  </si>
+  <si>
+    <t>Targeting $1m in 2024</t>
+  </si>
+  <si>
+    <t>$1.2m</t>
+  </si>
+  <si>
+    <t>To be provided at the next stage</t>
+  </si>
+  <si>
+    <t>https://www.healthxafrica.com/privacy-policy/</t>
+  </si>
+  <si>
+    <t>Encryption of at rest and in transit data, two factor authentication for log into the application, role based access to information.</t>
+  </si>
+  <si>
+    <t>database audit trail</t>
+  </si>
+  <si>
+    <t>Set of email, password and OTP for mobile application access, 2FA for users accessing the web application.</t>
+  </si>
+  <si>
+    <t>Patient Record Management, Individual Registration, Clinical decision support, Encounter Coding, Patient Billing, Patient Data Import/Export, ER - Triage and Dashboard, Encounter Data Import/Export, Virtual care</t>
+  </si>
+  <si>
+    <t>Dispensing and Medication Administration Record (MAR), Inventory Management, Drug interaction monitoring, Electronic prescribing, EHR Integration</t>
+  </si>
+  <si>
+    <t>Database plugs into analytics platforms</t>
+  </si>
+  <si>
+    <t>Integration and data exchange with local health facility (EMR)</t>
+  </si>
+  <si>
+    <t>https://www.healthxafrica.com/</t>
+  </si>
+  <si>
+    <t>Stephen Ogweno</t>
+  </si>
+  <si>
+    <t>lifesten.health@gmail.com</t>
+  </si>
+  <si>
+    <t>Lifesten Health</t>
+  </si>
+  <si>
+    <t>We provide a personalized healthcare platform that combines AI-driven health screenings with tailored wellness programs. Our innovative app uses transdermal optical imaging to deliver quick, accurate health assessments. It offers incentive-based gamified health challenges, community support, and tools for wellness, all designed to enhance physical, mental, and nutritional well-being. Our mission is to help users proactively manage their health and prevent lifestyle-related diseases.</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1nIvcqquJRqH_CLwhT8kT25jTnrn9Myg9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lifesten Health leverages advanced AI, gamification principles  and machine learning algorithms to offer a comprehensive health and wellness platform tailored to individual and corporate needs. The core technology integrates real-time health data from the users devices, wearables, user inputs, and their health records on the app to provide personalized and gamified health challenges, insights and recommendations. Our app through the transdermal optical imaging AI analyzes patterns of blood flow on users face and in 30-seconds provides users with diagnostics for 13 key health indicators including blood pressure, stress index and others enabling early detection and proactive intervention. </t>
+  </si>
+  <si>
+    <t>We aim to address the growing burden of lifestyle diseases such as heart disease, diabetes, and hypertension, which affect millions across Africa. Limited access to preventive healthcare and early diagnostics exacerbates these conditions. Through our AI-powered platform, we provide personalized health assessments and wellness programs, empowering users to take control of their health.  Compared to existing solutions, Lifesten's competitive edge lies in its instant health screening capabilities, which led to screening and education for 1.6 million people in a 1-year pilot project with the Government of Rwanda. This technology not only enhances individual health outcomes but also supports organizations in fostering more productive workforce.</t>
+  </si>
+  <si>
+    <t>Kigali - Rwanda</t>
+  </si>
+  <si>
+    <t>Rwanda and Kenya</t>
+  </si>
+  <si>
+    <t>The Lifesten Application has had 3 deployments with the lattest version being Version 2.37 and has reached over 10,000 users.</t>
+  </si>
+  <si>
+    <t>Lifesten has users in more than 70 countries.</t>
+  </si>
+  <si>
+    <t>2300 to 3000</t>
+  </si>
+  <si>
+    <t>This is set to be released in the third major update , however , we provide data to our different users for intergration via customized dashboards and private API conections.</t>
+  </si>
+  <si>
+    <t>https://lifestenhealth.com/data-privacy/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lifesten data is double encypted and hashed and Lifesten has gone through rigoros local and international data compliance checks becoming the first fully AI based data privacy compliant company registered in Rwanda. </t>
+  </si>
+  <si>
+    <t>We do audit logging and get error reporting via a combination of internal debugging and testing and leveraging on Supabase, Firebase and Playstore console which provides logging and error reporting for the platform.</t>
+  </si>
+  <si>
+    <t>We currently use Twilio for verification and OTP.</t>
+  </si>
+  <si>
+    <t>However in the new resease coming up in November we will be using Powersync to provide full offlie support. This is work in progress</t>
+  </si>
+  <si>
+    <t>AI BP Diagnosis  using Transdermal Optical Imaging AI</t>
+  </si>
+  <si>
+    <t>Lifesten app provides end users ability to create and engagein health challenges and plans earn points for improvement and redeem those points for rewards.
+Lifesten App Users and community health workers have access to health screening and diagnostics tools including  mannual health diagnostics forms for blood pressure, blood sugar, BMI  and mental health screenings. Lifesten also includes transdermal optical imaging AI for both users.
+Lifesten provides customized dashboards for companies, health insurances and community health workers/ organizations that use lifesten app for the various use cases befitting their contexts including for productivity enhancement, for health and wellness tracking and for health education and screening campaigns.</t>
+  </si>
+  <si>
+    <t>https://lifestenhealth.com/</t>
+  </si>
+  <si>
+    <t>Jelle Schuitemaker</t>
+  </si>
+  <si>
+    <t>jelle@goal3.org</t>
+  </si>
+  <si>
+    <t>GOAL 3</t>
+  </si>
+  <si>
+    <t>IMPALA System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To address challenges of shortage of staff and lack of suitable equipment in many LMIC hospitals, GOAL 3 developed the IMPALA system: a comprehensive patient monitoring solution to support health workers who are working in resource-constrained settings. It consists of:
+- The IMPALA monitoring device: an easy-to-use multiparameter vital sign monitoring device designed for African settings. It provides ECG, pulse-oximetry, respiratory rate, non-invasive blood pressure and temperature. It has a touch screen, was designed to resist dust, heat and moisture and has an extended battery life.
+- The IMPALA server: Robust and fit-for-context communication and data infrastructure with backup power that provides a local network to connect the IMPALA devices and ensures safe data storage without the need for the Internet.
+- The IMPALA clinical application is a tablet-based central patient overview that is connected to the monitors and gives healthcare workers ultimate control over their ward. It has alarms for when patients go outside expected vital sign ranges and 
+IMPALA enables health workers to manage and monitor their patients better in a resource-constrained environment, allowing them to prioritize scarce time and resources and intervene at an early stage when treatments are more effective and low-cost. This improves patient outcomes but also allows them to recover faster. By reducing the time patients are admitted to the hospital, IMPALA contributes to saving costs as well as reducing workload.  Additionally, IMPALA reduces workload by automating the monitoring of vital signs and facilitating task redistribution.  
+</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1l3WuuIR3mwYo4XHQ3heO-Yg4LbE4M0Bc</t>
+  </si>
+  <si>
+    <t>info@goal3.org</t>
+  </si>
+  <si>
+    <t>The IMPALA system is co-designed with healthcare workers from Malawi and Rwanda, ensuring it directly meets the needs of health professionals in these countries and across the broader region.
+Key features of this innovation include:
+Tailored to Local Needs: The system addresses challenges faced by public hospitals, with a strong emphasis on affordability, sensor availability, and prolonged battery life—critical in resource-limited environments.
+Collaborative Development: Through partnerships with major NGOs and funders, the system has been successfully rolled out in Malawi, Rwanda, and Tanzania, with expansion planned for Uganda and Kenya.
+Durability and Usability: Designed for robustness, the system includes training materials specifically adapted to the needs of healthcare workers in African settings, ensuring both effective use and sustainable impact.</t>
+  </si>
+  <si>
+    <t>Lack of skilled staff and equipment in low-resource settings causes a downward spiral. Because the healthcare facilities are under-resourced, healthcare workers are unable to properly monitor and assess patients, resulting in delays in treatment. This delay increases the need for emergency care for patients and often results in worse patient outcomes. Because of the deterioration of patients, treating them becomes more resource-intensive, causing a vicious cycle, as staff then become more overburdened responding to resource-intensive care.
+In order to break the cycle in low-resource settings, proper risk assessment and monitoring is needed. With the implementation of IMPALA, hospitals are able to properly assess and monitor all patients, reducing delays in treatment. The result being a significant reduction in emergency care – which improves patient outcomes and reduces the burden on the staff. 
+Early pilot results from a district hospital in Malawi demonstrated a 42% reduction in pediatric mortality, translating to an internal cost-effectiveness estimate of approximately $208 per life saved. If these results hold up on further research, IMPALA is a potentially game-changing intervention, with cost-effectiveness competitive with the most effective standard of care interventions such as treatments for malaria.
+With 167 IMPALA systems incorporated in 11 hospitals, we are making a significant impact every day. If we translate these results into our growth projections, in the recommended five years we will train and relieve more than 150,000 doctors and nurses and make their work more bearable, 40 million people will receive the better care they deserve and we can prevent more than 120,000 deaths.</t>
+  </si>
+  <si>
+    <t>Rwanda, Malawi, Tanzania</t>
+  </si>
+  <si>
+    <t>11 hospitals are using in total 167 IMPALA systems</t>
+  </si>
+  <si>
+    <t>3 countries: Malawi, Tanzania, Rwanda</t>
+  </si>
+  <si>
+    <t>About 15 health workers per hospital x 11 hospitals = 165 daily active users, monitoring over 200 patients daily</t>
+  </si>
+  <si>
+    <t>On average 12 patients a month per monitor x 167 monitors = 2004 patients monitored per month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Around $500,000 </t>
+  </si>
+  <si>
+    <t>Around $4,5 million</t>
+  </si>
+  <si>
+    <t>https://eu1.hubs.ly/H0cNzrL0</t>
+  </si>
+  <si>
+    <t>Available after NDA</t>
+  </si>
+  <si>
+    <t>In the roadmap for 2025</t>
+  </si>
+  <si>
+    <t>Yes, the solution is developed using GDPR standards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOAL 3 has set-up direct communication channels with hospitals for error reporting. </t>
+  </si>
+  <si>
+    <t>Patients are admitted using the patient ID's used by the national system and patient files</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1qB1Nbo7eXgrbF9dk80C4_uZNG6whRBm5?usp=sharing</t>
+  </si>
+  <si>
+    <t>Patient Record Management, Individual Registration, Clinical decision support, Patient Data Import/Export, Encounter Data Import/Export, Encounter Workflow Support</t>
+  </si>
+  <si>
+    <t>EHR Integration</t>
+  </si>
+  <si>
+    <t>Longitudinal health records</t>
+  </si>
+  <si>
+    <t>Guided self help, Remote patient (or person) monitoring</t>
+  </si>
+  <si>
+    <t>www.goal3.org</t>
+  </si>
+  <si>
+    <t>Yaw Asamoah</t>
+  </si>
+  <si>
+    <t>yaw@medpharma.care</t>
+  </si>
+  <si>
+    <t>Medpharma Alliance International Limited</t>
+  </si>
+  <si>
+    <t>Medpharma</t>
+  </si>
+  <si>
+    <t>Medpharma Alliance International Limited is a healthcare platform. Our aim is to build a community of partners (practitioners, service providers, big pharma) that provide healthcare to the patient. Our primary services are e-consultation, e-prescription, diagnostics, storage of medical records and delivery of medicines and devices.</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1XgrD20NQJLstL8TAXREV3akMFUoJtBaz</t>
+  </si>
+  <si>
+    <t>customer@medpharma.care</t>
+  </si>
+  <si>
+    <t>Electronic Health Record, Pharmacy, Laboratory and Diagnostics, National and Community Health, Analytics and Data Aggregation, AI for Health, Virtual Health</t>
+  </si>
+  <si>
+    <t>We have built a platform that allows patients to put their medical requests on our mobile, web, or chatbot. Our intuitive platform provides services in the areas of e-consultation, e-prescription, delivery of medicines, diagnostics, and storage of medical records. We have also creatively bundled products like the Chronic Disease Management Product to cater to specific demographic groups. Other products we will be introducing in the future are a subscription model, PregCare, and WestCare for healthcare remittances.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After almost three and a half years in operations, we have exceeded GHS 25M in sales. Had over 1.5M medicines served, 400K customer touchpoints, 80K consultations and 70K unique customers served. We have also opened a pipeline to over 15M customers with MTN. </t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Over 50,000 Unique customers</t>
+  </si>
+  <si>
+    <t>about 50+</t>
+  </si>
+  <si>
+    <t>700+</t>
+  </si>
+  <si>
+    <t>$290k</t>
+  </si>
+  <si>
+    <t>1 - grant through the Gates Foundation</t>
+  </si>
+  <si>
+    <t>Records are encrypted</t>
+  </si>
+  <si>
+    <t>Email / txt OTP</t>
+  </si>
+  <si>
+    <t>Patient Record Management, Individual Registration, Clinical decision support, Patient Billing, Patient Data Import/Export, Virtual care</t>
+  </si>
+  <si>
+    <t>Dispensing and Medication Administration Record (MAR), Electronic prescribing</t>
+  </si>
+  <si>
+    <t>Send diagnostic results to providers, Inventory Management</t>
+  </si>
+  <si>
+    <t>Telemedicine appointments, Interactive services/chatbots</t>
+  </si>
+  <si>
+    <t>Patient vaccination record, Digital vaccine card</t>
+  </si>
+  <si>
+    <t>www.medpharma.care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">courtney@reachdigitalhealth.org </t>
+  </si>
+  <si>
+    <t>Alô Vida+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alô Vida originated as a nationwide hotline in Mozambique, offering health-related guidance in Portuguese, English, and eight other local languages. It was originally launched as a health hotline that provides personalized health information on sexual and reproductive health (SRH), HIV, COVID-19, and immunizations through real-time interactions with healthcare professionals. With a dedicated call center, Alô Vida enables direct communication between users and trained health professionals, offering a trusted source of medical advice and guidance.
+Alô Vida+ builds on this foundation by incorporating Interactive Voice Recording (IVR) and WhatsApp-based services, enhancing accessibility and engagement. Reach Digital Health is developing the WhatsApp chatbot component that complements the hotline service, allowing users to receive personalized health information and engage in interactive health assessments through a widely used and cost-effective platform.
+Alô Vida+ is designed as a scalable and sustainable digital health solution under the ownership of Mozambique’s Ministry of Health (MISAU). By engaging both caregivers and healthcare professionals through mobile and voice technology, it aims to improve health outcomes for vulnerable populations, with a special focus on immunization and HIV prevention. The platform is fully adaptable for nationwide scale-up, ensuring continued support across Mozambique’s health system.
+</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1ztGJqJ_XaWNh5byPOqdpNv7IAtM9iUBn</t>
+  </si>
+  <si>
+    <t>Electronic Health Record, National and Community Health, Analytics and Data Aggregation, AI for Health, Vaccination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Alô Vida+ service is designed to improve health outcomes by leveraging widely accessible mobile technology, like WhatsApp, to engage citizens and provide them with vital healthcare information and services. By offering personalized support and guidance, Alô Vida+ empowers individuals to take control of their health and make informed decisions, specifically around childhood vaccination. The aim is to bolster the persistence of childhood inoculations by empowering users and fostering informed decision-making. This involves helping users overcome contextual barriers, promoting equitable access to health information and services, leveraging real-time data for learning and decision-making, thus benefiting both the health system and its constituents. 
+The specific aims of Alô Vida+ are to improve maternal and child health outcomes. The desired outcomes include:
+- Increased antenatal care attendance
+- Improved childhood vaccination rates
+- Increased knowledge and self-efficacy regarding contraceptive use, family planning services, and breastfeeding
+- Improved birth outcomes
+- Improved adherence to PMTCT protocols among HIV-positive mothers
+- Reduced maternal and neonatal mortality rates
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Mozambique, Alô Vida+ fits into a landscape of MNCH and immunization challenges, including low childhood vaccination rates, leaving many children unprotected from preventable diseases like measles, polio, and pneumonia, which can lead to severe complications or death. Barriers to accessing healthcare information and services, such as limited health literacy, misinformation about vaccines, geographical isolation, poverty, and cultural beliefs, further exacerbate the problem, particularly in areas with limited healthcare infrastructure and resources. Remote communities often lack access to healthcare facilities, while socioeconomic challenges and cultural practices discourage vaccination and healthcare-seeking behaviors. These issues contribute to high rates of preventable diseases and mortality among mothers and children. 
+By leveraging mobile technology and a user-centered design, Alô Vida+ addresses barriers such as low health literacy, misinformation, and missed appointments, ultimately improving health outcomes. Alô Vida+ is currently scheduled for a general programmatic evaluation of outcomes in October 2024. In addition, a Danger Signs study will capture evidence on the number of people seeking care for pregnancy or neonatal emergencies (expected by the end of the calendar year).
+</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>1 in Mozambique</t>
+  </si>
+  <si>
+    <t>30,494 all time users in 3 months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total interactions not available, but we have 7,730 push messages sent out and 3,010 messages received in the last 3 months. 1,226 users have also searched for health information, and 1,985 informational messages have been viewed in the last 3 months. </t>
+  </si>
+  <si>
+    <t>The WhatsApp service is integrated with the MISAU’s national health hotline service, Alô Vida, which offers personalised information on sexual and reproductive health, HIV, COVID-19, and vaccinations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/document/d/1JKBB-UTxE8Ctb7LFkKarPX6Z6j_92DTQu91UJe8tVjQ/edit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alô Vida+ ensures the privacy and protection of PHI through:
+- Compliance with Regulations: Alô Vida+ adheres to Article 71 of the Constitution of the Republic of Mozambique, the EU General Data Protection Regulations and the Protection of Personal Information Act, 4 of 2013 (SA) and other relevant data privacy laws and regulations.
+- Informed Consent: Alô Vida+ obtains informed consent from users before collecting, processing, or sharing their PHI. Users are informed about the purpose of data collection, how their data will be used, and who will have access to it.
+- Data Minimization: Alô Vida+ collects only the minimum necessary PHI required to provide the service and achieve its public health objectives.
+- Secure Data Storage and Transmission: Alô Vida+ employs robust security measures to protect PHI from unauthorized access, use, or disclosure.
+- Data Retention and Deletion: Alô Vida+ has clear policies for data retention and deletion, ensuring that PHI is not kept longer than necessary and is securely deleted or anonymized when no longer needed.
+- User Control: Alô Vida+ provides users with control over their PHI, allowing them to access, update, correct, and delete their information as needed.
+- Transparency: Alô Vida+ maintains transparency about its data practices, providing users with clear and accessible information about how their PHI is handled.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Audit Logs: All logs are sent to AWS Cloudtrail to ensure a record of actions taken by a user, role, or an AWS service is captured. This information can be used to determine the request that was made, the IP address from which the request was made, who made the request, when it was made, and additional details. Administrator access to critical system hardware and servers is logged
+Monitoring: A set of rules and services have been implemented to monitor for changes to services, alert administrators of any potential risks, and diagnose overly permissive security group rules.
+</t>
+  </si>
+  <si>
+    <t>Targeted health promotion messages: Alô Vida+ sends stage-based health messages to pregnant women and new mothers, promoting healthy behaviors and timely healthcare utilization, contributing to improved MNCH and immunization outcomes at both community and national levels. Interactive feedback mechanism: Alô Vida+ provides a platform for women to provide feedback on the quality of care received at public health facilities, enabling the Department of Health to monitor and improve service delivery, impacting community health directly. Helpdesk and Chatbot Support: Alô Vida+ offers a helpdesk for users to ask questions or report concerns, providing personalized support and guidance, contributing to positive health outcomes in the community.</t>
+  </si>
+  <si>
+    <t>Patient vaccination record, Digital vaccine card, Vaccination reminders and follow-ups</t>
+  </si>
+  <si>
+    <t>https://www.reachdigitalhealth.org/projects/alovidaplus</t>
+  </si>
+  <si>
+    <t>Victoria Mabel Sackey</t>
+  </si>
+  <si>
+    <t>victoria@medtrack.africa</t>
+  </si>
+  <si>
+    <t>MedTrack Technologies Limited</t>
+  </si>
+  <si>
+    <t>MedTrack</t>
+  </si>
+  <si>
+    <t>An interoperable, comprehensive and secure cloud-based health information management system that links patient health data to national biometric IDs.</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1i1dyED1IkSCdmFryHCCKqBYcKjvqnzix</t>
+  </si>
+  <si>
+    <t>info@medtrack.africa</t>
+  </si>
+  <si>
+    <t>Electronic Health Record, Pharmacy, Laboratory and Diagnostics</t>
+  </si>
+  <si>
+    <t>MedTrack is addressing key challenges in the African healthcare landscape by leveraging national biometric IDs in its platform to create unified, portable health records, enhancing continuity of care across different providers and facilities.
+The system's data aggregation capabilities are designed to enable public health officials to identify trends and predict outbreaks, informing crucial policy decisions. The design considers unique local challenges, offering offline functionality for areas with limited connectivity, as well as partnerships with telecom providers and tech companies for accessibility in low-resource settings.
+By digitizing records and automating processes, MedTrack reduces errors and improves efficiency in healthcare delivery. The platform's interoperability with existing systems, combined with patient engagement features like SMS reminders, enhances overall care quality. Additionally, its support for telemedicine expands access to specialized care in remote regions.
+Through this comprehensive approach, MedTrack is addressing the systemic inefficiencies to improve health outcomes.</t>
+  </si>
+  <si>
+    <t>MedTrack addresses a critical market need in the African healthcare ecosystem by tackling the challenge of fragmented and inefficient health record management. This need is particularly acute in Africa, where the healthcare system struggles with disjointed records across multiple facilities, leading to inefficiencies, duplicated efforts, and compromised patient care.
+The platform has linked over 210,000 health records to national biometric IDs, benefiting over 16,000 registered patients. It has been tested and piloted in select facilities in rural and suburban settings, enhancing efficiency for health workers. MedTrack is improving healthcare access in low-resource settings through strategic partnerships. Its data aggregation capabilities are enabling more informed public health decision-making.</t>
+  </si>
+  <si>
+    <t>Accra - Ghana</t>
+  </si>
+  <si>
+    <t>Over 11,000 unique patients</t>
+  </si>
+  <si>
+    <t>https://icd.who.int/docs/icd-api/APIDoc-Version2/</t>
+  </si>
+  <si>
+    <t>MedTrack integrates with several national health systems in Ghana:
+1. District Health Information System 2 (DHIS2): MedTrack's platform is designed to integrate with Ghana's DHIS2, which is the national health management information system used by the Ghana Health Service. This integration allows for seamless reporting and data sharing between MedTrack and the national health information system.
+2. National Health Insurance Scheme (NHIS): MedTrack's solution is built to interoperate with the NHIS, enabling healthcare providers to easily verify patient insurance status and process claims within the MedTrack platform.
+3. Ghana Card (National Biometric ID System): MedTrack leverages Ghana's national biometric digital ID system to provide portable Electronic Health Records to every citizen. This integration ensures secure data storage and sharing across healthcare facilities, linking health records to patients' unique national ID numbers.</t>
+  </si>
+  <si>
+    <t>https://medtrack.africa/privacy-policy</t>
+  </si>
+  <si>
+    <t>We maintain application, security and user audit logs. All user actions are time stamped and associated with the user that performed the action. This information is persisted to the database. In addition we also maintain related application logs in log files that are persisted to our s3 buckets. These also contains relevant information about user and application making the request such as IP, browser, etc.
+For the system we leverage both our application and cloud provider to keep logs of system wide activities such as deployments, restarts, shutdowns, etc.
+Our error reporting mechanism involves both system and user reports.
+We also leverage log files for system error reporting. For user error reporting, we have a customer support form/document for collecting error reports from our users.
+We continue to evaluate external logging and reporting systems that meet HIPPA standards for integration in the future.</t>
+  </si>
+  <si>
+    <t>We leverage industry standards for  Identity and Access Management (IAM) on our platform while also considering accessibility for our target market.
+Authentication:
+We leverage JWT tokens for user authentication. All requests to our authenticated Graphql and REST endpoints must have authentication token in the headers. We also allow users to leverage 2FA for our web based login.
+In order to verify the identity of our users we validate phone numbers during registration by sending an SMS code for the user to verify that they own that number.
+Authorization:
+We use Role Based Access Control (RBAC) to ensure users in a facility have access to only the information they are authorized to. For instance, a nurse in a facility has different access from a physician based on their roles.
+We also use SMS code authorization when a facility wants to access a patient's information. In this case, we send a code to the patient that the patient must provide to the facility before access is granted. Once authorized, the facility will have access to the patient information. We also provide a mechanism for the patient to revoke a facility’s access to their information at any time.</t>
+  </si>
+  <si>
+    <t>Patient Record Management, Individual Registration, Clinical decision support, CPOE/Order Management, Encounter Coding, Patient Data Import/Export, Patient care templates, ER - Triage and Dashboard, Encounter Data Import/Export, Encounter Workflow Support</t>
+  </si>
+  <si>
+    <t>Dispensing and Medication Administration Record (MAR), Decision Support, Electronic prescribing, EHR Integration</t>
+  </si>
+  <si>
+    <t>Longitudinal health records, Clinical data repository</t>
+  </si>
+  <si>
+    <t>Data visualization, Dashboards, Clinical data dashboards</t>
+  </si>
+  <si>
+    <t>www.medtrack.africa</t>
+  </si>
+  <si>
+    <t>Bryan Plummer</t>
+  </si>
+  <si>
+    <t>bryan.plummer@signalytic.ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signalytic </t>
+  </si>
+  <si>
+    <t>The S+ Platform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The S+ Platform is a solar-powered network of computing devices focused on the outcome of ‘digital uptime’ and ‘data accessibility’. This approach enables improved visibility of health data such as health supply chain data, through a commitment to ensuring power, connectivity, hardware and software offerings are adequately integrated and performing, all the time.
+Each Unit of the S+ Platform consists of an S+ Box (containing a processor, IoT SIM card, batteries, and antennas), a solar panel, and tablet. The platform runs on a first-of-its-kind off-grid Distributed Ledger Technology (DLT) with decentralized data storage and accessibility, and hosts 3rd party softwares, like EMRs, lab systems, etc. 
+This approach to Decentralized Physical Infrastructure will provide the technical foundation for the inclusive and equitable digital health system of the future - through tokenized data governance and smart contract based Universal Health schemes. 
+</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1ZXXHT5lVC7Mxhymawml5ro45Vtoj7dAM</t>
+  </si>
+  <si>
+    <t>Electronic Health Record, Pharmacy, Laboratory and Diagnostics, Disease Surveillance, National and Community Health, Analytics and Data Aggregation, Front-line (CHW) tools, Vaccination</t>
+  </si>
+  <si>
+    <t>In order to improve health outcomes, all access points to the health system need to be equipped with the context appropriate infrastructure to ensure data events, transactions and resources can be digitized from the onset. This data needs to be stored and made available in a format that can be accessible and usable by other stakeholders that need to or can benefit from that data. In doing so, the infrastructure is able to ensure that all work flows and decision making is digital and data-driven.  The S+ Platform is a fit-for-purpose infrastructure, for all access points, that can bring digital tools and devices like EMRs, eLMISs, lab systems, biometric devices, and more, to the places they need to be to ensure the high quality provision of care.</t>
+  </si>
+  <si>
+    <t>Billions of dollars are spent every year by ministries and international organizations to provide access to medicines and quality care in LMICs, however the infrastructure, systems and financing structures are not designed properly, resulting in poor health outcomes and wasted resources. 
+The market need is around having integrated digital infrastructure that works. Too often, the current digital paradigm fails patients and health care providers because one or more of hardware, connectivity, power, data accessibility or access to financial resources prevents digital from being possible and resulting in analog and paper based processes. Digital systems are only as good as the weakest of these factors. 
+By providing an always-on infrastructure platform, our S+ Platform clients (heath center staff, software providers, development partners and Ministry of Health) are finally all connected to the same, equitable infrastructure and critical data. This results in better health outcomes, resource allocation and a health system that works for everyone.</t>
+  </si>
+  <si>
+    <t>Vancouver, Canada</t>
+  </si>
+  <si>
+    <t>Uganda, Kenya, Nigeria, Burundi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our solution is hardware and firmware. We support 3rd party softwares that often times are entirely or mostly done by African developers. </t>
+  </si>
+  <si>
+    <t>6 active deployments; across them there are 100+ private health facilities, 3 software providers, 1 medicine distributor, 2 NGO's, 1 data aggregator</t>
+  </si>
+  <si>
+    <t>150+</t>
+  </si>
+  <si>
+    <t>100,000+</t>
+  </si>
+  <si>
+    <t>$450,000 USD</t>
+  </si>
+  <si>
+    <t>$2m USD</t>
+  </si>
+  <si>
+    <t>We implement the standards that are tied to the solutions and softwares that we support and work with.  In 2025, our S+ DLT database will be FHIR-native.</t>
+  </si>
+  <si>
+    <t>By request.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can integrate to any national or regional health systems that our clients already connect to, or want to connect to, including ERPs, DHIS2 and existing dashboards they use. When we onboard a new client or tool, we take these integrations as requirements and implement in the best mutually agreed upon way. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Safety - Locked, steel enclosures, bolted to a wall without possibility of unbolting externally. Malware access points eliminated through locked down tablets and selective
+restriction of connecting devices.
+Data Security - mTLS 1.3. Private root certificate and intermediate certification authorities for key creation and rotation. Data encryption and key management options of 3rd Party Client applications. Data locally hosted in-country.
+Access Control - Role-based access control system manages the
+association between user accounts and access to edge server locations and applications. Access management performed via the S+ Console. Local accounts creation and assignment by a designated local administrator.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All S+ system data is stored on an immutable Distributed Ledger Technology (DLT).  Error reporting (on all hardware and infrastructure performance) is automated and is presented in a web-based dashboard for remote visibility and response.    End-users can also report errors via the S+ tablet and kiosk interface where they access digital tools. </t>
+  </si>
+  <si>
+    <t>Hosted client softwares are responsible for their own user access handling. Accounts that access Signalytic functions use a traditional username and password. Passwords are stored and transmitted in hashed form. Engineering access to systems is protected with short duration encryption key pairs.</t>
+  </si>
+  <si>
+    <t>The S+ Platform allows for the offline support of the S+ Platform (infrastructure), while also enabling offline support for our software clients (if and as available)</t>
+  </si>
+  <si>
+    <t>Patient Record Management, All EHR/EMR modules and functionalities that our software partners have or want to use, are possible on the S+ Platform.</t>
+  </si>
+  <si>
+    <t>Inventory Management, The S+ Platform does have a native (optional) open-source Stock Management tool.</t>
+  </si>
+  <si>
+    <t>All that are currently available within our partners/clients solutions.</t>
+  </si>
+  <si>
+    <t>Data visualization, Dashboards, Data processing (extract, transform, load - ETL), The S+ DLT transmits data to existing client analytics and tools.</t>
+  </si>
+  <si>
+    <t>The S+ DLT creates data sources that could be leveraged by 3rd party AI capabilities.</t>
+  </si>
+  <si>
+    <t>All that are currently available within our partners/clients solutions, however offline or intermittent forms of Virtual Health might be preferred.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The S+ Platform has a value proposition for all stakeholders that contribute to the creation, utilisation and consumption of critical health data.  As such, Signalytic strives to unlock a value-based marketplace where incentives are aligned by all parties, and both costs and benefits of this digital infrastructure can be shared.  Signalytic is already piloting unique cost-sharing models where facilities, software providers and medicine distributor are all paying a nominal amount into a shared and mutually beneficial, S+ data ecosystem. 
+The S+ DLT, over time, will be used to implement data ownership and access modalities, while also enabling smart contracts and more automated forms of Results Based Financing.
+</t>
+  </si>
+  <si>
+    <t>www.signalytic.ca</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -1467,7 +3079,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border/>
     <border>
       <left style="thin">
@@ -1623,11 +3235,25 @@
         <color rgb="FF442F65"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF442F65"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF442F65"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1739,6 +3365,12 @@
     <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -1749,6 +3381,9 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1809,7 +3444,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:BD17" displayName="Form_Responses1" name="Form_Responses1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:BD35" displayName="Form_Responses1" name="Form_Responses1" id="1">
   <tableColumns count="56">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Your name" id="2"/>
@@ -4315,128 +5950,2819 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="37">
+      <c r="A17" s="25">
         <v>45565.592789525464</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="26" t="s">
         <v>373</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="26" t="s">
         <v>374</v>
       </c>
-      <c r="D17" s="38" t="s">
+      <c r="D17" s="26" t="s">
         <v>375</v>
       </c>
-      <c r="E17" s="38" t="s">
+      <c r="E17" s="26" t="s">
         <v>376</v>
       </c>
-      <c r="F17" s="38" t="s">
+      <c r="F17" s="26" t="s">
         <v>377</v>
       </c>
-      <c r="G17" s="39" t="s">
+      <c r="G17" s="27" t="s">
         <v>378</v>
       </c>
-      <c r="H17" s="38" t="s">
+      <c r="H17" s="26" t="s">
         <v>379</v>
       </c>
-      <c r="I17" s="38" t="s">
+      <c r="I17" s="26" t="s">
         <v>380</v>
       </c>
-      <c r="J17" s="38" t="s">
+      <c r="J17" s="26" t="s">
         <v>381</v>
       </c>
-      <c r="L17" s="38" t="s">
+      <c r="L17" s="26" t="s">
         <v>382</v>
       </c>
-      <c r="M17" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="N17" s="38" t="s">
+      <c r="M17" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="N17" s="26" t="s">
         <v>383</v>
       </c>
-      <c r="O17" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="P17" s="40">
+      <c r="O17" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="P17" s="28">
         <v>1.0</v>
       </c>
-      <c r="Q17" s="40">
+      <c r="Q17" s="28">
         <v>1.0</v>
       </c>
-      <c r="R17" s="38" t="s">
+      <c r="R17" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="S17" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="T17" s="38" t="s">
+      <c r="S17" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="T17" s="26" t="s">
         <v>384</v>
       </c>
-      <c r="U17" s="38" t="s">
+      <c r="U17" s="26" t="s">
         <v>385</v>
       </c>
-      <c r="V17" s="38">
+      <c r="V17" s="26">
         <v>9000.0</v>
       </c>
-      <c r="W17" s="38">
+      <c r="W17" s="26">
         <v>800000.0</v>
       </c>
-      <c r="X17" s="38">
+      <c r="X17" s="26">
         <v>250000.0</v>
       </c>
-      <c r="Y17" s="38" t="s">
+      <c r="Y17" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="Z17" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB17" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD17" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="AF17" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="AG17" s="39" t="s">
+      <c r="Z17" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB17" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD17" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF17" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG17" s="27" t="s">
         <v>386</v>
       </c>
-      <c r="AI17" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ17" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="AM17" s="38" t="s">
+      <c r="AI17" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ17" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM17" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="AN17" s="38" t="s">
+      <c r="AN17" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="AO17" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="AQ17" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="AR17" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS17" s="38" t="s">
+      <c r="AO17" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ17" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR17" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS17" s="26" t="s">
         <v>387</v>
       </c>
-      <c r="AT17" s="38" t="s">
+      <c r="AT17" s="26" t="s">
         <v>388</v>
       </c>
-      <c r="AU17" s="38" t="s">
+      <c r="AU17" s="26" t="s">
         <v>389</v>
       </c>
-      <c r="AX17" s="38" t="s">
+      <c r="AX17" s="26" t="s">
         <v>349</v>
       </c>
-      <c r="AY17" s="38" t="s">
+      <c r="AY17" s="26" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="31">
+        <v>45565.83219244213</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>391</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>392</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>393</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>394</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>395</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>396</v>
+      </c>
+      <c r="I18" s="32" t="s">
+        <v>397</v>
+      </c>
+      <c r="J18" s="32" t="s">
+        <v>398</v>
+      </c>
+      <c r="K18" s="32" t="s">
+        <v>399</v>
+      </c>
+      <c r="L18" s="32" t="s">
+        <v>400</v>
+      </c>
+      <c r="M18" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="N18" s="32" t="s">
+        <v>400</v>
+      </c>
+      <c r="O18" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="P18" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="Q18" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="R18" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="S18" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="T18" s="32" t="s">
+        <v>401</v>
+      </c>
+      <c r="U18" s="32" t="s">
+        <v>402</v>
+      </c>
+      <c r="V18" s="32" t="s">
+        <v>403</v>
+      </c>
+      <c r="W18" s="32" t="s">
+        <v>404</v>
+      </c>
+      <c r="X18" s="32" t="s">
+        <v>405</v>
+      </c>
+      <c r="Y18" s="32" t="s">
+        <v>406</v>
+      </c>
+      <c r="Z18" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA18" s="33" t="s">
+        <v>407</v>
+      </c>
+      <c r="AB18" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD18" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF18" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG18" s="33" t="s">
+        <v>408</v>
+      </c>
+      <c r="AH18" s="32" t="s">
+        <v>409</v>
+      </c>
+      <c r="AI18" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ18" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK18" s="32" t="s">
+        <v>410</v>
+      </c>
+      <c r="AL18" s="32" t="s">
+        <v>411</v>
+      </c>
+      <c r="AM18" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN18" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO18" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ18" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR18" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS18" s="32" t="s">
+        <v>412</v>
+      </c>
+      <c r="AT18" s="32" t="s">
+        <v>413</v>
+      </c>
+      <c r="AU18" s="32" t="s">
+        <v>414</v>
+      </c>
+      <c r="AV18" s="32" t="s">
+        <v>413</v>
+      </c>
+      <c r="AW18" s="32" t="s">
+        <v>413</v>
+      </c>
+      <c r="AX18" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="AY18" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="AZ18" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="BA18" s="32" t="s">
+        <v>413</v>
+      </c>
+      <c r="BB18" s="32" t="s">
+        <v>415</v>
+      </c>
+      <c r="BC18" s="33" t="s">
+        <v>416</v>
+      </c>
+      <c r="BD18" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="25">
+        <v>45566.00334708333</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>417</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>418</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>419</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>420</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>421</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>422</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>423</v>
+      </c>
+      <c r="I19" s="26" t="s">
+        <v>424</v>
+      </c>
+      <c r="J19" s="26" t="s">
+        <v>425</v>
+      </c>
+      <c r="K19" s="26" t="s">
+        <v>426</v>
+      </c>
+      <c r="L19" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="M19" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="N19" s="26" t="s">
+        <v>428</v>
+      </c>
+      <c r="O19" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="P19" s="26" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q19" s="26" t="s">
+        <v>430</v>
+      </c>
+      <c r="R19" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="S19" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="T19" s="26" t="s">
+        <v>431</v>
+      </c>
+      <c r="U19" s="26" t="s">
+        <v>432</v>
+      </c>
+      <c r="V19" s="26" t="s">
+        <v>433</v>
+      </c>
+      <c r="W19" s="26" t="s">
+        <v>434</v>
+      </c>
+      <c r="X19" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="Y19" s="26" t="s">
+        <v>436</v>
+      </c>
+      <c r="Z19" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB19" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD19" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF19" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG19" s="27" t="s">
+        <v>437</v>
+      </c>
+      <c r="AH19" s="26" t="s">
+        <v>438</v>
+      </c>
+      <c r="AI19" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ19" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK19" s="26" t="s">
+        <v>439</v>
+      </c>
+      <c r="AL19" s="26" t="s">
+        <v>440</v>
+      </c>
+      <c r="AM19" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN19" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO19" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AQ19" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR19" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS19" s="26" t="s">
+        <v>441</v>
+      </c>
+      <c r="AT19" s="26" t="s">
+        <v>442</v>
+      </c>
+      <c r="AU19" s="26" t="s">
+        <v>443</v>
+      </c>
+      <c r="AV19" s="26" t="s">
+        <v>444</v>
+      </c>
+      <c r="AW19" s="26" t="s">
+        <v>445</v>
+      </c>
+      <c r="AX19" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="AY19" s="26" t="s">
+        <v>446</v>
+      </c>
+      <c r="AZ19" s="26" t="s">
+        <v>447</v>
+      </c>
+      <c r="BA19" s="26" t="s">
+        <v>448</v>
+      </c>
+      <c r="BB19" s="26" t="s">
+        <v>449</v>
+      </c>
+      <c r="BC19" s="27" t="s">
+        <v>450</v>
+      </c>
+      <c r="BD19" s="30" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="31">
+        <v>45566.09739380787</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>451</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>452</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>453</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="F20" s="32" t="s">
+        <v>455</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>456</v>
+      </c>
+      <c r="H20" s="32" t="s">
+        <v>457</v>
+      </c>
+      <c r="I20" s="32" t="s">
+        <v>458</v>
+      </c>
+      <c r="J20" s="32" t="s">
+        <v>459</v>
+      </c>
+      <c r="K20" s="32" t="s">
+        <v>460</v>
+      </c>
+      <c r="L20" s="32" t="s">
+        <v>461</v>
+      </c>
+      <c r="M20" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="N20" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="O20" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="P20" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="Q20" s="34">
+        <v>0.6</v>
+      </c>
+      <c r="R20" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="S20" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="T20" s="32" t="s">
+        <v>462</v>
+      </c>
+      <c r="U20" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="V20" s="37">
+        <v>447000.0</v>
+      </c>
+      <c r="W20" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="X20" s="35">
+        <v>200000.0</v>
+      </c>
+      <c r="Y20" s="35">
+        <v>650000.0</v>
+      </c>
+      <c r="Z20" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB20" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC20" s="32" t="s">
+        <v>464</v>
+      </c>
+      <c r="AD20" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF20" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG20" s="32" t="s">
+        <v>465</v>
+      </c>
+      <c r="AH20" s="32" t="s">
+        <v>466</v>
+      </c>
+      <c r="AI20" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK20" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="AL20" s="32" t="s">
+        <v>468</v>
+      </c>
+      <c r="AM20" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN20" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="AO20" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ20" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR20" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS20" s="32" t="s">
+        <v>469</v>
+      </c>
+      <c r="AX20" s="32" t="s">
+        <v>470</v>
+      </c>
+      <c r="AY20" s="32" t="s">
+        <v>446</v>
+      </c>
+      <c r="AZ20" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="BC20" s="33" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="25">
+        <v>45566.125998055555</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>472</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>473</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>474</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>475</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>476</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>477</v>
+      </c>
+      <c r="I21" s="26" t="s">
+        <v>478</v>
+      </c>
+      <c r="J21" s="26" t="s">
+        <v>479</v>
+      </c>
+      <c r="K21" s="26" t="s">
+        <v>480</v>
+      </c>
+      <c r="L21" s="26" t="s">
+        <v>481</v>
+      </c>
+      <c r="M21" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="N21" s="26" t="s">
+        <v>482</v>
+      </c>
+      <c r="O21" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="P21" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="Q21" s="28">
+        <v>0.9</v>
+      </c>
+      <c r="R21" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="S21" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="T21" s="26" t="s">
+        <v>483</v>
+      </c>
+      <c r="U21" s="26" t="s">
+        <v>484</v>
+      </c>
+      <c r="V21" s="26">
+        <v>200.0</v>
+      </c>
+      <c r="W21" s="26" t="s">
+        <v>485</v>
+      </c>
+      <c r="X21" s="26" t="s">
+        <v>486</v>
+      </c>
+      <c r="Y21" s="29">
+        <v>5000000.0</v>
+      </c>
+      <c r="Z21" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB21" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD21" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE21" s="26" t="s">
+        <v>487</v>
+      </c>
+      <c r="AF21" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH21" s="26" t="s">
+        <v>488</v>
+      </c>
+      <c r="AI21" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ21" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM21" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN21" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="AO21" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP21" s="26" t="s">
+        <v>489</v>
+      </c>
+      <c r="AQ21" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR21" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AT21" s="26" t="s">
+        <v>490</v>
+      </c>
+      <c r="AU21" s="26" t="s">
+        <v>490</v>
+      </c>
+      <c r="AV21" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="AX21" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="BC21" s="27" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="31">
+        <v>45566.16559164352</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>492</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>493</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>494</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="F22" s="32" t="s">
+        <v>496</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>497</v>
+      </c>
+      <c r="H22" s="32" t="s">
+        <v>498</v>
+      </c>
+      <c r="I22" s="32" t="s">
+        <v>499</v>
+      </c>
+      <c r="J22" s="32" t="s">
+        <v>500</v>
+      </c>
+      <c r="K22" s="32" t="s">
+        <v>501</v>
+      </c>
+      <c r="L22" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="M22" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="N22" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="O22" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="P22" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="Q22" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="R22" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="S22" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="T22" s="32">
+        <v>1.0</v>
+      </c>
+      <c r="U22" s="32" t="s">
+        <v>502</v>
+      </c>
+      <c r="V22" s="32" t="s">
+        <v>503</v>
+      </c>
+      <c r="W22" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="X22" s="32" t="s">
+        <v>505</v>
+      </c>
+      <c r="Y22" s="35">
+        <v>1700000.0</v>
+      </c>
+      <c r="Z22" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA22" s="32" t="s">
+        <v>506</v>
+      </c>
+      <c r="AB22" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC22" s="32" t="s">
+        <v>506</v>
+      </c>
+      <c r="AD22" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE22" s="32" t="s">
+        <v>506</v>
+      </c>
+      <c r="AF22" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG22" s="33" t="s">
+        <v>507</v>
+      </c>
+      <c r="AH22" s="32" t="s">
+        <v>508</v>
+      </c>
+      <c r="AI22" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ22" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK22" s="32" t="s">
+        <v>509</v>
+      </c>
+      <c r="AL22" s="32" t="s">
+        <v>510</v>
+      </c>
+      <c r="AM22" s="32" t="s">
+        <v>511</v>
+      </c>
+      <c r="AN22" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="AO22" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP22" s="32" t="s">
+        <v>506</v>
+      </c>
+      <c r="AQ22" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR22" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS22" s="32" t="s">
+        <v>512</v>
+      </c>
+      <c r="AW22" s="32" t="s">
+        <v>513</v>
+      </c>
+      <c r="AX22" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="AY22" s="32" t="s">
+        <v>515</v>
+      </c>
+      <c r="BB22" s="32" t="s">
+        <v>516</v>
+      </c>
+      <c r="BC22" s="33" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="25">
+        <v>45566.17615865741</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>518</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>493</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>519</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>520</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>521</v>
+      </c>
+      <c r="G23" s="27" t="s">
+        <v>522</v>
+      </c>
+      <c r="H23" s="26" t="s">
+        <v>523</v>
+      </c>
+      <c r="I23" s="26" t="s">
+        <v>499</v>
+      </c>
+      <c r="J23" s="26" t="s">
+        <v>524</v>
+      </c>
+      <c r="K23" s="26" t="s">
+        <v>525</v>
+      </c>
+      <c r="L23" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="M23" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="N23" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="O23" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="P23" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="Q23" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="R23" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="S23" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="T23" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="U23" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="V23" s="26" t="s">
+        <v>526</v>
+      </c>
+      <c r="W23" s="26" t="s">
+        <v>527</v>
+      </c>
+      <c r="X23" s="26" t="s">
+        <v>505</v>
+      </c>
+      <c r="Y23" s="29">
+        <v>1860000.0</v>
+      </c>
+      <c r="Z23" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA23" s="26" t="s">
+        <v>528</v>
+      </c>
+      <c r="AB23" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC23" s="26" t="s">
+        <v>506</v>
+      </c>
+      <c r="AD23" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE23" s="26" t="s">
+        <v>529</v>
+      </c>
+      <c r="AF23" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG23" s="27" t="s">
+        <v>530</v>
+      </c>
+      <c r="AH23" s="26" t="s">
+        <v>531</v>
+      </c>
+      <c r="AI23" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ23" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK23" s="26" t="s">
+        <v>532</v>
+      </c>
+      <c r="AL23" s="26" t="s">
+        <v>510</v>
+      </c>
+      <c r="AM23" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN23" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="AO23" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP23" s="26" t="s">
+        <v>506</v>
+      </c>
+      <c r="AQ23" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR23" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS23" s="26" t="s">
+        <v>512</v>
+      </c>
+      <c r="AW23" s="26" t="s">
+        <v>533</v>
+      </c>
+      <c r="AX23" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="AY23" s="26" t="s">
+        <v>515</v>
+      </c>
+      <c r="BB23" s="26" t="s">
+        <v>534</v>
+      </c>
+      <c r="BC23" s="27" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="31">
+        <v>45566.18747153935</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>536</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>537</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>538</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>539</v>
+      </c>
+      <c r="F24" s="32" t="s">
+        <v>540</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>541</v>
+      </c>
+      <c r="H24" s="32" t="s">
+        <v>537</v>
+      </c>
+      <c r="I24" s="32" t="s">
+        <v>542</v>
+      </c>
+      <c r="J24" s="32" t="s">
+        <v>543</v>
+      </c>
+      <c r="K24" s="32" t="s">
+        <v>544</v>
+      </c>
+      <c r="L24" s="32" t="s">
+        <v>545</v>
+      </c>
+      <c r="M24" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="N24" s="32" t="s">
+        <v>546</v>
+      </c>
+      <c r="O24" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="P24" s="34">
+        <v>0.9</v>
+      </c>
+      <c r="Q24" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="R24" s="32" t="s">
+        <v>547</v>
+      </c>
+      <c r="S24" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="T24" s="32">
+        <v>1.0</v>
+      </c>
+      <c r="U24" s="32">
+        <v>1.0</v>
+      </c>
+      <c r="V24" s="32">
+        <v>41.0</v>
+      </c>
+      <c r="W24" s="32">
+        <v>77954.0</v>
+      </c>
+      <c r="X24" s="38">
+        <v>1483.86</v>
+      </c>
+      <c r="Y24" s="32">
+        <v>0.0</v>
+      </c>
+      <c r="Z24" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC24" s="32" t="s">
+        <v>548</v>
+      </c>
+      <c r="AD24" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF24" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH24" s="32" t="s">
+        <v>549</v>
+      </c>
+      <c r="AI24" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ24" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL24" s="32" t="s">
+        <v>550</v>
+      </c>
+      <c r="AM24" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN24" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="AO24" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP24" s="32" t="s">
+        <v>551</v>
+      </c>
+      <c r="AQ24" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR24" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS24" s="32" t="s">
+        <v>552</v>
+      </c>
+      <c r="AT24" s="32" t="s">
+        <v>371</v>
+      </c>
+      <c r="AU24" s="32" t="s">
+        <v>553</v>
+      </c>
+      <c r="AX24" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="BB24" s="32" t="s">
+        <v>554</v>
+      </c>
+      <c r="BC24" s="33" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="25">
+        <v>45566.3002931713</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>556</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>557</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>558</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>559</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>560</v>
+      </c>
+      <c r="G25" s="27" t="s">
+        <v>561</v>
+      </c>
+      <c r="H25" s="26" t="s">
+        <v>562</v>
+      </c>
+      <c r="I25" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="J25" s="26" t="s">
+        <v>564</v>
+      </c>
+      <c r="K25" s="26" t="s">
+        <v>565</v>
+      </c>
+      <c r="L25" s="26" t="s">
+        <v>566</v>
+      </c>
+      <c r="M25" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="N25" s="26" t="s">
+        <v>567</v>
+      </c>
+      <c r="O25" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="P25" s="26" t="s">
+        <v>568</v>
+      </c>
+      <c r="Q25" s="26" t="s">
+        <v>569</v>
+      </c>
+      <c r="R25" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="S25" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="T25" s="26">
+        <v>6000.0</v>
+      </c>
+      <c r="U25" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="V25" s="26">
+        <v>25.0</v>
+      </c>
+      <c r="W25" s="26">
+        <v>250.0</v>
+      </c>
+      <c r="X25" s="29">
+        <v>3000.0</v>
+      </c>
+      <c r="Y25" s="29">
+        <v>40000.0</v>
+      </c>
+      <c r="Z25" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA25" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB25" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC25" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD25" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE25" s="27" t="s">
+        <v>570</v>
+      </c>
+      <c r="AF25" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG25" s="27" t="s">
+        <v>571</v>
+      </c>
+      <c r="AH25" s="26" t="s">
+        <v>572</v>
+      </c>
+      <c r="AI25" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ25" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK25" s="26" t="s">
+        <v>573</v>
+      </c>
+      <c r="AM25" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN25" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO25" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP25" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="AQ25" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR25" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS25" s="26" t="s">
+        <v>574</v>
+      </c>
+      <c r="AT25" s="26" t="s">
+        <v>575</v>
+      </c>
+      <c r="AV25" s="26" t="s">
+        <v>576</v>
+      </c>
+      <c r="AW25" s="26" t="s">
+        <v>576</v>
+      </c>
+      <c r="AX25" s="26" t="s">
+        <v>576</v>
+      </c>
+      <c r="AY25" s="26" t="s">
+        <v>577</v>
+      </c>
+      <c r="AZ25" s="26" t="s">
+        <v>578</v>
+      </c>
+      <c r="BA25" s="26" t="s">
+        <v>579</v>
+      </c>
+      <c r="BB25" s="26" t="s">
+        <v>580</v>
+      </c>
+      <c r="BC25" s="27" t="s">
+        <v>581</v>
+      </c>
+      <c r="BD25" s="30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="31">
+        <v>45566.3383565625</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>582</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>583</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>584</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>585</v>
+      </c>
+      <c r="F26" s="32" t="s">
+        <v>586</v>
+      </c>
+      <c r="G26" s="33" t="s">
+        <v>587</v>
+      </c>
+      <c r="H26" s="32" t="s">
+        <v>583</v>
+      </c>
+      <c r="I26" s="32" t="s">
+        <v>588</v>
+      </c>
+      <c r="J26" s="32" t="s">
+        <v>589</v>
+      </c>
+      <c r="K26" s="32" t="s">
+        <v>590</v>
+      </c>
+      <c r="L26" s="32" t="s">
+        <v>591</v>
+      </c>
+      <c r="M26" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="N26" s="32" t="s">
+        <v>592</v>
+      </c>
+      <c r="O26" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="P26" s="32" t="s">
+        <v>593</v>
+      </c>
+      <c r="Q26" s="32" t="s">
+        <v>594</v>
+      </c>
+      <c r="R26" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="S26" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="T26" s="32" t="s">
+        <v>595</v>
+      </c>
+      <c r="U26" s="32" t="s">
+        <v>596</v>
+      </c>
+      <c r="V26" s="32" t="s">
+        <v>597</v>
+      </c>
+      <c r="W26" s="32" t="s">
+        <v>597</v>
+      </c>
+      <c r="X26" s="32">
+        <v>0.0</v>
+      </c>
+      <c r="Y26" s="32">
+        <v>0.0</v>
+      </c>
+      <c r="Z26" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA26" s="32" t="s">
+        <v>598</v>
+      </c>
+      <c r="AB26" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC26" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="AD26" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF26" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG26" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="AH26" s="32" t="s">
+        <v>600</v>
+      </c>
+      <c r="AI26" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ26" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK26" s="32" t="s">
+        <v>601</v>
+      </c>
+      <c r="AL26" s="32" t="s">
+        <v>602</v>
+      </c>
+      <c r="AM26" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN26" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="AO26" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ26" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR26" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS26" s="32" t="s">
+        <v>603</v>
+      </c>
+      <c r="AT26" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="AU26" s="32" t="s">
+        <v>604</v>
+      </c>
+      <c r="AV26" s="32" t="s">
+        <v>604</v>
+      </c>
+      <c r="AX26" s="32" t="s">
+        <v>605</v>
+      </c>
+      <c r="AY26" s="32" t="s">
+        <v>606</v>
+      </c>
+      <c r="AZ26" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="BA26" s="32" t="s">
+        <v>607</v>
+      </c>
+      <c r="BC26" s="33" t="s">
+        <v>608</v>
+      </c>
+      <c r="BD26" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="25">
+        <v>45566.46754570602</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>609</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>610</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>611</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>611</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>612</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>613</v>
+      </c>
+      <c r="H27" s="26" t="s">
+        <v>614</v>
+      </c>
+      <c r="I27" s="26" t="s">
+        <v>615</v>
+      </c>
+      <c r="J27" s="26" t="s">
+        <v>616</v>
+      </c>
+      <c r="K27" s="26" t="s">
+        <v>617</v>
+      </c>
+      <c r="L27" s="26" t="s">
+        <v>567</v>
+      </c>
+      <c r="M27" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="N27" s="26" t="s">
+        <v>618</v>
+      </c>
+      <c r="O27" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="P27" s="26">
+        <v>100.0</v>
+      </c>
+      <c r="Q27" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="R27" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="S27" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="T27" s="26">
+        <v>6.0</v>
+      </c>
+      <c r="U27" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="V27" s="26" t="s">
+        <v>619</v>
+      </c>
+      <c r="W27" s="26" t="s">
+        <v>619</v>
+      </c>
+      <c r="X27" s="26" t="s">
+        <v>620</v>
+      </c>
+      <c r="Y27" s="26" t="s">
+        <v>621</v>
+      </c>
+      <c r="Z27" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA27" s="26" t="s">
+        <v>622</v>
+      </c>
+      <c r="AB27" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC27" s="26" t="s">
+        <v>622</v>
+      </c>
+      <c r="AD27" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF27" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG27" s="26" t="s">
+        <v>622</v>
+      </c>
+      <c r="AH27" s="26" t="s">
+        <v>623</v>
+      </c>
+      <c r="AI27" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ27" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK27" s="26" t="s">
+        <v>622</v>
+      </c>
+      <c r="AL27" s="26" t="s">
+        <v>622</v>
+      </c>
+      <c r="AM27" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN27" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="AO27" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ27" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR27" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AW27" s="26" t="s">
+        <v>624</v>
+      </c>
+      <c r="AX27" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="BC27" s="27" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="31">
+        <v>45566.668890057874</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>626</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>627</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>628</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>629</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>630</v>
+      </c>
+      <c r="G28" s="33" t="s">
+        <v>631</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>632</v>
+      </c>
+      <c r="I28" s="32" t="s">
+        <v>633</v>
+      </c>
+      <c r="J28" s="32" t="s">
+        <v>634</v>
+      </c>
+      <c r="K28" s="32" t="s">
+        <v>635</v>
+      </c>
+      <c r="L28" s="32" t="s">
+        <v>636</v>
+      </c>
+      <c r="M28" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="N28" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="O28" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="P28" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="Q28" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="R28" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="S28" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="T28" s="32">
+        <v>8843.0</v>
+      </c>
+      <c r="U28" s="32" t="s">
+        <v>637</v>
+      </c>
+      <c r="V28" s="32">
+        <v>20.0</v>
+      </c>
+      <c r="W28" s="32">
+        <v>600.0</v>
+      </c>
+      <c r="X28" s="35">
+        <v>200000.0</v>
+      </c>
+      <c r="Y28" s="32">
+        <v>0.0</v>
+      </c>
+      <c r="Z28" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA28" s="32" t="s">
+        <v>638</v>
+      </c>
+      <c r="AB28" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC28" s="32" t="s">
+        <v>639</v>
+      </c>
+      <c r="AD28" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE28" s="32" t="s">
+        <v>640</v>
+      </c>
+      <c r="AF28" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG28" s="33" t="s">
+        <v>641</v>
+      </c>
+      <c r="AH28" s="32" t="s">
+        <v>642</v>
+      </c>
+      <c r="AI28" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ28" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK28" s="32" t="s">
+        <v>643</v>
+      </c>
+      <c r="AL28" s="32" t="s">
+        <v>644</v>
+      </c>
+      <c r="AM28" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN28" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="AO28" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ28" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR28" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS28" s="32" t="s">
+        <v>645</v>
+      </c>
+      <c r="AT28" s="32" t="s">
+        <v>646</v>
+      </c>
+      <c r="AU28" s="32" t="s">
+        <v>647</v>
+      </c>
+      <c r="AV28" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="AW28" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="AX28" s="32" t="s">
+        <v>325</v>
+      </c>
+      <c r="AY28" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="AZ28" s="32" t="s">
+        <v>651</v>
+      </c>
+      <c r="BC28" s="33" t="s">
+        <v>652</v>
+      </c>
+      <c r="BD28" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="25">
+        <v>45567.1347021875</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>653</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>654</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>655</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>656</v>
+      </c>
+      <c r="F29" s="26" t="s">
+        <v>657</v>
+      </c>
+      <c r="G29" s="27" t="s">
+        <v>658</v>
+      </c>
+      <c r="H29" s="26" t="s">
+        <v>659</v>
+      </c>
+      <c r="I29" s="26" t="s">
+        <v>660</v>
+      </c>
+      <c r="J29" s="26" t="s">
+        <v>661</v>
+      </c>
+      <c r="K29" s="26" t="s">
+        <v>662</v>
+      </c>
+      <c r="L29" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="M29" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="N29" s="26" t="s">
+        <v>592</v>
+      </c>
+      <c r="O29" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="P29" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="Q29" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="R29" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="S29" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="T29" s="26" t="s">
+        <v>663</v>
+      </c>
+      <c r="U29" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="V29" s="26" t="s">
+        <v>664</v>
+      </c>
+      <c r="W29" s="26" t="s">
+        <v>665</v>
+      </c>
+      <c r="X29" s="26" t="s">
+        <v>666</v>
+      </c>
+      <c r="Y29" s="26" t="s">
+        <v>667</v>
+      </c>
+      <c r="Z29" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA29" s="26" t="s">
+        <v>668</v>
+      </c>
+      <c r="AB29" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC29" s="26" t="s">
+        <v>668</v>
+      </c>
+      <c r="AD29" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE29" s="26" t="s">
+        <v>668</v>
+      </c>
+      <c r="AF29" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG29" s="27" t="s">
+        <v>669</v>
+      </c>
+      <c r="AH29" s="26" t="s">
+        <v>670</v>
+      </c>
+      <c r="AI29" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ29" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK29" s="26" t="s">
+        <v>671</v>
+      </c>
+      <c r="AL29" s="26" t="s">
+        <v>672</v>
+      </c>
+      <c r="AM29" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN29" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="AO29" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ29" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR29" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS29" s="26" t="s">
+        <v>673</v>
+      </c>
+      <c r="AT29" s="26" t="s">
+        <v>674</v>
+      </c>
+      <c r="AX29" s="26" t="s">
+        <v>675</v>
+      </c>
+      <c r="AY29" s="26" t="s">
+        <v>650</v>
+      </c>
+      <c r="AZ29" s="26" t="s">
+        <v>676</v>
+      </c>
+      <c r="BC29" s="27" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="31">
+        <v>45567.153902094906</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>678</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>679</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>680</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>680</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>681</v>
+      </c>
+      <c r="G30" s="33" t="s">
+        <v>682</v>
+      </c>
+      <c r="H30" s="32" t="s">
+        <v>679</v>
+      </c>
+      <c r="I30" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="J30" s="32" t="s">
+        <v>683</v>
+      </c>
+      <c r="K30" s="32" t="s">
+        <v>684</v>
+      </c>
+      <c r="L30" s="32" t="s">
+        <v>685</v>
+      </c>
+      <c r="M30" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="N30" s="32" t="s">
+        <v>686</v>
+      </c>
+      <c r="O30" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="P30" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="Q30" s="34">
+        <v>0.75</v>
+      </c>
+      <c r="R30" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="S30" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="T30" s="32" t="s">
+        <v>687</v>
+      </c>
+      <c r="U30" s="32" t="s">
+        <v>688</v>
+      </c>
+      <c r="V30" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="W30" s="37">
+        <v>21000.0</v>
+      </c>
+      <c r="X30" s="35">
+        <v>18000.0</v>
+      </c>
+      <c r="Y30" s="35">
+        <v>350000.0</v>
+      </c>
+      <c r="Z30" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB30" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC30" s="32" t="s">
+        <v>690</v>
+      </c>
+      <c r="AD30" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF30" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG30" s="33" t="s">
+        <v>691</v>
+      </c>
+      <c r="AH30" s="32" t="s">
+        <v>692</v>
+      </c>
+      <c r="AI30" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ30" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK30" s="32" t="s">
+        <v>693</v>
+      </c>
+      <c r="AL30" s="32" t="s">
+        <v>694</v>
+      </c>
+      <c r="AM30" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN30" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="AO30" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP30" s="32" t="s">
+        <v>695</v>
+      </c>
+      <c r="AQ30" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR30" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AY30" s="32" t="s">
+        <v>696</v>
+      </c>
+      <c r="AZ30" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="BB30" s="32" t="s">
+        <v>697</v>
+      </c>
+      <c r="BC30" s="33" t="s">
+        <v>698</v>
+      </c>
+      <c r="BD30" s="36" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="25">
+        <v>45567.29273365741</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>699</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>700</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>701</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>702</v>
+      </c>
+      <c r="F31" s="26" t="s">
+        <v>703</v>
+      </c>
+      <c r="G31" s="27" t="s">
+        <v>704</v>
+      </c>
+      <c r="H31" s="26" t="s">
+        <v>705</v>
+      </c>
+      <c r="I31" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="J31" s="26" t="s">
+        <v>706</v>
+      </c>
+      <c r="K31" s="26" t="s">
+        <v>707</v>
+      </c>
+      <c r="L31" s="26" t="s">
+        <v>685</v>
+      </c>
+      <c r="M31" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="N31" s="26" t="s">
+        <v>708</v>
+      </c>
+      <c r="O31" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="P31" s="28">
+        <v>0.4</v>
+      </c>
+      <c r="Q31" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="R31" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="S31" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="T31" s="26" t="s">
+        <v>709</v>
+      </c>
+      <c r="U31" s="26" t="s">
+        <v>710</v>
+      </c>
+      <c r="V31" s="26" t="s">
+        <v>711</v>
+      </c>
+      <c r="W31" s="26" t="s">
+        <v>712</v>
+      </c>
+      <c r="X31" s="26" t="s">
+        <v>713</v>
+      </c>
+      <c r="Y31" s="26" t="s">
+        <v>714</v>
+      </c>
+      <c r="Z31" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA31" s="27" t="s">
+        <v>715</v>
+      </c>
+      <c r="AB31" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC31" s="26" t="s">
+        <v>716</v>
+      </c>
+      <c r="AD31" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE31" s="26" t="s">
+        <v>717</v>
+      </c>
+      <c r="AF31" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH31" s="26" t="s">
+        <v>718</v>
+      </c>
+      <c r="AI31" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ31" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK31" s="26" t="s">
+        <v>719</v>
+      </c>
+      <c r="AL31" s="26" t="s">
+        <v>720</v>
+      </c>
+      <c r="AM31" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN31" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="AO31" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP31" s="27" t="s">
+        <v>721</v>
+      </c>
+      <c r="AQ31" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR31" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS31" s="26" t="s">
+        <v>722</v>
+      </c>
+      <c r="AU31" s="26" t="s">
+        <v>723</v>
+      </c>
+      <c r="AW31" s="26" t="s">
+        <v>724</v>
+      </c>
+      <c r="AX31" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="AY31" s="26" t="s">
+        <v>725</v>
+      </c>
+      <c r="BC31" s="27" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="31">
+        <v>45567.32146018519</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>727</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>728</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>729</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>730</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>731</v>
+      </c>
+      <c r="G32" s="33" t="s">
+        <v>732</v>
+      </c>
+      <c r="H32" s="32" t="s">
+        <v>733</v>
+      </c>
+      <c r="I32" s="32" t="s">
+        <v>734</v>
+      </c>
+      <c r="J32" s="32" t="s">
+        <v>735</v>
+      </c>
+      <c r="K32" s="32" t="s">
+        <v>736</v>
+      </c>
+      <c r="L32" s="32" t="s">
+        <v>737</v>
+      </c>
+      <c r="M32" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="N32" s="32" t="s">
+        <v>737</v>
+      </c>
+      <c r="O32" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="P32" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="Q32" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="R32" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="S32" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="T32" s="32" t="s">
+        <v>738</v>
+      </c>
+      <c r="U32" s="32">
+        <v>1.0</v>
+      </c>
+      <c r="V32" s="32" t="s">
+        <v>739</v>
+      </c>
+      <c r="W32" s="32" t="s">
+        <v>740</v>
+      </c>
+      <c r="X32" s="32" t="s">
+        <v>741</v>
+      </c>
+      <c r="Y32" s="32" t="s">
+        <v>742</v>
+      </c>
+      <c r="Z32" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB32" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD32" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF32" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH32" s="32" t="s">
+        <v>743</v>
+      </c>
+      <c r="AI32" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ32" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL32" s="32" t="s">
+        <v>744</v>
+      </c>
+      <c r="AM32" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN32" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO32" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ32" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR32" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS32" s="32" t="s">
+        <v>745</v>
+      </c>
+      <c r="AT32" s="32" t="s">
+        <v>746</v>
+      </c>
+      <c r="AU32" s="32" t="s">
+        <v>747</v>
+      </c>
+      <c r="AX32" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="AY32" s="32" t="s">
+        <v>748</v>
+      </c>
+      <c r="AZ32" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="BA32" s="32" t="s">
+        <v>749</v>
+      </c>
+      <c r="BC32" s="32" t="s">
+        <v>750</v>
+      </c>
+      <c r="BD32" s="36" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="25">
+        <v>45567.34257298611</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>518</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>751</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>494</v>
+      </c>
+      <c r="E33" s="26" t="s">
+        <v>752</v>
+      </c>
+      <c r="F33" s="26" t="s">
+        <v>753</v>
+      </c>
+      <c r="G33" s="27" t="s">
+        <v>754</v>
+      </c>
+      <c r="H33" s="26" t="s">
+        <v>523</v>
+      </c>
+      <c r="I33" s="26" t="s">
+        <v>755</v>
+      </c>
+      <c r="J33" s="26" t="s">
+        <v>756</v>
+      </c>
+      <c r="K33" s="26" t="s">
+        <v>757</v>
+      </c>
+      <c r="L33" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="M33" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="N33" s="26" t="s">
+        <v>758</v>
+      </c>
+      <c r="O33" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="P33" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="Q33" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="R33" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="S33" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="T33" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="U33" s="26" t="s">
+        <v>759</v>
+      </c>
+      <c r="V33" s="26" t="s">
+        <v>760</v>
+      </c>
+      <c r="W33" s="26" t="s">
+        <v>761</v>
+      </c>
+      <c r="X33" s="26" t="s">
+        <v>505</v>
+      </c>
+      <c r="Y33" s="29">
+        <v>1470000.0</v>
+      </c>
+      <c r="Z33" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA33" s="26" t="s">
+        <v>506</v>
+      </c>
+      <c r="AB33" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC33" s="26" t="s">
+        <v>506</v>
+      </c>
+      <c r="AD33" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE33" s="26" t="s">
+        <v>762</v>
+      </c>
+      <c r="AF33" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG33" s="27" t="s">
+        <v>763</v>
+      </c>
+      <c r="AH33" s="26" t="s">
+        <v>764</v>
+      </c>
+      <c r="AI33" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ33" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK33" s="26" t="s">
+        <v>765</v>
+      </c>
+      <c r="AL33" s="26" t="s">
+        <v>510</v>
+      </c>
+      <c r="AM33" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN33" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="AO33" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP33" s="26" t="s">
+        <v>506</v>
+      </c>
+      <c r="AQ33" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR33" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS33" s="26" t="s">
+        <v>512</v>
+      </c>
+      <c r="AW33" s="26" t="s">
+        <v>766</v>
+      </c>
+      <c r="AX33" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="AY33" s="26" t="s">
+        <v>515</v>
+      </c>
+      <c r="BA33" s="26" t="s">
+        <v>767</v>
+      </c>
+      <c r="BC33" s="27" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="31">
+        <v>45567.40895445602</v>
+      </c>
+      <c r="B34" s="32" t="s">
+        <v>769</v>
+      </c>
+      <c r="C34" s="32" t="s">
+        <v>770</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>771</v>
+      </c>
+      <c r="E34" s="32" t="s">
+        <v>772</v>
+      </c>
+      <c r="F34" s="32" t="s">
+        <v>773</v>
+      </c>
+      <c r="G34" s="33" t="s">
+        <v>774</v>
+      </c>
+      <c r="H34" s="32" t="s">
+        <v>775</v>
+      </c>
+      <c r="I34" s="32" t="s">
+        <v>776</v>
+      </c>
+      <c r="J34" s="32" t="s">
+        <v>777</v>
+      </c>
+      <c r="K34" s="32" t="s">
+        <v>778</v>
+      </c>
+      <c r="L34" s="32" t="s">
+        <v>779</v>
+      </c>
+      <c r="M34" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="N34" s="32" t="s">
+        <v>737</v>
+      </c>
+      <c r="O34" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="P34" s="34">
+        <v>0.6</v>
+      </c>
+      <c r="Q34" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="R34" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="S34" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="T34" s="32" t="s">
+        <v>780</v>
+      </c>
+      <c r="U34" s="32">
+        <v>1.0</v>
+      </c>
+      <c r="V34" s="32">
+        <v>250.0</v>
+      </c>
+      <c r="W34" s="32">
+        <v>14000.0</v>
+      </c>
+      <c r="X34" s="35">
+        <v>60000.0</v>
+      </c>
+      <c r="Y34" s="35">
+        <v>400000.0</v>
+      </c>
+      <c r="Z34" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA34" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="AD34" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE34" s="32" t="s">
+        <v>782</v>
+      </c>
+      <c r="AF34" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG34" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="AI34" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ34" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK34" s="32" t="s">
+        <v>784</v>
+      </c>
+      <c r="AL34" s="32" t="s">
+        <v>785</v>
+      </c>
+      <c r="AM34" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN34" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="AR34" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS34" s="32" t="s">
+        <v>786</v>
+      </c>
+      <c r="AT34" s="32" t="s">
+        <v>787</v>
+      </c>
+      <c r="AU34" s="32" t="s">
+        <v>443</v>
+      </c>
+      <c r="AW34" s="32" t="s">
+        <v>788</v>
+      </c>
+      <c r="AX34" s="32" t="s">
+        <v>789</v>
+      </c>
+      <c r="AZ34" s="32" t="s">
+        <v>327</v>
+      </c>
+      <c r="BC34" s="32" t="s">
+        <v>790</v>
+      </c>
+      <c r="BD34" s="36" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="39">
+        <v>45567.54524048611</v>
+      </c>
+      <c r="B35" s="40" t="s">
+        <v>791</v>
+      </c>
+      <c r="C35" s="40" t="s">
+        <v>792</v>
+      </c>
+      <c r="D35" s="40" t="s">
+        <v>793</v>
+      </c>
+      <c r="E35" s="40" t="s">
+        <v>794</v>
+      </c>
+      <c r="F35" s="40" t="s">
+        <v>795</v>
+      </c>
+      <c r="G35" s="41" t="s">
+        <v>796</v>
+      </c>
+      <c r="H35" s="40" t="s">
+        <v>792</v>
+      </c>
+      <c r="I35" s="40" t="s">
+        <v>797</v>
+      </c>
+      <c r="J35" s="40" t="s">
+        <v>798</v>
+      </c>
+      <c r="K35" s="40" t="s">
+        <v>799</v>
+      </c>
+      <c r="L35" s="40" t="s">
+        <v>800</v>
+      </c>
+      <c r="M35" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="N35" s="40" t="s">
+        <v>801</v>
+      </c>
+      <c r="O35" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="P35" s="42">
+        <v>0.25</v>
+      </c>
+      <c r="Q35" s="40" t="s">
+        <v>802</v>
+      </c>
+      <c r="R35" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="S35" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="T35" s="40" t="s">
+        <v>803</v>
+      </c>
+      <c r="U35" s="40">
+        <v>4.0</v>
+      </c>
+      <c r="V35" s="40" t="s">
+        <v>804</v>
+      </c>
+      <c r="W35" s="40" t="s">
+        <v>805</v>
+      </c>
+      <c r="X35" s="40" t="s">
+        <v>806</v>
+      </c>
+      <c r="Y35" s="40" t="s">
+        <v>807</v>
+      </c>
+      <c r="Z35" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA35" s="40" t="s">
+        <v>808</v>
+      </c>
+      <c r="AB35" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC35" s="40" t="s">
+        <v>809</v>
+      </c>
+      <c r="AD35" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE35" s="40" t="s">
+        <v>810</v>
+      </c>
+      <c r="AF35" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH35" s="40" t="s">
+        <v>811</v>
+      </c>
+      <c r="AI35" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ35" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK35" s="40" t="s">
+        <v>812</v>
+      </c>
+      <c r="AL35" s="40" t="s">
+        <v>813</v>
+      </c>
+      <c r="AM35" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN35" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="AO35" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP35" s="40" t="s">
+        <v>814</v>
+      </c>
+      <c r="AQ35" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR35" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS35" s="40" t="s">
+        <v>815</v>
+      </c>
+      <c r="AT35" s="40" t="s">
+        <v>816</v>
+      </c>
+      <c r="AU35" s="40" t="s">
+        <v>817</v>
+      </c>
+      <c r="AV35" s="40" t="s">
+        <v>817</v>
+      </c>
+      <c r="AW35" s="40" t="s">
+        <v>817</v>
+      </c>
+      <c r="AX35" s="40" t="s">
+        <v>818</v>
+      </c>
+      <c r="AY35" s="40" t="s">
+        <v>819</v>
+      </c>
+      <c r="AZ35" s="40" t="s">
+        <v>820</v>
+      </c>
+      <c r="BA35" s="40" t="s">
+        <v>817</v>
+      </c>
+      <c r="BB35" s="40" t="s">
+        <v>821</v>
+      </c>
+      <c r="BC35" s="41" t="s">
+        <v>822</v>
+      </c>
+      <c r="BD35" s="43" t="s">
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -4482,10 +8808,59 @@
     <hyperlink r:id="rId39" ref="BC16"/>
     <hyperlink r:id="rId40" ref="G17"/>
     <hyperlink r:id="rId41" ref="AG17"/>
+    <hyperlink r:id="rId42" ref="G18"/>
+    <hyperlink r:id="rId43" ref="AA18"/>
+    <hyperlink r:id="rId44" ref="AG18"/>
+    <hyperlink r:id="rId45" ref="BC18"/>
+    <hyperlink r:id="rId46" ref="G19"/>
+    <hyperlink r:id="rId47" ref="AG19"/>
+    <hyperlink r:id="rId48" ref="BC19"/>
+    <hyperlink r:id="rId49" ref="G20"/>
+    <hyperlink r:id="rId50" ref="BC20"/>
+    <hyperlink r:id="rId51" ref="G21"/>
+    <hyperlink r:id="rId52" ref="BC21"/>
+    <hyperlink r:id="rId53" ref="G22"/>
+    <hyperlink r:id="rId54" ref="AG22"/>
+    <hyperlink r:id="rId55" ref="BC22"/>
+    <hyperlink r:id="rId56" ref="G23"/>
+    <hyperlink r:id="rId57" ref="AG23"/>
+    <hyperlink r:id="rId58" ref="BC23"/>
+    <hyperlink r:id="rId59" ref="G24"/>
+    <hyperlink r:id="rId60" ref="BC24"/>
+    <hyperlink r:id="rId61" ref="G25"/>
+    <hyperlink r:id="rId62" ref="AE25"/>
+    <hyperlink r:id="rId63" ref="AG25"/>
+    <hyperlink r:id="rId64" ref="BC25"/>
+    <hyperlink r:id="rId65" ref="G26"/>
+    <hyperlink r:id="rId66" ref="BC26"/>
+    <hyperlink r:id="rId67" ref="G27"/>
+    <hyperlink r:id="rId68" ref="BC27"/>
+    <hyperlink r:id="rId69" ref="G28"/>
+    <hyperlink r:id="rId70" ref="AG28"/>
+    <hyperlink r:id="rId71" ref="BC28"/>
+    <hyperlink r:id="rId72" ref="G29"/>
+    <hyperlink r:id="rId73" ref="AG29"/>
+    <hyperlink r:id="rId74" ref="BC29"/>
+    <hyperlink r:id="rId75" ref="G30"/>
+    <hyperlink r:id="rId76" ref="AG30"/>
+    <hyperlink r:id="rId77" ref="BC30"/>
+    <hyperlink r:id="rId78" ref="G31"/>
+    <hyperlink r:id="rId79" ref="AA31"/>
+    <hyperlink r:id="rId80" ref="AP31"/>
+    <hyperlink r:id="rId81" ref="BC31"/>
+    <hyperlink r:id="rId82" ref="G32"/>
+    <hyperlink r:id="rId83" ref="G33"/>
+    <hyperlink r:id="rId84" ref="AG33"/>
+    <hyperlink r:id="rId85" ref="BC33"/>
+    <hyperlink r:id="rId86" ref="G34"/>
+    <hyperlink r:id="rId87" ref="AA34"/>
+    <hyperlink r:id="rId88" ref="AG34"/>
+    <hyperlink r:id="rId89" ref="G35"/>
+    <hyperlink r:id="rId90" ref="BC35"/>
   </hyperlinks>
-  <drawing r:id="rId42"/>
+  <drawing r:id="rId91"/>
   <tableParts count="1">
-    <tablePart r:id="rId44"/>
+    <tablePart r:id="rId93"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New solutions data and backend for map view
</commit_message>
<xml_diff>
--- a/utils/HealthSolutionsData.xlsx
+++ b/utils/HealthSolutionsData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="823">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="840">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1223,7 +1223,7 @@
     <t>Tanzania</t>
   </si>
   <si>
-    <t>Kenya, Congo (DRC), Uganda and USA</t>
+    <t>Kenya, Democratic Republic of the Congo, Uganda, USA</t>
   </si>
   <si>
     <t>https://tanzmed.co.tz/privacy-policy.html</t>
@@ -1544,7 +1544,7 @@
     <t>Abidjan, Côte d'Ivoire</t>
   </si>
   <si>
-    <t>BENIN, SENEGAL, TOGO, BURKINA FASO</t>
+    <t>Benin, Senega, Togo, Burkina Faso</t>
   </si>
   <si>
     <t>100% (All members of the management team are based in Africa, specifically in Ivory Coast)</t>
@@ -1745,7 +1745,7 @@
     <t>Kigali, Rwanda</t>
   </si>
   <si>
-    <t>Rwanda, Kenya, DRC</t>
+    <t>Rwanda, Kenya, Democratic Republic of the Congo</t>
   </si>
   <si>
     <t>1000+ healthcare providers served</t>
@@ -2537,7 +2537,7 @@
     <t>Kigali - Rwanda</t>
   </si>
   <si>
-    <t>Rwanda and Kenya</t>
+    <t>Rwanda, Kenya</t>
   </si>
   <si>
     <t>The Lifesten Application has had 3 deployments with the lattest version being Version 2.37 and has reached over 10,000 users.</t>
@@ -3012,6 +3012,65 @@
   </si>
   <si>
     <t>www.signalytic.ca</t>
+  </si>
+  <si>
+    <t>Michelle Mumbi</t>
+  </si>
+  <si>
+    <t>mmumbi@tpn.africa</t>
+  </si>
+  <si>
+    <t>The Pathology Network Limited</t>
+  </si>
+  <si>
+    <t>Spes 360</t>
+  </si>
+  <si>
+    <t>The Spes360  is a diagnostic platform designed to enhance workflows across multiple laboratories within a healthcare network. It facilitates inter-laboratory coordination through real-time sample tracking and standardized protocols, ensuring efficient handling and consistent quality. By automating routine tasks and managing resources, the platform improves processing times and overall efficiency.
+A key feature of Spes360 is its collaboration with network pathologists, who provide expert consultation and insights, enhancing diagnostic accuracy and patient care. The platform also includes logistics coordination and sample tracking, ensuring timely and secure transportation of samples while maintaining their integrity. Real-time updates on sample status further enhance reliability.
+Centralizing data from various labs allows seamless access to patient information and interoperability with existing systems. Improved communication is supported through collaboration tools and automated alerts that foster interaction among labs, pathologists, and healthcare providers. Additionally, Spes360 offers data analytics capabilities for performance analysis and quality control, optimizing resource allocation and compliance.
+With its flexible architecture, Spes360 adapts to the needs of both small clusters and larger healthcare networks. In summary, it streamlines laboratory diagnostics, enhances collaboration with pathologists, improves logistics coordination, and ultimately supports better patient outcomes.</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1cDxvN_GEHPi46iGMgmK4Onb9pMwLTCb4</t>
+  </si>
+  <si>
+    <t>info@tpn.africa</t>
+  </si>
+  <si>
+    <t>Laboratory and Diagnostics</t>
+  </si>
+  <si>
+    <t>The Spes360 L-DMS is designed to improve health outcomes in Africa by leveraging digital innovations tailored to the continent's specific healthcare challenges. By connecting multiple laboratories, the platform enhances access to diagnostic services in remote and underserved areas, ensuring timely diagnoses that can significantly impact patient management. Its real-time sample tracking reduces turnaround times, while collaboration with network pathologists provides healthcare providers in these regions with expert insights, enhancing diagnostic accuracy.
+Spes360’s flexible architecture allows it to adapt to diverse health needs, while its analytics capabilities help identify health trends, enabling proactive public health responses. Additionally, the platform supports training programs for healthcare professionals, fostering skill development and community engagement to raise awareness about the importance of timely diagnostics. .</t>
+  </si>
+  <si>
+    <t>1 active deployments. 150 hospitals, with 200-300 users.</t>
+  </si>
+  <si>
+    <t>$100,000 USD</t>
+  </si>
+  <si>
+    <t>$1,000,000 USD</t>
+  </si>
+  <si>
+    <t>Currently, we are logging a comprehensive range of application data, including application logs that capture errors and exceptions, API access logs, and front-end user activity logs. This multi-faceted approach enables us to monitor system performance, troubleshoot issues effectively, and gain insights into user interactions.
+For front-end user activity, we are utilizing Google Analytics alongside our logging practices. Google Analytics provides valuable data on user behavior, including page views, session duration, and user demographics, allowing us to understand how users engage with our application. This insight helps us identify trends, optimize user experience, and tailor content to meet user needs more effectively.
+Additionally, we are leveraging New Relic for Application Performance Monitoring (APM) and alerting. New Relic offers real-time visibility into application performance, helping us identify bottlenecks and optimize resource allocation. Its alerting capabilities ensure that we are promptly notified of any performance issues or anomalies, allowing us to respond quickly and maintain a seamless user experience.</t>
+  </si>
+  <si>
+    <t>For authentication, we are utilizing OAuth2 provided by Keycloak as our Identity Provider (IDP). This integration allows us to manage user identities and permissions securely, facilitating a robust authentication process.
+In addition to OAuth2, we have implemented a custom authorization system based on CASL (Code Access Security Language) and Attribute-Based Access Control (ABAC). This combination enables fine-grained control over user permissions, allowing us to define and enforce access rules based on user attributes and roles. By leveraging CASL, we can specify complex access conditions in a clear and manageable way, ensuring that users have the appropriate level of access to resources based on their attributes.
+Together, this approach to authentication and authorization enhances security and provides a flexible framework for managing user access across our application, ensuring that sensitive data and functionalities are adequately protected while still being user-friendly.</t>
+  </si>
+  <si>
+    <t>Transmit and track diagnostic orders, Send diagnostic results to providers</t>
+  </si>
+  <si>
+    <t>Data visualization, Dashboards, Business Intelligence, Data processing (extract, transform, load - ETL)</t>
+  </si>
+  <si>
+    <t>https://spes360.com</t>
   </si>
 </sst>
 </file>
@@ -3079,7 +3138,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border/>
     <border>
       <left style="thin">
@@ -3212,10 +3271,10 @@
         <color rgb="FF442F65"/>
       </left>
       <right style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -3223,27 +3282,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF442F65"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFF8F9FA"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF442F65"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -3253,7 +3298,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3383,9 +3428,6 @@
     <xf borderId="11" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -3444,7 +3486,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:BD35" displayName="Form_Responses1" name="Form_Responses1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:BD36" displayName="Form_Responses1" name="Form_Responses1" id="1">
   <tableColumns count="56">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Your name" id="2"/>
@@ -8599,170 +8641,292 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="39">
+      <c r="A35" s="25">
         <v>45567.54524048611</v>
       </c>
-      <c r="B35" s="40" t="s">
+      <c r="B35" s="26" t="s">
         <v>791</v>
       </c>
-      <c r="C35" s="40" t="s">
+      <c r="C35" s="26" t="s">
         <v>792</v>
       </c>
-      <c r="D35" s="40" t="s">
+      <c r="D35" s="26" t="s">
         <v>793</v>
       </c>
-      <c r="E35" s="40" t="s">
+      <c r="E35" s="26" t="s">
         <v>794</v>
       </c>
-      <c r="F35" s="40" t="s">
+      <c r="F35" s="26" t="s">
         <v>795</v>
       </c>
-      <c r="G35" s="41" t="s">
+      <c r="G35" s="27" t="s">
         <v>796</v>
       </c>
-      <c r="H35" s="40" t="s">
+      <c r="H35" s="26" t="s">
         <v>792</v>
       </c>
-      <c r="I35" s="40" t="s">
+      <c r="I35" s="26" t="s">
         <v>797</v>
       </c>
-      <c r="J35" s="40" t="s">
+      <c r="J35" s="26" t="s">
         <v>798</v>
       </c>
-      <c r="K35" s="40" t="s">
+      <c r="K35" s="26" t="s">
         <v>799</v>
       </c>
-      <c r="L35" s="40" t="s">
+      <c r="L35" s="26" t="s">
         <v>800</v>
       </c>
-      <c r="M35" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="N35" s="40" t="s">
+      <c r="M35" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="N35" s="26" t="s">
         <v>801</v>
       </c>
-      <c r="O35" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="P35" s="42">
+      <c r="O35" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="P35" s="28">
         <v>0.25</v>
       </c>
-      <c r="Q35" s="40" t="s">
+      <c r="Q35" s="26" t="s">
         <v>802</v>
       </c>
-      <c r="R35" s="40" t="s">
+      <c r="R35" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="S35" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="T35" s="40" t="s">
+      <c r="S35" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="T35" s="26" t="s">
         <v>803</v>
       </c>
-      <c r="U35" s="40">
+      <c r="U35" s="26">
         <v>4.0</v>
       </c>
-      <c r="V35" s="40" t="s">
+      <c r="V35" s="26" t="s">
         <v>804</v>
       </c>
-      <c r="W35" s="40" t="s">
+      <c r="W35" s="26" t="s">
         <v>805</v>
       </c>
-      <c r="X35" s="40" t="s">
+      <c r="X35" s="26" t="s">
         <v>806</v>
       </c>
-      <c r="Y35" s="40" t="s">
+      <c r="Y35" s="26" t="s">
         <v>807</v>
       </c>
-      <c r="Z35" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA35" s="40" t="s">
+      <c r="Z35" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA35" s="26" t="s">
         <v>808</v>
       </c>
-      <c r="AB35" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC35" s="40" t="s">
+      <c r="AB35" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC35" s="26" t="s">
         <v>809</v>
       </c>
-      <c r="AD35" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE35" s="40" t="s">
+      <c r="AD35" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE35" s="26" t="s">
         <v>810</v>
       </c>
-      <c r="AF35" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH35" s="40" t="s">
+      <c r="AF35" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH35" s="26" t="s">
         <v>811</v>
       </c>
-      <c r="AI35" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ35" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK35" s="40" t="s">
+      <c r="AI35" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ35" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK35" s="26" t="s">
         <v>812</v>
       </c>
-      <c r="AL35" s="40" t="s">
+      <c r="AL35" s="26" t="s">
         <v>813</v>
       </c>
-      <c r="AM35" s="40" t="s">
+      <c r="AM35" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="AN35" s="40" t="s">
+      <c r="AN35" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="AO35" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="AP35" s="40" t="s">
+      <c r="AO35" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP35" s="26" t="s">
         <v>814</v>
       </c>
-      <c r="AQ35" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="AR35" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS35" s="40" t="s">
+      <c r="AQ35" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR35" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS35" s="26" t="s">
         <v>815</v>
       </c>
-      <c r="AT35" s="40" t="s">
+      <c r="AT35" s="26" t="s">
         <v>816</v>
       </c>
-      <c r="AU35" s="40" t="s">
+      <c r="AU35" s="26" t="s">
         <v>817</v>
       </c>
-      <c r="AV35" s="40" t="s">
+      <c r="AV35" s="26" t="s">
         <v>817</v>
       </c>
-      <c r="AW35" s="40" t="s">
+      <c r="AW35" s="26" t="s">
         <v>817</v>
       </c>
-      <c r="AX35" s="40" t="s">
+      <c r="AX35" s="26" t="s">
         <v>818</v>
       </c>
-      <c r="AY35" s="40" t="s">
+      <c r="AY35" s="26" t="s">
         <v>819</v>
       </c>
-      <c r="AZ35" s="40" t="s">
+      <c r="AZ35" s="26" t="s">
         <v>820</v>
       </c>
-      <c r="BA35" s="40" t="s">
+      <c r="BA35" s="26" t="s">
         <v>817</v>
       </c>
-      <c r="BB35" s="40" t="s">
+      <c r="BB35" s="26" t="s">
         <v>821</v>
       </c>
-      <c r="BC35" s="41" t="s">
+      <c r="BC35" s="27" t="s">
         <v>822</v>
       </c>
-      <c r="BD35" s="43" t="s">
+      <c r="BD35" s="30" t="s">
         <v>327</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="39">
+        <v>45568.29184928241</v>
+      </c>
+      <c r="B36" s="40" t="s">
+        <v>823</v>
+      </c>
+      <c r="C36" s="40" t="s">
+        <v>824</v>
+      </c>
+      <c r="D36" s="40" t="s">
+        <v>825</v>
+      </c>
+      <c r="E36" s="40" t="s">
+        <v>826</v>
+      </c>
+      <c r="F36" s="40" t="s">
+        <v>827</v>
+      </c>
+      <c r="G36" s="41" t="s">
+        <v>828</v>
+      </c>
+      <c r="H36" s="40" t="s">
+        <v>829</v>
+      </c>
+      <c r="I36" s="40" t="s">
+        <v>830</v>
+      </c>
+      <c r="J36" s="40" t="s">
+        <v>831</v>
+      </c>
+      <c r="L36" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="M36" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="O36" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="P36" s="42">
+        <v>1.0</v>
+      </c>
+      <c r="Q36" s="42">
+        <v>1.0</v>
+      </c>
+      <c r="R36" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="S36" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="T36" s="40" t="s">
+        <v>832</v>
+      </c>
+      <c r="U36" s="40">
+        <v>1.0</v>
+      </c>
+      <c r="V36" s="40">
+        <v>100.0</v>
+      </c>
+      <c r="W36" s="40">
+        <v>500.0</v>
+      </c>
+      <c r="X36" s="40" t="s">
+        <v>833</v>
+      </c>
+      <c r="Y36" s="40" t="s">
+        <v>834</v>
+      </c>
+      <c r="Z36" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB36" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD36" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF36" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI36" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ36" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK36" s="40" t="s">
+        <v>835</v>
+      </c>
+      <c r="AL36" s="40" t="s">
+        <v>836</v>
+      </c>
+      <c r="AM36" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN36" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="AO36" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ36" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR36" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="AU36" s="40" t="s">
+        <v>837</v>
+      </c>
+      <c r="AV36" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="AX36" s="40" t="s">
+        <v>838</v>
+      </c>
+      <c r="BC36" s="41" t="s">
+        <v>839</v>
       </c>
     </row>
   </sheetData>
@@ -8857,10 +9021,12 @@
     <hyperlink r:id="rId88" ref="AG34"/>
     <hyperlink r:id="rId89" ref="G35"/>
     <hyperlink r:id="rId90" ref="BC35"/>
+    <hyperlink r:id="rId91" ref="G36"/>
+    <hyperlink r:id="rId92" ref="BC36"/>
   </hyperlinks>
-  <drawing r:id="rId91"/>
+  <drawing r:id="rId93"/>
   <tableParts count="1">
-    <tablePart r:id="rId93"/>
+    <tablePart r:id="rId95"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>